<commit_message>
1) Changed the Rest URL 2) Added few folders to git ignore
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19575" windowHeight="8130" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="22650" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,24 +12,19 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:S25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>API</t>
   </si>
   <si>
-    <t>text=test</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
-    <t>md5=098f6bcd4621d373cade4e832627b4f6</t>
-  </si>
-  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -72,18 +67,9 @@
     <t>T1</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>T2</t>
   </si>
   <si>
-    <t>text=mohan</t>
-  </si>
-  <si>
-    <t>md5=e9206237def4b4ef46fd933ed0f5a08f</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -93,38 +79,37 @@
     <t>XYZ</t>
   </si>
   <si>
-    <t>text=Jorge</t>
-  </si>
-  <si>
-    <t>text=Kumar</t>
-  </si>
-  <si>
-    <t>text=Hello</t>
-  </si>
-  <si>
-    <t>text=Hi</t>
-  </si>
-  <si>
-    <t>md5=8b1a9953c4611296a827abf8c47804d7</t>
-  </si>
-  <si>
-    <t>md5=c1a5298f939e87e8f962a5edfc206918</t>
-  </si>
-  <si>
-    <t>md5=f4a1c8901a3d406f17af67144a3ec71a</t>
-  </si>
-  <si>
-    <t>md5=6bfef5d5db4a5344fb9c4eecda34dd0d</t>
-  </si>
-  <si>
-    <t/>
+    <t>codes=co</t>
+  </si>
+  <si>
+    <t>codes=rus</t>
+  </si>
+  <si>
+    <t>name=Colombia</t>
+  </si>
+  <si>
+    <t>name=Russia</t>
+  </si>
+  <si>
+    <t>codes=no</t>
+  </si>
+  <si>
+    <t>name=Norway</t>
+  </si>
+  <si>
+    <t>name=India</t>
+  </si>
+  <si>
+    <t>codes=in</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -498,128 +483,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="11" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-      <c r="O2" s="1" t="s">
-        <v>18</v>
+      <c r="O2" t="s">
+        <v>28</v>
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-    </row>
+    <row r="3" spans="1:16"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -630,126 +587,117 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="11" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3"/>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
+        <v>21</v>
+      </c>
       <c r="J3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
+        <v>23</v>
+      </c>
       <c r="O3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -762,78 +710,78 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
-    <col min="11" max="14" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="14" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>27</v>
@@ -843,46 +791,18 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-    </row>
+    <row r="3" spans="1:16"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added the files / folders under logs and test-reponses to git ignore. Changed the src/test/test-result to src/test/test-responses
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>GET</t>
   </si>
@@ -82,22 +82,19 @@
     <t>/users/user/a99ba4dc-45be-4ad2-9c9e-22e78584b82b</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>S1_TC_T1</t>
   </si>
   <si>
     <t>S1_TC_T2</t>
   </si>
   <si>
-    <t>/users/user/{S1_TC_T1_truid}</t>
-  </si>
-  <si>
     <t>DEPENDENCYTESTS</t>
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>/users/user/(S1_TC_T1_truid)</t>
   </si>
 </sst>
 </file>
@@ -488,7 +485,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -533,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
@@ -547,7 +544,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -572,12 +569,12 @@
         <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -586,7 +583,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -599,14 +596,14 @@
         <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
       </c>
       <c r="K3"/>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Test cases for Bulk profile API in 1PPROFILE
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>GET</t>
   </si>
@@ -164,6 +164,48 @@
   </si>
   <si>
     <t>status=200||summary=I am test user for API Automation</t>
+  </si>
+  <si>
+    <t>S1_TC_T10</t>
+  </si>
+  <si>
+    <t>Get Bulkprofiles data by passing max truids</t>
+  </si>
+  <si>
+    <t>/users</t>
+  </si>
+  <si>
+    <t>?id=</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||truid=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>S1_TC_T11</t>
+  </si>
+  <si>
+    <t>status=413||errorCode=413||errorMessage=Too many TRUIDs provided</t>
+  </si>
+  <si>
+    <t>Get Bulkprofiles data by passing more than max truids and validating error status</t>
+  </si>
+  <si>
+    <t>S1_TC_T12</t>
+  </si>
+  <si>
+    <t>Get Bulkprofiles data by doesn't passing truids and validating error status</t>
+  </si>
+  <si>
+    <t>status=400||errorCode=400||errorMessage=TRUID is missing</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER2)</t>
   </si>
 </sst>
 </file>
@@ -537,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -551,7 +593,7 @@
     <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="52.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="96.42578125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="80.5703125" style="5" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="90.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -820,6 +862,81 @@
         <v>49</v>
       </c>
     </row>
+    <row r="11" spans="1:12" ht="105">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11"/>
+      <c r="J11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="105">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12"/>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13"/>
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed bulk profile API Max length to 100
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
   <si>
     <t>GET</t>
   </si>
@@ -166,9 +166,6 @@
     <t>S1_TC_T10</t>
   </si>
   <si>
-    <t>Get Bulkprofiles data by passing max truids</t>
-  </si>
-  <si>
     <t>/users</t>
   </si>
   <si>
@@ -199,16 +196,16 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>?id=(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>?id=(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>status=200||imageContent=""</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>Get Bulkprofiles data by passing max truids(Max Truid =100)</t>
   </si>
 </sst>
 </file>
@@ -585,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -668,7 +665,7 @@
       </c>
       <c r="K2" s="1"/>
       <c r="L2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -700,7 +697,7 @@
       </c>
       <c r="K3"/>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -728,7 +725,7 @@
       </c>
       <c r="K4"/>
       <c r="L4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -760,7 +757,7 @@
       </c>
       <c r="K5"/>
       <c r="L5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -784,11 +781,11 @@
       <c r="H6"/>
       <c r="I6"/>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -820,7 +817,7 @@
       </c>
       <c r="K7"/>
       <c r="L7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
@@ -852,7 +849,7 @@
       </c>
       <c r="K8"/>
       <c r="L8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -884,7 +881,7 @@
       </c>
       <c r="K9"/>
       <c r="L9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -916,21 +913,21 @@
       </c>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="105">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="180">
       <c r="A11" t="s">
         <v>49</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
         <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
@@ -942,25 +939,25 @@
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="105">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="180">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
@@ -972,41 +969,41 @@
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K12"/>
       <c r="L12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
       </c>
       <c r="F13"/>
       <c r="G13" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
       <c r="J13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K13"/>
       <c r="L13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test cases for Media type
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="110">
   <si>
     <t>GET</t>
   </si>
@@ -85,30 +85,18 @@
     <t>S1_TC_T5</t>
   </si>
   <si>
-    <t>Update user image</t>
-  </si>
-  <si>
     <t>Get user image</t>
   </si>
   <si>
-    <t>{"imageContent":""}</t>
-  </si>
-  <si>
     <t>/users/user/(SYS_USER1)</t>
   </si>
   <si>
     <t>/users/user/(SYS_USER1)/image</t>
   </si>
   <si>
-    <t>Update user image without image type</t>
-  </si>
-  <si>
     <t>S1_TC_T6</t>
   </si>
   <si>
-    <t>{"imageContent":"test","imageType":""}</t>
-  </si>
-  <si>
     <t>S1_TC_T7</t>
   </si>
   <si>
@@ -121,9 +109,6 @@
     <t>S1_TC_T8</t>
   </si>
   <si>
-    <t>Use Update user image API to update the first name</t>
-  </si>
-  <si>
     <t>Get user profile and verify user details.</t>
   </si>
   <si>
@@ -193,12 +178,6 @@
     <t>status=400||errorCode=400||errorMessage=TRUID is missing</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>status=200||imageContent=""</t>
-  </si>
-  <si>
     <t>?id=(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2)</t>
   </si>
   <si>
@@ -206,13 +185,171 @@
   </si>
   <si>
     <t>Get Bulkprofiles data by passing max truids(Max Truid =100)</t>
+  </si>
+  <si>
+    <t>Retrieve user profile with wrong user id and check the error status</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER1)1</t>
+  </si>
+  <si>
+    <t>status=404||errorCode=404||errorMessage=User not found.</t>
+  </si>
+  <si>
+    <t>Create user profile with existing truid and check the error status</t>
+  </si>
+  <si>
+    <t>/users/user</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>status=409||errorCode=409||errorMessage=User already exists.</t>
+  </si>
+  <si>
+    <t>Upload existing media to S3</t>
+  </si>
+  <si>
+    <t>/users/user/media</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER2)","mediaCategory":"image-full","mediaType": "raw","base64Content":"data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxQSEhUTExQWFhQXFhkYGBUVFRQUFRcYFxcaFhcaFBUYHCggGBwlHBUVITEhJSkrLy4uFx8zODMsNygtLysBCgoKDg0OGxAQGywkHSU0LC03LywvNSwvLC0sLTcxLzA3LC8sKywsNCwwMS00LCwsNC0sLDcsLC8sLCwsNSwsNP/AABEIAMMBAgMBIgACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAAFAAECAwQGB"}</t>
+  </si>
+  <si>
+    <t>status=409||errorCode=409||errorMessage=Media already exists.</t>
+  </si>
+  <si>
+    <t>Retrieve user profile with missing truid and check the error status</t>
+  </si>
+  <si>
+    <t>/users/user/</t>
+  </si>
+  <si>
+    <t>status=400||errorCode=400||errorMessage=TRUID is missing.</t>
+  </si>
+  <si>
+    <t>Update user profile with only one parameter and check the error status</t>
+  </si>
+  <si>
+    <t>{"title": "Project Neon1"}</t>
+  </si>
+  <si>
+    <t>status=400||errorCode=400||errorMessage=Missing one or more required values.</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER2)/image</t>
+  </si>
+  <si>
+    <t>{"imageType": "jpg","imageHeight": 182,"imageWidth": 183}</t>
+  </si>
+  <si>
+    <t>Use Update user image API to update the first name and check the error code</t>
+  </si>
+  <si>
+    <t>Get User Image with non existing truids and validating error status</t>
+  </si>
+  <si>
+    <t>Update user image with empty data</t>
+  </si>
+  <si>
+    <t>Update user image with data</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER2)/media</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||mediaCategory=image-full||mediaType=image/jpg</t>
+  </si>
+  <si>
+    <t>status=404||errorCode=404||errorMessage=Media not found.</t>
+  </si>
+  <si>
+    <t>Get media info for the User id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get media image directly for the User id </t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER2)/media/image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get raw image directly for the User id </t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER2)/raw/image</t>
+  </si>
+  <si>
+    <t>Get media info for non existing User id and check media status</t>
+  </si>
+  <si>
+    <t>Get raw image with non existing truid and check the error status</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER2)a/raw/image</t>
+  </si>
+  <si>
+    <t>S1_TC_T13</t>
+  </si>
+  <si>
+    <t>S1_TC_T14</t>
+  </si>
+  <si>
+    <t>S1_TC_T15</t>
+  </si>
+  <si>
+    <t>S1_TC_T16</t>
+  </si>
+  <si>
+    <t>S1_TC_T17</t>
+  </si>
+  <si>
+    <t>S1_TC_T19</t>
+  </si>
+  <si>
+    <t>S1_TC_T20</t>
+  </si>
+  <si>
+    <t>S1_TC_T21</t>
+  </si>
+  <si>
+    <t>S1_TC_T22</t>
+  </si>
+  <si>
+    <t>S1_TC_T23</t>
+  </si>
+  <si>
+    <t>S1_TC_T25</t>
+  </si>
+  <si>
+    <t>Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||imageType=jpg||mediaCategory=image-full</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||imageType=jpg||mediaCategory=image-full||title=Project Neon2</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER2)a/image</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER1)a/media</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)","firstName": "Project","lastName": "Neon1","title": "Project Neon 1","role": "QA","primaryInstitution": "Thomson reuters, Bangalore","location": "india"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -271,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -286,6 +423,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,26 +724,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="I14" workbookViewId="0">
+      <selection activeCell="L24" sqref="L2:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="49.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="52.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="96.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="80.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="90.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="52.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="96.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="80.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="90.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -640,371 +784,579 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="45">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4"/>
-      <c r="L4" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5"/>
-      <c r="H5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5"/>
-      <c r="J5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>59</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7"/>
+        <v>0</v>
+      </c>
+      <c r="H7"/>
       <c r="J7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8"/>
+        <v>41</v>
+      </c>
       <c r="H8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8"/>
+        <v>29</v>
+      </c>
       <c r="J8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9"/>
+        <v>41</v>
+      </c>
       <c r="H9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9"/>
-      <c r="J9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>42</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="180">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10"/>
-      <c r="H10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10"/>
+      <c r="J10" t="s">
         <v>47</v>
-      </c>
-      <c r="I10"/>
-      <c r="J10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="180">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
         <v>0</v>
       </c>
-      <c r="F11"/>
       <c r="G11" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H11"/>
-      <c r="I11"/>
       <c r="J11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="180">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
-      <c r="F12"/>
       <c r="G12" s="5" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="H12"/>
-      <c r="I12"/>
       <c r="J12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12"/>
-      <c r="L12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
         <v>0</v>
       </c>
-      <c r="F13"/>
-      <c r="G13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13"/>
-      <c r="L13" t="s">
+      <c r="H16" s="8"/>
+      <c r="J16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18"/>
+      <c r="J18" s="1" t="s">
         <v>59</v>
       </c>
+    </row>
+    <row r="19" spans="1:11" ht="90">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved Profile module testing coverage.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
   <si>
     <t>GET</t>
   </si>
@@ -380,6 +380,18 @@
   </si>
   <si>
     <t>status=200||truid=(SYS_USER2)||imageType=jpeg||mediaCategory=image-full||title=Project Neon2||imageHeight=151||imageWidth=200||imageContent=data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD//gA7Q1JFQVRPUjogZ2QtanBlZyB2MS4wICh1c2luZyBJSkcgSlBFRyB2ODApLCBxdWFsaXR5ID0gNjUK/9sAQwALCAgKCAcLCgkKDQwLDREcEhEPDxEiGRoUHCkkKyooJCcnLTJANy0wPTAnJzhMOT1DRUhJSCs2T1VORlRAR0hF/9sAQwEMDQ0RDxEhEhIhRS4nLkVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVF/8AAEQgAlwDIAwEiAAIRAQMRAf/EAB8AAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKC//EALUQAAIBAwMCBAMFBQQEAAABfQECAwAEEQUSITFBBhNRYQcicRQygZGhCCNCscEVUtHwJDNicoIJChYXGBkaJSYnKCkqNDU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6g4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2drh4uPk5ebn6Onq8fLz9PX29/j5+v/EAB8BAAMBAQEBAQEBAQEAAAAAAAABAgMEBQYHCAkKC//EALURAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/aAAwDAQACEQMRAD8A6+OaEy+UJUMg/h3DP5U6bSrO8minnt0eWJg6P3BHQ1zXlx6Cp1nVwLrV7g+XFHEOhPSNB/M1bv8AUtT0zRpL++uYoblh+5s4owwLn7qZPLH1xigDWv8ARmu9WstQV1Y2isFhkzsJP8XHcVHJYi3uxq2sym4eAEwxwxkpF6kDqT7mrDaxHYaVb3mqqbcui+YApYIxxxx7mtOGRZokkQna6hhkY4NAGNokE+o3Z1q83QiQYgt1bhU9Xx1Y/pVq41iX+24dOsYkuGxuuCSQIV7En1PYVotErxlclR6ocEVRsdHTS7S6jspGM05Z/Nl+Zi56EnvQBcbU7NLlrdp1MyjLIvJUe+OlOMNnfeTchI5dp3RyDnHuDXOadZajpWiC0tLMtqs+TPdSMNm89XJ6n2FOnz4f0Sz0XS5Wm1ObKxkHoc5Z29ACf6UAbUulA6wNThYeeIfJCycqBnOR6Gsa40W7h1WKV5nkjunLXs6cHCj5EGOQtakuqjTPsdhK0l7qMy8JGoBbHVz2UVat9Uhl1KTT5AY7uOMSlM5BUnGQfqKAKOnfaZdcmmhR4NMjh8tVcY8x853AHsBxVnTNY+2reTuESygcqk+cB8feP0ByM1oSwxXULROdyMMHa2P5Vm3/AIfin8P/ANlWreVENu1exAOdp9j0oAtrdWOowqpZJIpgQoYcOPbPWrMkLC1MVuwjO3apIzj0rIutOur3UdPZ1S3srFvMwGyztjAHsBS2l7NfeJLpYJj9gtIwkncPKeeD7D+dADZrC607Q7e0sXO4SKJpV+8VJ+Zh7morvWn06+YRRSTWoRUBP8UrNgAE+3WrcPiGCe0ub1In+xQMVMx6NjqQO4960ZFt7uFVk2Mj4ZeevcEUAQ/2jHHc/Z7rbHJ5Xm5zxtHXmmvY2d9Eyq2YnYOyo3DHrzVbUvD8N7HOwZjPKFUs5z8qnO36Gq2qJqUEst7ZxhFgtiir13sSOcegAoA02tpv7WSfAEMcRUAHqc96rRapNHDC90BvlnMflgcrycVJHftDf21k7+cZYTIWHBBGPTsc1Ytri2vJJSigvbyFG3L0bH/16AFJtbi7aBkBljxIQR+RpGtGE11NFJh5k2j/AGSBxSfYVM9xOkp3zoEJ/u46Y/OqtrBdWsljAiHaikTOTweOD9c0AWLdrmOWKJkZk8o72bsw9/eo2ltbvT287ESSsYzzyTnH9Kli1FQL1rggR2zYLDuMA/1pTb211GqxjYVYSqMYIPXOKAKF5YysZZ7STc7QhE56MM4P+NFSXFrc2lpdvC7NK8nmIqDoOMj9D+dFAGTfaTBqL2skhZJbWTzIpEPKn8eDTP7DiS6GoTibULuP/ViVhhP90cKD706XW7GC6+ymZpLgDJihRpGUe4UHH41esb+21CDzrWVZEyVOOoI6gg8g0AYdpZ3Ovaq15rELwQWb4t7Jxxn/AJ6MejH0x0o0++uvE91cXK3Mlno9s5jTyztecjqxbqF+ldOKy5PDWnSo8RSRLeRy7wRyssbMepKg0AU/DOoXGo6pqT28jyaRGwS3eQlizj7xBPJWtPSdeTVb27to7eRfsjbXlyGQt6Ajqap61BqkOl/Y9Bt4Yo2ATejbWiXvtXgZx05qjrbN4Z8P2Gl6IvlS3ky2yTN/AW6uf9qgDsRKm/bvXd6Z5qL+z7Q3i3YgjW4AI81RhiPQnuK4nX7O10rSodF0pPO1q8dQkpOZQc5MjN1Fb+uazP4f0q1KhLq8kZYUibO6d+Bxjp3NAFp9GeLXptXtnR5pYBCUlzhQDkEEdPpUNrYR6C17q+pzm4vJxmSREOFUDhFHPH862YpWW0SS6CRNsBkG75VOOeafBcwXKFoJo5VBwSjAigDD8JWsj28+r3K7LjUW8wRA8RJ/Cv1xyfc1aXV55fFD6XBGkkEMQknk5BjJ+6vuT1rVMQ8oohMY9UwMVn6Voo0lb0pM00t1IZWlkHzFj6kdh2oAstqdktxJAbhPMjGXUHOz6+n41OkMOGeNEHmDkqPvVx2nLcaJ4XuraS0ln1i5eXcoQt5rsThi3TbjHertw9z4X8DQIZi19BEkSd98hwAvPUZP5CgC3L4bDaSdKhuTFYsTuULlipOSuaZqsD3Or6TaRxOlrBIZnlxgfKMKufcn9K2bdpo7GM3H7ycIN+wYy2OcCo9L1O21e0+02jFot5TLLjkHBoAg13UZNLsklgCvK8qRJG38RYgVanvre2lhhnkAmmzsQAknHXgdqbe6bb38kEkwbfbyCSMg8Bh0OKr3Ng665BqagyBIGhZB1GSDkflQBciit2JmgVNzDG9QM/SsyTR5otL1GC2nJnumeQSdCGaq1ol1p+k6teXm63MkstxHGGGUXHH48Z/GtPSJriXRLSe4/eXDwq79skjNAFOBpodRsYLeKRYvJbz9wOFIxjn1zVu11MOb43G1I7SQqX7EbQc/rU2n38Wp2a3MQYIxZfm68HB/lTJNLt3trqFQVW6B8zB6kjGaAHILO+gkVACs6ZIxgsD3pEsHW8WdptyLD5QQDrz1NVUsbr7fYMSoitY2V2B5fIAHH60Qag0A1V5GaRLVyVHfG0HAoAYl3c2lhHvQs5ufKJk/hUscH+VFXIryO6WOK4jCNNH5gQnII7/lRQBwYubLwrpy2Glp9t1ObkIp3PI5/jc9hVnTLaPwp4buZ9SuiJ5S008q4zvbsuep7CtqC1t7cH7PDFET3RAKxbjQr6/1y0uNRniurG2+ZIVBTD9mYc7vzoAteGbjU206W+1ufZG/zxJIqqY4/ViAOasr4q01oXuFaZrRDhroRN5Q5x97HT36VieJjLqniLTNCkYw6fIpmmOcedt/gz+H60eILn+2FTwvoYUq+FuZo+Ut4x/D9TjpQB2sbq6K6MGVhkEHIIpZoIbqIxXESSxnqrjIrlPE14+k6ZZaZpUsy6jLthtY42GcAY3NkHgCul0+Ke2sIY7u4a6nRPnlKgFz9BxQAtppdnZM72dtFDI/V1Tk/U9TWZBod7J4q/tTU5IbiOKLZarHkCIn7xIPc+uas6b4is9S1G4sIkuEubYAypLEV2+nPTvWwOtAGJ4n8RJo9g6WxWXUZmEVvAOpduhx6DrVrwzoq6Do8duTvuHPm3En9+Q9TV2e1t7tNlxCkq9QGXOPpRdR3DWxWymSGUfdZ03jp6ZFAGTp2s3t74rvtPi8mSws0HmTbCGEh6IDnBwK1Jtb063u2tZbtBOg3OgySg9Wx0/GsvQNIuPD/h6aDCzX3zyNKDnzpDyCc9OwxWJ4Xv7TQvBE2p3zqb6dpHnVz+8eXcQEx1zwOKAO9jkSWNXjdXRhkMpyCKoaloltqk1vLM0ge3kEseGO3cOhK9DWF4YhuNF8BI99K1vIkb3DErkxgktjB9u1afhO/v8AU/D9ve6mFEtxl1Crtwn8OffHP40AXNZa9XSrgadCJbkxkICwXBxwaZ4esF0zQrO0UMPKjCtuGDu7/rmpbfWLK4v3sElIu0Te0ToysFzjPI6VcdFkQo6hlPBBoA57w9dS3Wq63cebIbKKYQwozEgFR85GferFp4nhudPbUWt5IrDzCizMRyM43Y7DNXrbSbWytpre1j8qGXcSingE9SK5670TUl8Kp4eto0cHERuSwCrHuzkjrnHagDqJoYbuExzRrLG45VhkEUCHyrfy4MKFGFB5ArnfEKqt7oFnC2JWulBZThtiKSR9OBV+71iVfEEGk2sKNI8JnkeRiAq5wBgdyaAJdFsG0vR4rO4KuYgdzjo2STnH41lafqDWPhrUr5F8wwzTuiE44DHA+lbNjqsN3HcFyIXtZDFMrNwrD39CCDVgpb3du+BHLFKpBK4IYdOtAFGHUpI5rKC8Cb7tCyNHnG4DJHPt/KrqS2100salHZflkXuM9jVH+xFN5ZTNcOY7IN5UWB1Ixye+BTLNZE8Rag7xukcscWxmHDEbs4/SgCwukqLq0lEzeXahhHHj1GOT7Cimw3Uy+IJ7NpC8X2dZkBAyDuIP8hRQBjWWo2t+jNazLJsOGA4Kn3B5FXVPFeaaZrL2l9d6y8DyXWrMEtLNerKOjH06da3tS1jWdC0tdSvntGG9Q1qiEHBPQNnr+FAHWTW0F0my5gjmX0kUMP1oW0S3tmisEhtSfulYhtH1AxmoG1O1hto57meOBZFDASuF6jpzVm3uYbqISwSpLGejIwIP5UAYuj6JeQ6/eanqzRXFxIuyCSPIWNP7oU9PrVjxF4mg0axkW3dJtQdhFDbqcsXbpkelbSmormwtL5QLq3il2nKllBKn1B6g/SgDE023g8FeGJ72/fzLkgz3MneSQ9F/XApmkQalqWmyaxrOoXFt5qGWKCB9iwJjIJ/vHHPNX/FGgnX9CewjlET7ldC2SCV6A+1UtWsNb1yxj0sRxadaMAtxMsu9nUfwoB0B96AGaB4zjbwxaXmsSE3M0jRRLGmXnwcAhR/+qugs9ctbu8+xMstvd7PMEE6bWZfUdj+BrjvCenxS+LtUkkQCPSMWdpG38CjPzfU4zn3NKdRXVPHM2rxHOnaJbtD5g6SSHOQPz/T3o2Gk27I9CEsbMyK6ll6gHkVG9laSTLNJbQtKOkhQFh+NeZWVyLrVZJ7u9ktN5LGVM5z2HH+eK6DQfEV02qrYPJ9sgZiqzbcHHrWKq3O+rgJQTcXeyuza8UaNe65pj2dteJDFJt8xGT74ByRuB4z9DWojxWGnxmVRBHEiqVHIQDjHTpVW512xs71bS4l2SEA5I45rSBBGe1a3RwuMo2bW5yXgxv7U1PWteb7txP5EGe0aDj8yaXw/fah4lXUNTN9JbWqytFaRRquAF/ibI5zXVRW0ELO8UUaM5y5VQN319a5xfDuoaZpt3p2i3MEdvcOzK0oO6AN94DHX26UyS74f8Qf2p4bh1O4jZWO5XESFuVYgkAc44zWnp+oW2qWaXVlIJYHztbBGcHB61gXxtPB3gmW0jlwYbZ1iLcF3IPP1yc1o+F7L7B4Y0636MsClsepGT+poAvXFha3Msc0sKGaM5SQDDL9D1qndaUx1mHVbYr5yRGB42OA6E5HPYg1n6FfXdx4l1q0e5ea0szGkfmBchiCTyAK1LzWrawvLe2uRKjXLiOJvLJVmPbIoAoaXYSaVDql5qMkQlvJjMwU5VBgADJ69KTwUCfCNiQcFlds+mXY1vkAjB5FRxwRwqywosYY5+QAc0AZukahPdT6nDcsjCzn8sOq7cjaDzz71PZaxZagFNvKWDkhCylQ+Ou3PX8Kr2Ojy2cupb5xMt85kLY2lTt24x07Vzlwzab4VtNOkG3UrS5jSFR958SfeX1BX+tAHYfYIBf8A2xQyzlNhOeq5zjH1oqhe3M9r4h02NZnMF15ivGcEZC5BHcd6KAPOdBa2j8Rarf6tJHDNbt5cMchx5cY6FRVbXtUbV2GpTxMui2TZhRxg3Uvbj0/pXdyWlvOwaaCORh0LKCRWb4k0I63p8MULrHJBKJUDD5WI7GgCr4d0cpA2ta8VlvZV3jzOVgTrgDtxUXgVnu9Q1rUYlMdhcz/uExgHGcnH5VYv9M1jXo0tLt4bGx481YXLvKPTOBgVb1HVLHwtoLLa7MwgRQwIckueg/rQAReJrtvE/wDYpsY3YDe8sUxIjXtnjr7e9dRnFcr4T0s6Npc1/qTD7bdZnuZG/hHXH4VnaKk3ja+m1HUDINIicpbWwJUSEfxNjrQB3oPpTq4fRrj7N8QL7S9OJGnx26tJECSscnHT061uah4ptNL1CCyura7WS4fZCyxgrIeOhB9xQBeutE0++leW4twZHG13RihYehIIyPrVbUPDsMukpp+nbLOFG3BET5T9a1wacDSaurMqE3CSlHdHHW1lqeiW0tvJpkN7A5yWXk5/z7VL4Rs7+0vJppoXhtipJDDHPtXWrmnjpWaprQ7JYyUoyi477nn+nh9c8VeZIMr5hc+yjoP0FdB4u1eaxjt4bWUxys24lTzgU258OT2t+19o0yxSnJaN+hz1rOm0LWdY1NZdQVEQYBYEYA9hUWkk1bVnWp0qtSNSTXLFbHSafqf2fRYLnVZ1V5BnJGM+nH0qS38SaXcuES6VWPQOCv8AOuW8Zo8d7aJyIFiwuOgOef6Vp3aaJpscFvPYl4ZEz56rkfnV8zvbsc7w9NwU9W5X26HUMkc0ZR1V0YYIIyCKYlutvbeTaBYQAQgxkL+FY3h6JY5ZjZ3vn2OBsQnJQ+hq8uvWLaoums7pdsCVjeJl3AdSCRgitE7o4akeSVih4e0a70m71OS7eOZr64Nx5seR1/h2npj6mqXiC5iu/F3h2yjdWeKeSaRM8rhDjI/GurqGe0t7oAXEKSbTldwzg+o9KZBzt9PcX3jq30wzyxWcVmbhkicp5jbsDJHOBVrRtSnOpatpcxa4awZWjc43OjLkAn1HTNWtQ0cz6lb6naOsV7AhjBcZWRD1U/jzmq+j6RLplzqWpX8qy3V4weTygdqKowAO54oAvaXq0Wqi5EUcsb20phkSUDIYD2J9aukA84Fcz4PmSebXJEYENfuw+mBinu7W/jq3hjllEM9pI7xmQlSwYc4J4/CgDTv9L+23tpdrO6S2jFkXgoSQQcjr0PrRVWTX3/ta6s7ayedbNFed1cAjPQKO5wPUUUAUQakBrir3UdSl8Vx6fpd6WjHzTgoCIx6ZrrXuI7aIyTyKiKOWY4FAFxTWff8Ah7TNTkWW5tl85SGWVPlYH1yKLPWdPvZPLtruKR/QNya0AaAKetafNfeHbuxt5D50kJRWc8k+/wBaxdO1O60jw1badaaVdNqUcfliMxEIG/vF+mO9dWDTwaAMLwnoDaFaT3F7IJL+6bzLiT0Pp9BWZoWfFHi261uQE2VjmCzB6E/xN/n1rotW0ttUtniS9uLUujITERgg+oNN8OaU+iaUlixiZYuFaMEbh6ketAGXret3154gi8P6LKIZtvmXNzgN5S+gB7/4ik1C+u/DevaPbLezXdvfuYpI5yGYHjDA49+lUfCJjsfEPiOXUpFiumuCf3pxmPJIIz2qjd6i2q69ceIyhOk6NEwtywwJZPUfif0FAHd3fiHTbC7FrNcZucbvKiRpGA9SFBxV6xvrbULcT2kyTRE43Ke/p9a5P4f6cYtIOq3eXvtQYyySv1254H071iaN4jj0V/E2pqC9tJdhLaIdJJDnp+hNAHqOacDXGz6xr2kaIusakLV4wVaa0SMq0ak44bPJGfSuoivYJLOO6EirBIgdXY4GCMigA1HTrfVLcw3KZHUEdVPqK5270DV4rNrO1uluLU4wr8MK6iKeOZA8Tq6noynIqUdalxTN6WInT0Wq89TH8LabNpmnuLlNk0jkkZzx2rNjb7d8UJu62FiF+jOc/wAjXVOodCpzhhg4OD+dY+neHotL1a5vra4lZrvAnE53k4zjDdR196aVlYzqVHUk5y3ZSu9RvdS8Zf2NZ3TWttawedcSRgF2J6LyDjrVrRdXnk1nUdGvWEs9ntdJQMGSNumQOMj2qm1rJo3jW61WRGNjfW6o0qqW8t1x1A5wQOtR+GYZr7xTrOuNE8dtMFgty6lS6r1bB7cCmQdBaa5YX17JZ28xNzGu94mRlYDOM8gVerk9MPnfEfWZO0NpFF+eD/SpI7y/1bxZqNlDdta2unxoP3aqS7sM5OQeB6UAdKIIhMZRGokIwXA5I+tZFzo9y3iK31aO4VxCjReQ64+VuuGH9RS6HrTXtldfbgqXNjK0M+wHBI6MB15FX7LUbTUo3ksplmRGKMVzww7GgDGC/wBj+Kru6nOyzv4U/fH7qSLkYJ7ZBorfZVYEMAQeoNFAHnHhvSv7H057i7bN1NmSaRuv0rKsvM8Zay9xOWGk2rYjj7SMO59a2vEUdxL4eu47bLTGPAx3rK0TWbHRfDEEYJNyqnMAHzl/TFACeLGjGtaHZWKBLlZg+UGCq8V1ep6jJplkblbZ7hEGXCMAVHrzXO+GdJuZ7+bW9VXbczcRxn/lmtJ4tvJdRu7bw9Zn57ghp2H8KCgDo9B1tNe08XkUEkMZYhfMx83vWsGqjZWsVjZxW8ChY4lCgVzHi/UdRsb2yh0u/dbm6cKINqlQPXpmgDuAaeDVO3Lx2yCZ9zqo3t0ye5quniDTGnMK38BcHGN46+lAF2606yvsfa7WGfHTzEBqDVtHh1TQ7jTFAhjlTau0cL3HH4VdVs8joaeDxQByXl+IYtAi0a2skjuFjEJvPMHlhem4DrnHtWLeaDHpWteFdGyWthK00jH/AJaSZB5r0kGqmoaXa6rGi3SEmNt8bqcMjeoNAHP/ABFvf+JLFpUPzXWoSrGiDrgEEn+VULO1Gu+LE0qZjJpmhwIhi/hkkxj5h3/+tXS2fhm0t9S/tGeWa8vANqS3DZKD0AAwKxtKC+GPEutyahuS2vXE8U+0lT1yuex5oAfLKNG+IllZ2KiK2vrYtNCowu4bsMB2PFadv4te/nuhpenS3dtaHbJOHChj3CA9a5dmur+61vxRJC8UMNq0FmJBgkf3sfj+tdJ4Ft49P8F2bcAOhlc/Xn+VAG9pmp22r2EV5aPvikHcYII4IPvVwGuH+HSNP4fvW3MkdxdSFCpwQOmRU3hK5u5vEWuwyXs9xaWjrFEJmyQec/yoA7PNIw3AjJGRjIPNZ+p6xbaPD512JRH3dI2YL9SOlWLK8hv7SK6t23QzKHRiMZBoAz9O0D+zdYur6G6eb7Xt84TgFvlGBgjH6iqUUZ0PxbqN3c/LZajGjibHyo6DBDemetdLmlHvQBzPg1Xmm1nUdrLDeXZaEsMblAxn6U7wkcTa7/2Epf5CujdS0bKrFcjG4dRWTpGkSaTNd/6QJ47qZp2ZxhgxxnpxjigDF07VNVvdIvtYSfcYppBHaFRsMa9s9c9ec/hRS6eV8OWeq2N6fLjEkk0Dno6MOgPrnIxRQAA0gtoPM8zyU3/3tozTQalU0AMvDdrBmyEZkH8L9DXP+FbC5g1S+utUiYX0zcNjK7fQGumBp4NAD3mSGJndgFUZJPauP8MK2veILvXpxmKM+VbA9h61uavoyatAyNcTQll25jbGR7in6BpsmkaclmzIyR/dZRgke9AGN4v1G4ur600CwkKS3R/fMvVUq5rem2Gj+CrqBYkVEhwDjkt2OfXNZWnjZ8SL6S8O0mIeSW6EcdKd4pu28R6hb6Dp53xhw9zIvIUDtQB0PhK5uX8JWUswaSUQjAJ5b0o0zxYNQ1uTSmsJoJ4hlyxBC/lV55IdH0ktwsVtF+gFc94CtHmhvNZuB++v5Swz2TtQB22cU8HiuHvtWvNd8SnRdOme3trYbrmeP7x/2Qe1TT3tz4d8SabZC5luLO+yhWZtzI3qDQB2gNBww5GfrVS4v7azCm6njhDdN7AZqW3uYrmMSwSLJGejKcigCWe2iu7WS3mUNFKpRl9Qa5pvD+rw6J/YlnewizIKCdwfMRD/AA46H610+aXNAGfZw2PhrR4bUSLFDCpVWdsbj1P4nmsX4eJv0m7vm+9eXckmfUZxXTyRxzKUlRXQ9VYZFQWWm2mnM5tIhCr9UQ4X8B0FAGZ48ufs/hC/I+86iMfiwFa2iwfZtFsYOnlwov6Vg+MdO1PVrJbW0iikgEqSN8+HwDyOeDXR202+1jcxtFxyrjBX60Ac/He6jB45i0175p7RrZp2Ro1BU5wBkCuivNQt9Ph826k8uPpuIJrmLNvtHxHvXByIbJUB+pBro9RcDTbot0ETH9DQBPZ3tvqFslxaSrLC/wB116GpSa57wMNvhKxx3Vj+bGi61G/s/FNhZNLFJa3nmHHl4ZdoyOc0Ab7KrDDKCPcUVVvdRttPjEl3KI1Y4GepPoBRQB514Q1Ga/0dZLliWUkbj3rbXUbXfs89N2cYzWbolmmm6XHCeAq5Nc1FZxa14uaSBNtvbkbmH8TUAehKwPI6U8Gs+7v7fTbYy3EgRFHGazV8WQiMTSW06W5P+tK8UAdIGp4aqsE6TxLLGwZGGQRU6mgCO70+0vgPtMCSEdCRyPxp1jp1ppyFbSBIs9do61KpzT80Acp42l1O501rKCzfyJHG+ZDn5M+ldDYtFaaFGLXmOKH5cD0FXM5GO1G1SpUgbTxigDk/hunmafeX0nM1zOxYnrTL5hrPxHs4EO6LTk3uR/erQt9Cv9IS4i0i4iWGZiwSVSdhPXGKveH9Bi0OKWR5PNupjummbqTQAzxxNDB4YuWliSR2GyPcM4Y8cVd8MWI0vw7ZwNgFIgX+pGTXN+KrqPV9c0fSoHEiGXzZNpzwK3/E94dO8M3sqcMsW1fx4oAhtvEt1ql5cR6RZpNb27bWmkfaHb0XitPRdbh1q3d41aOSJiksbdUYdqzfBVkth4YtAB80i+Y59SeazPBTGTWdemT/AFLXGB9aAO3zSg1w+oG5t/G+nWtvfXBil3Syxs+QAO1dbe30GnWklzcyBIoxkk0AXM80pwykMAQeorDtPE1nctCHSaDz/wDVNMm0P9DWyGoAoQaDZWt+by0VreZuH2HAcehFSa19pfS7iO1g855I2TaGA6j3q7mgNzQBk+Ela20G1s5o3jnt0CurDGD/AFqtrBz4y0I+iy/+g10IPPFZN3ocFxqEV+kkkdzESVO7I568GgDN187/ABhoSOcxjzGA7bscUVZ1+wlnazvYBuns5N+P7yngiigDiPEmrNZWHlRZ82X5QfTNXPDdium6WpY5kcbnPqaKKAMYu/iXxMYnJ+yWp5U9zWx4vkjtPDc0aqACAoAFFFAFzw2JIvD1sucuE4zWfH4su11xNNmtUDMfvK3aiigDr0anhuaKKAHA08NRRQA8NTs5HPIoooAzJvD9hJeJdxxeTcp0kj4NO8Q6c2qaDc2at87pwT6iiigDBj8Upp/hpLco325E8kIOm7p16VseEdJbR9GVJiGnlYySEHPJoooAzbFvtvxEvpW5FrAqL+NJ41la6vtI0zOI558uPUCiigC544RY/C0jKNrQFGQjsQRUE+t3l3eaZpdnL5Ms8IlmlwCQMds0UUAaNvqlzYa6ml3knnrMm+KXGDx1BrXudUtrSVY5nKu3QBSaKKALSShkDLyDzmms9FFAETyZooooA//Z</t>
+  </si>
+  <si>
+    <t>OPQA-497_1</t>
+  </si>
+  <si>
+    <t>Verify that update user profile summary with exceeds Max length and verify that API should truncate to 1500 characters</t>
+  </si>
+  <si>
+    <t>{"summary":"Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test ..... now leading to last chars 1500. Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length"}</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||summary=Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test ..... now leading to last chars 1500.</t>
   </si>
 </sst>
 </file>
@@ -833,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L28"/>
+      <selection activeCell="L2" sqref="L2:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -893,66 +905,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="45">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:12" ht="225">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="45">
+      <c r="A3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B3" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="4" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>116</v>
+        <v>39</v>
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="31.5">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>81</v>
+        <v>89</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -967,23 +980,23 @@
       <c r="G4" s="1"/>
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>20</v>
+      <c r="J4" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="31.5">
       <c r="A5" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>60</v>
+        <v>90</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -993,22 +1006,22 @@
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="31.5">
       <c r="A6" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>0</v>
@@ -1018,42 +1031,41 @@
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" t="s">
-        <v>21</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="31.5">
       <c r="A8" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1068,72 +1080,74 @@
         <v>25</v>
       </c>
       <c r="H8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="31.5">
+      <c r="A9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="21" customFormat="1" ht="31.5">
-      <c r="A9" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="20" t="s">
+    <row r="10" spans="1:12" s="21" customFormat="1" ht="31.5">
+      <c r="A10" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="21" t="s">
+      <c r="C10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G9"/>
-      <c r="H9" s="22" t="s">
+      <c r="G10"/>
+      <c r="H10" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I9"/>
-      <c r="J9" s="22" t="s">
+      <c r="I10"/>
+      <c r="J10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="K9"/>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:12" ht="180">
-      <c r="A10" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10"/>
-      <c r="J10" t="s">
-        <v>30</v>
-      </c>
+      <c r="K10"/>
+      <c r="L10"/>
     </row>
     <row r="11" spans="1:12" ht="180">
       <c r="A11" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1145,19 +1159,19 @@
         <v>0</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11"/>
       <c r="J11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="31.5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="180">
       <c r="A12" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1169,74 +1183,72 @@
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H12"/>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="31.5">
       <c r="A13" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13"/>
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="31.5">
+      <c r="A14" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B14" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="4" t="s">
+      <c r="G14" s="1"/>
+      <c r="H14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" ht="30">
-      <c r="A14" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" ht="30">
       <c r="A15" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>70</v>
+        <v>103</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1245,19 +1257,24 @@
         <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="8"/>
-      <c r="J15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="255">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1266,24 +1283,19 @@
         <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15.75">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="J16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="255">
       <c r="A17" s="9" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1292,19 +1304,24 @@
         <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="J17" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="240">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1313,157 +1330,154 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="31.5">
+        <v>0</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="J18" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="240">
       <c r="A19" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>82</v>
+        <v>118</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>19</v>
+        <v>41</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="J19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="60">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="31.5">
       <c r="A20" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>83</v>
+        <v>106</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>82</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
       </c>
       <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="60">
+      <c r="A21" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H21" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="31.5">
-      <c r="A21" s="9" t="s">
+    <row r="22" spans="1:12" ht="31.5">
+      <c r="A22" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B22" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
         <v>56</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>0</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21"/>
-      <c r="J21" s="1" t="s">
+      <c r="G22" s="5"/>
+      <c r="H22"/>
+      <c r="J22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="90">
-      <c r="A22" s="9" t="s">
+    <row r="23" spans="1:12" ht="90">
+      <c r="A23" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B23" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F23" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="6" t="s">
+      <c r="G23" s="1"/>
+      <c r="H23" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.75">
-      <c r="A23" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="6"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="31.5">
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>0</v>
@@ -1472,22 +1486,22 @@
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="31.5">
       <c r="A25" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>0</v>
@@ -1496,22 +1510,22 @@
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="31.5">
       <c r="A26" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>0</v>
@@ -1526,16 +1540,16 @@
     </row>
     <row r="27" spans="1:12" ht="31.5">
       <c r="A27" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>0</v>
@@ -1544,39 +1558,63 @@
       <c r="H27" s="6"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" ht="31.5">
+      <c r="A28" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" s="10" customFormat="1" ht="15.75">
-      <c r="A28" s="9" t="s">
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" s="10" customFormat="1" ht="15.75">
+      <c r="A29" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B29" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="10" t="s">
+      <c r="C29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F29" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G28"/>
-      <c r="H28" s="11" t="s">
+      <c r="G29"/>
+      <c r="H29" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I28"/>
-      <c r="J28" s="9" t="s">
+      <c r="I29"/>
+      <c r="J29" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="K28"/>
-      <c r="L28"/>
+      <c r="K29"/>
+      <c r="L29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed failed profile test cases and changed delay time of authoring 500 status.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -133,9 +133,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>status=409||errorCode=409||errorMessage=User already exists.</t>
-  </si>
-  <si>
     <t>/users/user/media</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>Verify that user is not able to update user image without image type and check the error status</t>
   </si>
   <si>
-    <t>errorCode=400||errorMessage=Image Type not set.</t>
-  </si>
-  <si>
     <t>{"imageType": "","imageHeight": 65,"imageWidth": 242,"imageContent":"data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAPIAAABBCAIAAABkVG4oAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAADsMAAA7DAcdvqGQAAA"}</t>
   </si>
   <si>
@@ -392,6 +386,12 @@
   </si>
   <si>
     <t>status=200||truid=(SYS_USER1)||summary=Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test ..... now leading to last chars 1500.</t>
+  </si>
+  <si>
+    <t>status=409||statusCode=Conflict||errorMessage=User already exists.</t>
+  </si>
+  <si>
+    <t>status=400||statusCode=Bad Request||errorMessage=Image Type not set.</t>
   </si>
 </sst>
 </file>
@@ -907,10 +907,10 @@
     </row>
     <row r="2" spans="1:12" ht="225">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>12</v>
@@ -925,18 +925,18 @@
         <v>25</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45">
       <c r="A3" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -948,24 +948,24 @@
         <v>38</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>39</v>
+        <v>124</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -981,16 +981,16 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="31.5">
       <c r="A5" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1012,10 +1012,10 @@
     </row>
     <row r="6" spans="1:12" ht="31.5">
       <c r="A6" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1037,16 +1037,16 @@
     </row>
     <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
@@ -1056,16 +1056,16 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="31.5">
       <c r="A8" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1088,10 +1088,10 @@
     </row>
     <row r="9" spans="1:12" ht="31.5">
       <c r="A9" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -1114,10 +1114,10 @@
     </row>
     <row r="10" spans="1:12" s="21" customFormat="1" ht="31.5">
       <c r="A10" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>12</v>
@@ -1144,10 +1144,10 @@
     </row>
     <row r="11" spans="1:12" ht="180">
       <c r="A11" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1168,10 +1168,10 @@
     </row>
     <row r="12" spans="1:12" ht="180">
       <c r="A12" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1192,10 +1192,10 @@
     </row>
     <row r="13" spans="1:12" ht="31.5">
       <c r="A13" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1216,10 +1216,10 @@
     </row>
     <row r="14" spans="1:12" ht="31.5">
       <c r="A14" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1235,140 +1235,140 @@
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75">
       <c r="A16" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
         <v>0</v>
       </c>
       <c r="H16" s="8"/>
       <c r="J16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="255">
       <c r="A17" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
       </c>
       <c r="H18" s="8"/>
       <c r="J18" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="240">
       <c r="A19" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" t="s">
         <v>65</v>
-      </c>
-      <c r="J19" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="31.5">
       <c r="A20" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -1391,42 +1391,42 @@
     </row>
     <row r="21" spans="1:12" ht="60">
       <c r="A21" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="31.5">
       <c r="A22" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
@@ -1439,45 +1439,45 @@
     </row>
     <row r="23" spans="1:12" ht="90">
       <c r="A23" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>0</v>
@@ -1486,22 +1486,22 @@
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="31.5">
       <c r="A25" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>0</v>
@@ -1510,22 +1510,22 @@
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="31.5">
       <c r="A26" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>0</v>
@@ -1540,16 +1540,16 @@
     </row>
     <row r="27" spans="1:12" ht="31.5">
       <c r="A27" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>0</v>
@@ -1564,16 +1564,16 @@
     </row>
     <row r="28" spans="1:12" ht="31.5">
       <c r="A28" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>0</v>
@@ -1588,10 +1588,10 @@
     </row>
     <row r="29" spans="1:12" s="10" customFormat="1" ht="15.75">
       <c r="A29" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>12</v>
@@ -1603,7 +1603,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G29"/>
       <c r="H29" s="11" t="s">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="I29"/>
       <c r="J29" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K29"/>
       <c r="L29"/>

</xml_diff>

<commit_message>
Fixed Profile failed test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="121">
   <si>
     <t>GET</t>
   </si>
@@ -127,9 +127,6 @@
     <t>status=404||errorCode=404||errorMessage=User not found.</t>
   </si>
   <si>
-    <t>/users/user</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>{"title": "Project Neon1"}</t>
   </si>
   <si>
-    <t>status=400||errorCode=400||errorMessage=Missing one or more required values.</t>
-  </si>
-  <si>
     <t>/users/user/(SYS_USER2)/image</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
     <t>/users/user/(SYS_USER2)a/raw/image</t>
   </si>
   <si>
-    <t>Content-Type=application/json</t>
-  </si>
-  <si>
     <t>{}</t>
   </si>
   <si>
@@ -187,21 +178,12 @@
     <t>/users/user/(SYS_USER1)a/media</t>
   </si>
   <si>
-    <t>{"truid":"(SYS_USER1)","firstName": "Project","lastName": "Neon1","title": "Project Neon 1","role": "QA","primaryInstitution": "Thomson reuters, Bangalore","location": "india"}</t>
-  </si>
-  <si>
-    <t>Verify that user profile is not created with existing truid and check the error status</t>
-  </si>
-  <si>
     <t>Verify that for the invalid user id, user profile is not returned and check the error status</t>
   </si>
   <si>
     <t>Verify that for the missing truid, user profile is not returned and check the error status</t>
   </si>
   <si>
-    <t>Verify that without manadatory data, user profile is not updated and check the error status</t>
-  </si>
-  <si>
     <t>Verify that for the existing media in S3, not able to upload again and check the error status</t>
   </si>
   <si>
@@ -274,9 +256,6 @@
     <t>status=500</t>
   </si>
   <si>
-    <t>OPQA-683</t>
-  </si>
-  <si>
     <t>OPQA-494</t>
   </si>
   <si>
@@ -388,10 +367,16 @@
     <t>status=200||truid=(SYS_USER1)||summary=Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test ..... now leading to last chars 1500.</t>
   </si>
   <si>
-    <t>status=409||statusCode=Conflict||errorMessage=User already exists.</t>
-  </si>
-  <si>
     <t>status=400||statusCode=Bad Request||errorMessage=Image Type not set.</t>
+  </si>
+  <si>
+    <t>Verify that user is able update only profile title and check no error is displayed throught API.</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=SM||interest=computers||title=Project Neon1</t>
+  </si>
+  <si>
+    <t>status=400||statusCode=Bad Request||errorMessage=Image Content not set</t>
   </si>
 </sst>
 </file>
@@ -845,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L29"/>
+      <selection activeCell="L2" sqref="L2:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -907,10 +892,10 @@
     </row>
     <row r="2" spans="1:12" ht="225">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>12</v>
@@ -925,47 +910,43 @@
         <v>25</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="45">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="H3" s="4"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>124</v>
+      <c r="J3" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="30">
+    <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>68</v>
+        <v>81</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -980,23 +961,23 @@
       <c r="G4" s="1"/>
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="7" t="s">
-        <v>114</v>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="31.5">
       <c r="A5" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -1006,22 +987,22 @@
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="31.5">
       <c r="A6" s="9" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>0</v>
@@ -1031,41 +1012,42 @@
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="31.5">
       <c r="A8" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1080,74 +1062,72 @@
         <v>25</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="31.5">
-      <c r="A9" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="21" customFormat="1" ht="31.5">
+      <c r="A9" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="21" customFormat="1" ht="31.5">
-      <c r="A10" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10"/>
-      <c r="H10" s="22" t="s">
+      <c r="G9"/>
+      <c r="H9" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I10"/>
-      <c r="J10" s="22" t="s">
+      <c r="I9"/>
+      <c r="J9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="K10"/>
-      <c r="L10"/>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="1:12" ht="180">
+      <c r="A10" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10"/>
+      <c r="J10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="180">
       <c r="A11" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1159,19 +1139,19 @@
         <v>0</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H11"/>
       <c r="J11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="180">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="31.5">
       <c r="A12" s="9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1183,301 +1163,301 @@
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H12"/>
       <c r="J12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="31.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="45">
       <c r="A13" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75">
+      <c r="A15" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13"/>
-      <c r="J13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="31.5">
-      <c r="A14" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="H15" s="8"/>
+      <c r="J15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="255">
+      <c r="A16" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
         <v>11</v>
       </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="4" t="s">
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
+      <c r="A17" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" ht="30">
-      <c r="A15" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="J17" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="240">
+      <c r="A18" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="F15" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75">
-      <c r="A16" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="J16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="255">
-      <c r="A17" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75">
-      <c r="A18" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="8"/>
-      <c r="J18" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="240">
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="31.5">
       <c r="A19" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>70</v>
+        <v>97</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>64</v>
+        <v>25</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="31.5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="60">
       <c r="A20" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>81</v>
+        <v>98</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>76</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="J20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="60">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="31.5">
       <c r="A21" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>82</v>
+        <v>99</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21"/>
+      <c r="J21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="90">
+      <c r="A22" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J21" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="31.5">
-      <c r="A22" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75">
+      <c r="A23" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22"/>
-      <c r="J22" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="90">
-      <c r="A23" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" t="s">
-        <v>40</v>
-      </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="H23" s="6"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75">
+    <row r="24" spans="1:12" ht="31.5">
       <c r="A24" s="9" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>0</v>
@@ -1486,22 +1466,22 @@
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="31.5">
       <c r="A25" s="9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>0</v>
@@ -1510,22 +1490,22 @@
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="31.5">
       <c r="A26" s="9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>0</v>
@@ -1540,16 +1520,16 @@
     </row>
     <row r="27" spans="1:12" ht="31.5">
       <c r="A27" s="9" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>0</v>
@@ -1558,63 +1538,39 @@
       <c r="H27" s="6"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="31.5">
+    <row r="28" spans="1:12" s="10" customFormat="1" ht="15.75">
       <c r="A28" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="1:12" s="10" customFormat="1" ht="15.75">
-      <c r="A29" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29"/>
-      <c r="H29" s="11" t="s">
+      <c r="F28" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="I29"/>
-      <c r="J29" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="K29"/>
-      <c r="L29"/>
+      <c r="I28"/>
+      <c r="J28" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K28"/>
+      <c r="L28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added test cases for Vanilla & Admin Profile APIs.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Profile" sheetId="1" r:id="rId1"/>
+    <sheet name="Vanilla-Profile" sheetId="1" r:id="rId1"/>
+    <sheet name="Admin-Profile" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="193">
   <si>
     <t>GET</t>
   </si>
@@ -337,9 +338,6 @@
     <t>OPQA-711</t>
   </si>
   <si>
-    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=SM</t>
-  </si>
-  <si>
     <t>OPQA-502_1</t>
   </si>
   <si>
@@ -377,6 +375,225 @@
   </si>
   <si>
     <t>status=400||statusCode=Bad Request||errorMessage=Image Content not set</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)","firstName": "Project","lastName": "Neon1","title": "API Automation Tester","role": "QA","primaryInstitution": "Thomson reuters, Bangalore","location": "india", "onboarded": false}</t>
+  </si>
+  <si>
+    <t>Verify that for the existing active truid, getOnboardedStatus API works as expected.</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER1)/status/onboarded</t>
+  </si>
+  <si>
+    <t>Verify that for the existing active truid, updateOnboardedStatus API works as expected.</t>
+  </si>
+  <si>
+    <t>/users/user</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||onboarded=true</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "onboarded": true}</t>
+  </si>
+  <si>
+    <t>status=409||statusCode=Conflict||errorMessage=User already exists.</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, API doesn't allow to create same profile again and check the error status</t>
+  </si>
+  <si>
+    <t>Verify that for the existing active truid, update active status  using  updateUserStatus of Admin API works as expected.</t>
+  </si>
+  <si>
+    <t>/admin/users/user/(SYS_USER1)/status</t>
+  </si>
+  <si>
+    <t>{"truid": "(SYS_USER1)","active": false,"onboarded": false}</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||active=false||deleted=false||onboarded=false</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||active=true||deleted=false||onboarded=false</t>
+  </si>
+  <si>
+    <t>{"truid": "(SYS_USER1)","active": true,"onboarded": false}</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||onboarded=false</t>
+  </si>
+  <si>
+    <t>Verify that for the inactive user id, user profile is not returned and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER1),(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project||lastName=Neon2||location=India||truid=(SYS_USER2)||location=INdia||primaryInstitution=Thomson reuters||role=QA</t>
+  </si>
+  <si>
+    <t>Verify that inactive user is not able to edit  info like title,role,Institution and country using Vanilla API &amp; check the error status.</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user image is not returned and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user raw image is not returned and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER1)/raw/image</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER1)/media</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user media info is not returned and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user media image is not returned and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user image is not updated and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER1)/media/image</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user media is not uploaded and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)","mediaType": "jpeg","base64Content":"data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD//gA7Q1JFQVRPUjogZ2QtanBlZyB2MS4wICh1c2luZyBJSkcgSlBFRyB2ODApLCBxdWFsaXR5ID0gNjUK/9sAQwALCAgKCAcLCgkKDQwLDREcEhEPDxEiGRoUHCkkKyooJCcnLTJANy0wPTAnJzhMOT1DRUhJSCs2T1VORlRAR0hF/9sAQwEMDQ0RDxEhEhIhRS4nLkVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVFRUVF/8AAEQgAlwDIAwEiAAIRAQMRAf/EAB8AAAEFAQEBAQEBAAAAAAAAAAABAgMEBQYHCAkKC//EALUQAAIBAwMCBAMFBQQEAAABfQECAwAEEQUSITFBBhNRYQcicRQygZGhCCNCscEVUtHwJDNicoIJChYXGBkaJSYnKCkqNDU2Nzg5OkNERUZHSElKU1RVVldYWVpjZGVmZ2hpanN0dXZ3eHl6g4SFhoeIiYqSk5SVlpeYmZqio6Slpqeoqaqys7S1tre4ubrCw8TFxsfIycrS09TV1tfY2drh4uPk5ebn6Onq8fLz9PX29/j5+v/EAB8BAAMBAQEBAQEBAQEAAAAAAAABAgMEBQYHCAkKC//EALURAAIBAgQEAwQHBQQEAAECdwABAgMRBAUhMQYSQVEHYXETIjKBCBRCkaGxwQkjM1LwFWJy0QoWJDThJfEXGBkaJicoKSo1Njc4OTpDREVGR0hJSlNUVVZXWFlaY2RlZmdoaWpzdHV2d3h5eoKDhIWGh4iJipKTlJWWl5iZmqKjpKWmp6ipqrKztLW2t7i5usLDxMXGx8jJytLT1NXW19jZ2uLj5OXm5+jp6vLz9PX29/j5+v/aAAwDAQACEQMRAD8A6+OaEy+UJUMg/h3DP5U6bSrO8minnt0eWJg6P3BHQ1zXlx6Cp1nVwLrV7g+XFHEOhPSNB/M1bv8AUtT0zRpL++uYoblh+5s4owwLn7qZPLH1xigDWv8ARmu9WstQV1Y2isFhkzsJP8XHcVHJYi3uxq2sym4eAEwxwxkpF6kDqT7mrDaxHYaVb3mqqbcui+YApYIxxxx7mtOGRZokkQna6hhkY4NAGNokE+o3Z1q83QiQYgt1bhU9Xx1Y/pVq41iX+24dOsYkuGxuuCSQIV7En1PYVotErxlclR6ocEVRsdHTS7S6jspGM05Z/Nl+Zi56EnvQBcbU7NLlrdp1MyjLIvJUe+OlOMNnfeTchI5dp3RyDnHuDXOadZajpWiC0tLMtqs+TPdSMNm89XJ6n2FOnz4f0Sz0XS5Wm1ObKxkHoc5Z29ACf6UAbUulA6wNThYeeIfJCycqBnOR6Gsa40W7h1WKV5nkjunLXs6cHCj5EGOQtakuqjTPsdhK0l7qMy8JGoBbHVz2UVat9Uhl1KTT5AY7uOMSlM5BUnGQfqKAKOnfaZdcmmhR4NMjh8tVcY8x853AHsBxVnTNY+2reTuESygcqk+cB8feP0ByM1oSwxXULROdyMMHa2P5Vm3/AIfin8P/ANlWreVENu1exAOdp9j0oAtrdWOowqpZJIpgQoYcOPbPWrMkLC1MVuwjO3apIzj0rIutOur3UdPZ1S3srFvMwGyztjAHsBS2l7NfeJLpYJj9gtIwkncPKeeD7D+dADZrC607Q7e0sXO4SKJpV+8VJ+Zh7morvWn06+YRRSTWoRUBP8UrNgAE+3WrcPiGCe0ub1In+xQMVMx6NjqQO4960ZFt7uFVk2Mj4ZeevcEUAQ/2jHHc/Z7rbHJ5Xm5zxtHXmmvY2d9Eyq2YnYOyo3DHrzVbUvD8N7HOwZjPKFUs5z8qnO36Gq2qJqUEst7ZxhFgtiir13sSOcegAoA02tpv7WSfAEMcRUAHqc96rRapNHDC90BvlnMflgcrycVJHftDf21k7+cZYTIWHBBGPTsc1Ytri2vJJSigvbyFG3L0bH/16AFJtbi7aBkBljxIQR+RpGtGE11NFJh5k2j/AGSBxSfYVM9xOkp3zoEJ/u46Y/OqtrBdWsljAiHaikTOTweOD9c0AWLdrmOWKJkZk8o72bsw9/eo2ltbvT287ESSsYzzyTnH9Kli1FQL1rggR2zYLDuMA/1pTb211GqxjYVYSqMYIPXOKAKF5YysZZ7STc7QhE56MM4P+NFSXFrc2lpdvC7NK8nmIqDoOMj9D+dFAGTfaTBqL2skhZJbWTzIpEPKn8eDTP7DiS6GoTibULuP/ViVhhP90cKD706XW7GC6+ymZpLgDJihRpGUe4UHH41esb+21CDzrWVZEyVOOoI6gg8g0AYdpZ3Ovaq15rELwQWb4t7Jxxn/AJ6MejH0x0o0++uvE91cXK3Mlno9s5jTyztecjqxbqF+ldOKy5PDWnSo8RSRLeRy7wRyssbMepKg0AU/DOoXGo6pqT28jyaRGwS3eQlizj7xBPJWtPSdeTVb27to7eRfsjbXlyGQt6Ajqap61BqkOl/Y9Bt4Yo2ATejbWiXvtXgZx05qjrbN4Z8P2Gl6IvlS3ky2yTN/AW6uf9qgDsRKm/bvXd6Z5qL+z7Q3i3YgjW4AI81RhiPQnuK4nX7O10rSodF0pPO1q8dQkpOZQc5MjN1Fb+uazP4f0q1KhLq8kZYUibO6d+Bxjp3NAFp9GeLXptXtnR5pYBCUlzhQDkEEdPpUNrYR6C17q+pzm4vJxmSREOFUDhFHPH862YpWW0SS6CRNsBkG75VOOeafBcwXKFoJo5VBwSjAigDD8JWsj28+r3K7LjUW8wRA8RJ/Cv1xyfc1aXV55fFD6XBGkkEMQknk5BjJ+6vuT1rVMQ8oohMY9UwMVn6Voo0lb0pM00t1IZWlkHzFj6kdh2oAstqdktxJAbhPMjGXUHOz6+n41OkMOGeNEHmDkqPvVx2nLcaJ4XuraS0ln1i5eXcoQt5rsThi3TbjHertw9z4X8DQIZi19BEkSd98hwAvPUZP5CgC3L4bDaSdKhuTFYsTuULlipOSuaZqsD3Or6TaRxOlrBIZnlxgfKMKufcn9K2bdpo7GM3H7ycIN+wYy2OcCo9L1O21e0+02jFot5TLLjkHBoAg13UZNLsklgCvK8qRJG38RYgVanvre2lhhnkAmmzsQAknHXgdqbe6bb38kEkwbfbyCSMg8Bh0OKr3Ng665BqagyBIGhZB1GSDkflQBciit2JmgVNzDG9QM/SsyTR5otL1GC2nJnumeQSdCGaq1ol1p+k6teXm63MkstxHGGGUXHH48Z/GtPSJriXRLSe4/eXDwq79skjNAFOBpodRsYLeKRYvJbz9wOFIxjn1zVu11MOb43G1I7SQqX7EbQc/rU2n38Wp2a3MQYIxZfm68HB/lTJNLt3trqFQVW6B8zB6kjGaAHILO+gkVACs6ZIxgsD3pEsHW8WdptyLD5QQDrz1NVUsbr7fYMSoitY2V2B5fIAHH60Qag0A1V5GaRLVyVHfG0HAoAYl3c2lhHvQs5ufKJk/hUscH+VFXIryO6WOK4jCNNH5gQnII7/lRQBwYubLwrpy2Glp9t1ObkIp3PI5/jc9hVnTLaPwp4buZ9SuiJ5S008q4zvbsuep7CtqC1t7cH7PDFET3RAKxbjQr6/1y0uNRniurG2+ZIVBTD9mYc7vzoAteGbjU206W+1ufZG/zxJIqqY4/ViAOasr4q01oXuFaZrRDhroRN5Q5x97HT36VieJjLqniLTNCkYw6fIpmmOcedt/gz+H60eILn+2FTwvoYUq+FuZo+Ut4x/D9TjpQB2sbq6K6MGVhkEHIIpZoIbqIxXESSxnqrjIrlPE14+k6ZZaZpUsy6jLthtY42GcAY3NkHgCul0+Ke2sIY7u4a6nRPnlKgFz9BxQAtppdnZM72dtFDI/V1Tk/U9TWZBod7J4q/tTU5IbiOKLZarHkCIn7xIPc+uas6b4is9S1G4sIkuEubYAypLEV2+nPTvWwOtAGJ4n8RJo9g6WxWXUZmEVvAOpduhx6DrVrwzoq6Do8duTvuHPm3En9+Q9TV2e1t7tNlxCkq9QGXOPpRdR3DWxWymSGUfdZ03jp6ZFAGTp2s3t74rvtPi8mSws0HmTbCGEh6IDnBwK1Jtb063u2tZbtBOg3OgySg9Wx0/GsvQNIuPD/h6aDCzX3zyNKDnzpDyCc9OwxWJ4Xv7TQvBE2p3zqb6dpHnVz+8eXcQEx1zwOKAO9jkSWNXjdXRhkMpyCKoaloltqk1vLM0ge3kEseGO3cOhK9DWF4YhuNF8BI99K1vIkb3DErkxgktjB9u1afhO/v8AU/D9ve6mFEtxl1Crtwn8OffHP40AXNZa9XSrgadCJbkxkICwXBxwaZ4esF0zQrO0UMPKjCtuGDu7/rmpbfWLK4v3sElIu0Te0ToysFzjPI6VcdFkQo6hlPBBoA57w9dS3Wq63cebIbKKYQwozEgFR85GferFp4nhudPbUWt5IrDzCizMRyM43Y7DNXrbSbWytpre1j8qGXcSingE9SK5670TUl8Kp4eto0cHERuSwCrHuzkjrnHagDqJoYbuExzRrLG45VhkEUCHyrfy4MKFGFB5ArnfEKqt7oFnC2JWulBZThtiKSR9OBV+71iVfEEGk2sKNI8JnkeRiAq5wBgdyaAJdFsG0vR4rO4KuYgdzjo2STnH41lafqDWPhrUr5F8wwzTuiE44DHA+lbNjqsN3HcFyIXtZDFMrNwrD39CCDVgpb3du+BHLFKpBK4IYdOtAFGHUpI5rKC8Cb7tCyNHnG4DJHPt/KrqS2100salHZflkXuM9jVH+xFN5ZTNcOY7IN5UWB1Ixye+BTLNZE8Rag7xukcscWxmHDEbs4/SgCwukqLq0lEzeXahhHHj1GOT7Cimw3Uy+IJ7NpC8X2dZkBAyDuIP8hRQBjWWo2t+jNazLJsOGA4Kn3B5FXVPFeaaZrL2l9d6y8DyXWrMEtLNerKOjH06da3tS1jWdC0tdSvntGG9Q1qiEHBPQNnr+FAHWTW0F0my5gjmX0kUMP1oW0S3tmisEhtSfulYhtH1AxmoG1O1hto57meOBZFDASuF6jpzVm3uYbqISwSpLGejIwIP5UAYuj6JeQ6/eanqzRXFxIuyCSPIWNP7oU9PrVjxF4mg0axkW3dJtQdhFDbqcsXbpkelbSmormwtL5QLq3il2nKllBKn1B6g/SgDE023g8FeGJ72/fzLkgz3MneSQ9F/XApmkQalqWmyaxrOoXFt5qGWKCB9iwJjIJ/vHHPNX/FGgnX9CewjlET7ldC2SCV6A+1UtWsNb1yxj0sRxadaMAtxMsu9nUfwoB0B96AGaB4zjbwxaXmsSE3M0jRRLGmXnwcAhR/+qugs9ctbu8+xMstvd7PMEE6bWZfUdj+BrjvCenxS+LtUkkQCPSMWdpG38CjPzfU4zn3NKdRXVPHM2rxHOnaJbtD5g6SSHOQPz/T3o2Gk27I9CEsbMyK6ll6gHkVG9laSTLNJbQtKOkhQFh+NeZWVyLrVZJ7u9ktN5LGVM5z2HH+eK6DQfEV02qrYPJ9sgZiqzbcHHrWKq3O+rgJQTcXeyuza8UaNe65pj2dteJDFJt8xGT74ByRuB4z9DWojxWGnxmVRBHEiqVHIQDjHTpVW512xs71bS4l2SEA5I45rSBBGe1a3RwuMo2bW5yXgxv7U1PWteb7txP5EGe0aDj8yaXw/fah4lXUNTN9JbWqytFaRRquAF/ibI5zXVRW0ELO8UUaM5y5VQN319a5xfDuoaZpt3p2i3MEdvcOzK0oO6AN94DHX26UyS74f8Qf2p4bh1O4jZWO5XESFuVYgkAc44zWnp+oW2qWaXVlIJYHztbBGcHB61gXxtPB3gmW0jlwYbZ1iLcF3IPP1yc1o+F7L7B4Y0636MsClsepGT+poAvXFha3Msc0sKGaM5SQDDL9D1qndaUx1mHVbYr5yRGB42OA6E5HPYg1n6FfXdx4l1q0e5ea0szGkfmBchiCTyAK1LzWrawvLe2uRKjXLiOJvLJVmPbIoAoaXYSaVDql5qMkQlvJjMwU5VBgADJ69KTwUCfCNiQcFlds+mXY1vkAjB5FRxwRwqywosYY5+QAc0AZukahPdT6nDcsjCzn8sOq7cjaDzz71PZaxZagFNvKWDkhCylQ+Ou3PX8Kr2Ojy2cupb5xMt85kLY2lTt24x07Vzlwzab4VtNOkG3UrS5jSFR958SfeX1BX+tAHYfYIBf8A2xQyzlNhOeq5zjH1oqhe3M9r4h02NZnMF15ivGcEZC5BHcd6KAPOdBa2j8Rarf6tJHDNbt5cMchx5cY6FRVbXtUbV2GpTxMui2TZhRxg3Uvbj0/pXdyWlvOwaaCORh0LKCRWb4k0I63p8MULrHJBKJUDD5WI7GgCr4d0cpA2ta8VlvZV3jzOVgTrgDtxUXgVnu9Q1rUYlMdhcz/uExgHGcnH5VYv9M1jXo0tLt4bGx481YXLvKPTOBgVb1HVLHwtoLLa7MwgRQwIckueg/rQAReJrtvE/wDYpsY3YDe8sUxIjXtnjr7e9dRnFcr4T0s6Npc1/qTD7bdZnuZG/hHXH4VnaKk3ja+m1HUDINIicpbWwJUSEfxNjrQB3oPpTq4fRrj7N8QL7S9OJGnx26tJECSscnHT061uah4ptNL1CCyura7WS4fZCyxgrIeOhB9xQBeutE0++leW4twZHG13RihYehIIyPrVbUPDsMukpp+nbLOFG3BET5T9a1wacDSaurMqE3CSlHdHHW1lqeiW0tvJpkN7A5yWXk5/z7VL4Rs7+0vJppoXhtipJDDHPtXWrmnjpWaprQ7JYyUoyi477nn+nh9c8VeZIMr5hc+yjoP0FdB4u1eaxjt4bWUxys24lTzgU258OT2t+19o0yxSnJaN+hz1rOm0LWdY1NZdQVEQYBYEYA9hUWkk1bVnWp0qtSNSTXLFbHSafqf2fRYLnVZ1V5BnJGM+nH0qS38SaXcuES6VWPQOCv8AOuW8Zo8d7aJyIFiwuOgOef6Vp3aaJpscFvPYl4ZEz56rkfnV8zvbsc7w9NwU9W5X26HUMkc0ZR1V0YYIIyCKYlutvbeTaBYQAQgxkL+FY3h6JY5ZjZ3vn2OBsQnJQ+hq8uvWLaoums7pdsCVjeJl3AdSCRgitE7o4akeSVih4e0a70m71OS7eOZr64Nx5seR1/h2npj6mqXiC5iu/F3h2yjdWeKeSaRM8rhDjI/GurqGe0t7oAXEKSbTldwzg+o9KZBzt9PcX3jq30wzyxWcVmbhkicp5jbsDJHOBVrRtSnOpatpcxa4awZWjc43OjLkAn1HTNWtQ0cz6lb6naOsV7AhjBcZWRD1U/jzmq+j6RLplzqWpX8qy3V4weTygdqKowAO54oAvaXq0Wqi5EUcsb20phkSUDIYD2J9aukA84Fcz4PmSebXJEYENfuw+mBinu7W/jq3hjllEM9pI7xmQlSwYc4J4/CgDTv9L+23tpdrO6S2jFkXgoSQQcjr0PrRVWTX3/ta6s7ayedbNFed1cAjPQKO5wPUUUAUQakBrir3UdSl8Vx6fpd6WjHzTgoCIx6ZrrXuI7aIyTyKiKOWY4FAFxTWff8Ah7TNTkWW5tl85SGWVPlYH1yKLPWdPvZPLtruKR/QNya0AaAKetafNfeHbuxt5D50kJRWc8k+/wBaxdO1O60jw1badaaVdNqUcfliMxEIG/vF+mO9dWDTwaAMLwnoDaFaT3F7IJL+6bzLiT0Pp9BWZoWfFHi261uQE2VjmCzB6E/xN/n1rotW0ttUtniS9uLUujITERgg+oNN8OaU+iaUlixiZYuFaMEbh6ketAGXret3154gi8P6LKIZtvmXNzgN5S+gB7/4ik1C+u/DevaPbLezXdvfuYpI5yGYHjDA49+lUfCJjsfEPiOXUpFiumuCf3pxmPJIIz2qjd6i2q69ceIyhOk6NEwtywwJZPUfif0FAHd3fiHTbC7FrNcZucbvKiRpGA9SFBxV6xvrbULcT2kyTRE43Ke/p9a5P4f6cYtIOq3eXvtQYyySv1254H071iaN4jj0V/E2pqC9tJdhLaIdJJDnp+hNAHqOacDXGz6xr2kaIusakLV4wVaa0SMq0ak44bPJGfSuoivYJLOO6EirBIgdXY4GCMigA1HTrfVLcw3KZHUEdVPqK5270DV4rNrO1uluLU4wr8MK6iKeOZA8Tq6noynIqUdalxTN6WInT0Wq89TH8LabNpmnuLlNk0jkkZzx2rNjb7d8UJu62FiF+jOc/wAjXVOodCpzhhg4OD+dY+neHotL1a5vra4lZrvAnE53k4zjDdR196aVlYzqVHUk5y3ZSu9RvdS8Zf2NZ3TWttawedcSRgF2J6LyDjrVrRdXnk1nUdGvWEs9ntdJQMGSNumQOMj2qm1rJo3jW61WRGNjfW6o0qqW8t1x1A5wQOtR+GYZr7xTrOuNE8dtMFgty6lS6r1bB7cCmQdBaa5YX17JZ28xNzGu94mRlYDOM8gVerk9MPnfEfWZO0NpFF+eD/SpI7y/1bxZqNlDdta2unxoP3aqS7sM5OQeB6UAdKIIhMZRGokIwXA5I+tZFzo9y3iK31aO4VxCjReQ64+VuuGH9RS6HrTXtldfbgqXNjK0M+wHBI6MB15FX7LUbTUo3ksplmRGKMVzww7GgDGC/wBj+Kru6nOyzv4U/fH7qSLkYJ7ZBorfZVYEMAQeoNFAHnHhvSv7H057i7bN1NmSaRuv0rKsvM8Zay9xOWGk2rYjj7SMO59a2vEUdxL4eu47bLTGPAx3rK0TWbHRfDEEYJNyqnMAHzl/TFACeLGjGtaHZWKBLlZg+UGCq8V1ep6jJplkblbZ7hEGXCMAVHrzXO+GdJuZ7+bW9VXbczcRxn/lmtJ4tvJdRu7bw9Zn57ghp2H8KCgDo9B1tNe08XkUEkMZYhfMx83vWsGqjZWsVjZxW8ChY4lCgVzHi/UdRsb2yh0u/dbm6cKINqlQPXpmgDuAaeDVO3Lx2yCZ9zqo3t0ye5quniDTGnMK38BcHGN46+lAF2606yvsfa7WGfHTzEBqDVtHh1TQ7jTFAhjlTau0cL3HH4VdVs8joaeDxQByXl+IYtAi0a2skjuFjEJvPMHlhem4DrnHtWLeaDHpWteFdGyWthK00jH/AJaSZB5r0kGqmoaXa6rGi3SEmNt8bqcMjeoNAHP/ABFvf+JLFpUPzXWoSrGiDrgEEn+VULO1Gu+LE0qZjJpmhwIhi/hkkxj5h3/+tXS2fhm0t9S/tGeWa8vANqS3DZKD0AAwKxtKC+GPEutyahuS2vXE8U+0lT1yuex5oAfLKNG+IllZ2KiK2vrYtNCowu4bsMB2PFadv4te/nuhpenS3dtaHbJOHChj3CA9a5dmur+61vxRJC8UMNq0FmJBgkf3sfj+tdJ4Ft49P8F2bcAOhlc/Xn+VAG9pmp22r2EV5aPvikHcYII4IPvVwGuH+HSNP4fvW3MkdxdSFCpwQOmRU3hK5u5vEWuwyXs9xaWjrFEJmyQec/yoA7PNIw3AjJGRjIPNZ+p6xbaPD512JRH3dI2YL9SOlWLK8hv7SK6t23QzKHRiMZBoAz9O0D+zdYur6G6eb7Xt84TgFvlGBgjH6iqUUZ0PxbqN3c/LZajGjibHyo6DBDemetdLmlHvQBzPg1Xmm1nUdrLDeXZaEsMblAxn6U7wkcTa7/2Epf5CujdS0bKrFcjG4dRWTpGkSaTNd/6QJ47qZp2ZxhgxxnpxjigDF07VNVvdIvtYSfcYppBHaFRsMa9s9c9ec/hRS6eV8OWeq2N6fLjEkk0Dno6MOgPrnIxRQAA0gtoPM8zyU3/3tozTQalU0AMvDdrBmyEZkH8L9DXP+FbC5g1S+utUiYX0zcNjK7fQGumBp4NAD3mSGJndgFUZJPauP8MK2veILvXpxmKM+VbA9h61uavoyatAyNcTQll25jbGR7in6BpsmkaclmzIyR/dZRgke9AGN4v1G4ur600CwkKS3R/fMvVUq5rem2Gj+CrqBYkVEhwDjkt2OfXNZWnjZ8SL6S8O0mIeSW6EcdKd4pu28R6hb6Dp53xhw9zIvIUDtQB0PhK5uX8JWUswaSUQjAJ5b0o0zxYNQ1uTSmsJoJ4hlyxBC/lV55IdH0ktwsVtF+gFc94CtHmhvNZuB++v5Swz2TtQB22cU8HiuHvtWvNd8SnRdOme3trYbrmeP7x/2Qe1TT3tz4d8SabZC5luLO+yhWZtzI3qDQB2gNBww5GfrVS4v7azCm6njhDdN7AZqW3uYrmMSwSLJGejKcigCWe2iu7WS3mUNFKpRl9Qa5pvD+rw6J/YlnewizIKCdwfMRD/AA46H610+aXNAGfZw2PhrR4bUSLFDCpVWdsbj1P4nmsX4eJv0m7vm+9eXckmfUZxXTyRxzKUlRXQ9VYZFQWWm2mnM5tIhCr9UQ4X8B0FAGZ48ufs/hC/I+86iMfiwFa2iwfZtFsYOnlwov6Vg+MdO1PVrJbW0iikgEqSN8+HwDyOeDXR202+1jcxtFxyrjBX60Ac/He6jB45i0175p7RrZp2Ro1BU5wBkCuivNQt9Ph826k8uPpuIJrmLNvtHxHvXByIbJUB+pBro9RcDTbot0ETH9DQBPZ3tvqFslxaSrLC/wB116GpSa57wMNvhKxx3Vj+bGi61G/s/FNhZNLFJa3nmHHl4ZdoyOc0Ab7KrDDKCPcUVVvdRttPjEl3KI1Y4GepPoBRQB514Q1Ga/0dZLliWUkbj3rbXUbXfs89N2cYzWbolmmm6XHCeAq5Nc1FZxa14uaSBNtvbkbmH8TUAehKwPI6U8Gs+7v7fTbYy3EgRFHGazV8WQiMTSW06W5P+tK8UAdIGp4aqsE6TxLLGwZGGQRU6mgCO70+0vgPtMCSEdCRyPxp1jp1ppyFbSBIs9do61KpzT80Acp42l1O501rKCzfyJHG+ZDn5M+ldDYtFaaFGLXmOKH5cD0FXM5GO1G1SpUgbTxigDk/hunmafeX0nM1zOxYnrTL5hrPxHs4EO6LTk3uR/erQt9Cv9IS4i0i4iWGZiwSVSdhPXGKveH9Bi0OKWR5PNupjummbqTQAzxxNDB4YuWliSR2GyPcM4Y8cVd8MWI0vw7ZwNgFIgX+pGTXN+KrqPV9c0fSoHEiGXzZNpzwK3/E94dO8M3sqcMsW1fx4oAhtvEt1ql5cR6RZpNb27bWmkfaHb0XitPRdbh1q3d41aOSJiksbdUYdqzfBVkth4YtAB80i+Y59SeazPBTGTWdemT/AFLXGB9aAO3zSg1w+oG5t/G+nWtvfXBil3Syxs+QAO1dbe30GnWklzcyBIoxkk0AXM80pwykMAQeorDtPE1nctCHSaDz/wDVNMm0P9DWyGoAoQaDZWt+by0VreZuH2HAcehFSa19pfS7iO1g855I2TaGA6j3q7mgNzQBk+Ela20G1s5o3jnt0CurDGD/AFqtrBz4y0I+iy/+g10IPPFZN3ocFxqEV+kkkdzESVO7I568GgDN187/ABhoSOcxjzGA7bscUVZ1+wlnazvYBuns5N+P7yngiigDiPEmrNZWHlRZ82X5QfTNXPDdium6WpY5kcbnPqaKKAMYu/iXxMYnJ+yWp5U9zWx4vkjtPDc0aqACAoAFFFAFzw2JIvD1sucuE4zWfH4su11xNNmtUDMfvK3aiigDr0anhuaKKAHA08NRRQA8NTs5HPIoooAzJvD9hJeJdxxeTcp0kj4NO8Q6c2qaDc2at87pwT6iiigDBj8Upp/hpLco325E8kIOm7p16VseEdJbR9GVJiGnlYySEHPJoooAzbFvtvxEvpW5FrAqL+NJ41la6vtI0zOI558uPUCiigC544RY/C0jKNrQFGQjsQRUE+t3l3eaZpdnL5Ms8IlmlwCQMds0UUAaNvqlzYa6ml3knnrMm+KXGDx1BrXudUtrSVY5nKu3QBSaKKALSShkDLyDzmms9FFAETyZooooA//Z"}</t>
+  </si>
+  <si>
+    <t>status=404||statusCode=Not Found||errorMessage=User not found.</t>
+  </si>
+  <si>
+    <t>status=200||mediaCategory=image-full||truid=(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, Admin API doesn't allow to create same profile again and check the error status</t>
+  </si>
+  <si>
+    <t>/admin/users/user</t>
+  </si>
+  <si>
+    <t>Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>/admin/users/user/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>truid=(SYS_USER1)||firstName=Project||lastName=Neon1||title=Project Neon1||primaryInstitution=Thomson Reuters||location=India||summary=I am test user for API Automation||active=true||deleted=false||onboarded=false</t>
+  </si>
+  <si>
+    <t>Verify that for the invalid user id, user profile is not returned using Admin API and check the error status</t>
+  </si>
+  <si>
+    <t>/admin/users/user/(SYS_USER1)1</t>
+  </si>
+  <si>
+    <t>truid=(SYS_USER1)||active=true||deleted=false||onboarded=false</t>
+  </si>
+  <si>
+    <t>{"truid": "(SYS_USER1)","active": false,"onboarded": true}</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||active=false||deleted=false||onboarded=true</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, user status is updated using Admin updateUserStatus API</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, user status is returned using Admin getUserStatus API</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, user profile is returned using Admin getUser API</t>
+  </si>
+  <si>
+    <t>Verify that for the inactive truid, user profile is not updated using Admin updateUser API and check the error status</t>
+  </si>
+  <si>
+    <t>Verify that for the existing active truid, user profile is updated using Admin updateUser API</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)","firstName": "Project","lastName": "Neon1","title": "API Automation Tester","role": "QA","primaryInstitution": "Thomson reuters, Bangalore","location": "india","onboarded": true}</t>
+  </si>
+  <si>
+    <t>truid=(SYS_USER1)||firstName=Project||lastName=Neon1||title=API Automation Tester||primaryInstitution=Thomson Reuters||location=India||summary=I am test user for API Automation||userStatusEntity.truid=(SYS_USER1)||userStatusEntity.active.userState=true||userStatusEntity.deleted.userState=false||userStatusEntity.onboarded.userState=false</t>
+  </si>
+  <si>
+    <t>OPQA-2574</t>
+  </si>
+  <si>
+    <t>OPQA-2575</t>
+  </si>
+  <si>
+    <t>OPQA-2576</t>
+  </si>
+  <si>
+    <t>OPQA-2577</t>
+  </si>
+  <si>
+    <t>OPQA-2577_1</t>
+  </si>
+  <si>
+    <t>OPQA-2578</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id in the bulk list, user profile is not returned and check the bulk profiles in the response using Vanilla API</t>
+  </si>
+  <si>
+    <t>OPQA-2579</t>
+  </si>
+  <si>
+    <t>OPQA-2580</t>
+  </si>
+  <si>
+    <t>OPQA-2581</t>
+  </si>
+  <si>
+    <t>OPQA-2582</t>
+  </si>
+  <si>
+    <t>OPQA-2583</t>
+  </si>
+  <si>
+    <t>OPQA-2584</t>
+  </si>
+  <si>
+    <t>OPQA-2585</t>
+  </si>
+  <si>
+    <t>OPQA-2586</t>
+  </si>
+  <si>
+    <t>OPQA-2587</t>
+  </si>
+  <si>
+    <t>OPQA-2588</t>
+  </si>
+  <si>
+    <t>OPQA-2589</t>
+  </si>
+  <si>
+    <t>OPQA-2590</t>
+  </si>
+  <si>
+    <t>OPQA-2591</t>
+  </si>
+  <si>
+    <t>OPQA-2591_1</t>
+  </si>
+  <si>
+    <t>OPQA-2592</t>
+  </si>
+  <si>
+    <t>OPQA-2593</t>
   </si>
 </sst>
 </file>
@@ -440,7 +657,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -463,24 +680,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -506,12 +710,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -830,15 +1028,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -847,16 +1045,16 @@
     <col min="7" max="7" width="96.42578125" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="80.5703125" style="5" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="90.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="90.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -880,7 +1078,7 @@
       <c r="I1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
@@ -894,8 +1092,8 @@
       <c r="A2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>114</v>
+      <c r="B2" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>12</v>
@@ -910,17 +1108,17 @@
         <v>25</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="12" t="s">
         <v>62</v>
       </c>
       <c r="C3" t="s">
@@ -937,7 +1135,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>107</v>
+        <v>167</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -945,7 +1143,7 @@
       <c r="A4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C4" t="s">
@@ -961,7 +1159,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="K4" s="1"/>
@@ -970,7 +1168,7 @@
       <c r="A5" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="12" t="s">
         <v>54</v>
       </c>
       <c r="C5" t="s">
@@ -986,7 +1184,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="4" t="s">
         <v>36</v>
       </c>
       <c r="K5" s="1"/>
@@ -995,7 +1193,7 @@
       <c r="A6" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C6" t="s">
@@ -1011,7 +1209,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="4"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="4" t="s">
         <v>43</v>
       </c>
       <c r="K6" s="1"/>
@@ -1020,7 +1218,7 @@
       <c r="A7" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>84</v>
       </c>
       <c r="C7" t="s">
@@ -1038,7 +1236,7 @@
       <c r="H7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1046,7 +1244,7 @@
       <c r="A8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>86</v>
       </c>
       <c r="C8" t="s">
@@ -1068,31 +1266,31 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="21" customFormat="1" ht="31.5">
-      <c r="A9" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="B9" s="20" t="s">
+    <row r="9" spans="1:12" s="19" customFormat="1" ht="31.5">
+      <c r="A9" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="21" t="s">
+      <c r="C9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="19" t="s">
         <v>25</v>
       </c>
       <c r="G9"/>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="20" t="s">
         <v>26</v>
       </c>
       <c r="I9"/>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="20" t="s">
         <v>27</v>
       </c>
       <c r="K9"/>
@@ -1102,7 +1300,7 @@
       <c r="A10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C10" t="s">
@@ -1118,7 +1316,7 @@
         <v>33</v>
       </c>
       <c r="H10"/>
-      <c r="J10" t="s">
+      <c r="J10" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1126,7 +1324,7 @@
       <c r="A11" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C11" t="s">
@@ -1142,7 +1340,7 @@
         <v>34</v>
       </c>
       <c r="H11"/>
-      <c r="J11" t="s">
+      <c r="J11" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1150,7 +1348,7 @@
       <c r="A12" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C12" t="s">
@@ -1166,7 +1364,7 @@
         <v>29</v>
       </c>
       <c r="H12"/>
-      <c r="J12" t="s">
+      <c r="J12" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1174,8 +1372,8 @@
       <c r="A13" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="14" t="s">
-        <v>118</v>
+      <c r="B13" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1195,7 +1393,7 @@
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K13" s="1"/>
     </row>
@@ -1203,7 +1401,7 @@
       <c r="A14" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>73</v>
       </c>
       <c r="C14" t="s">
@@ -1221,15 +1419,15 @@
       <c r="H14" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75">
+      <c r="J14" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="210">
       <c r="A15" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>63</v>
       </c>
       <c r="C15" t="s">
@@ -1242,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="8"/>
-      <c r="J15" t="s">
+      <c r="J15" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1250,7 +1448,7 @@
       <c r="A16" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C16" t="s">
@@ -1266,17 +1464,17 @@
         <v>39</v>
       </c>
       <c r="H16" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J16" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15.75">
+    </row>
+    <row r="17" spans="1:12" ht="210">
       <c r="A17" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>63</v>
       </c>
       <c r="C17" t="s">
@@ -1289,15 +1487,15 @@
         <v>0</v>
       </c>
       <c r="H17" s="8"/>
-      <c r="J17" s="8" t="s">
-        <v>112</v>
+      <c r="J17" s="7" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="240">
       <c r="A18" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C18" t="s">
@@ -1315,7 +1513,7 @@
       <c r="H18" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1323,7 +1521,7 @@
       <c r="A19" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>75</v>
       </c>
       <c r="C19" t="s">
@@ -1341,7 +1539,7 @@
       <c r="H19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1349,7 +1547,7 @@
       <c r="A20" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>76</v>
       </c>
       <c r="C20" t="s">
@@ -1367,15 +1565,15 @@
       <c r="H20" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J20" t="s">
-        <v>117</v>
+      <c r="J20" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="31.5">
       <c r="A21" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="12" t="s">
         <v>71</v>
       </c>
       <c r="C21" t="s">
@@ -1389,7 +1587,7 @@
       </c>
       <c r="G21" s="5"/>
       <c r="H21"/>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1397,7 +1595,7 @@
       <c r="A22" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C22" t="s">
@@ -1417,7 +1615,7 @@
         <v>40</v>
       </c>
       <c r="I22" s="1"/>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="K22" s="1"/>
@@ -1426,7 +1624,7 @@
       <c r="A23" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C23" t="s">
@@ -1441,7 +1639,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="6"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="1" t="s">
+      <c r="J23" s="4" t="s">
         <v>61</v>
       </c>
       <c r="K23" s="1"/>
@@ -1450,7 +1648,7 @@
       <c r="A24" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C24" t="s">
@@ -1465,7 +1663,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1" t="s">
+      <c r="J24" s="4" t="s">
         <v>47</v>
       </c>
       <c r="K24" s="1"/>
@@ -1474,7 +1672,7 @@
       <c r="A25" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C25" t="s">
@@ -1489,7 +1687,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="K25" s="1"/>
@@ -1498,7 +1696,7 @@
       <c r="A26" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="12" t="s">
         <v>66</v>
       </c>
       <c r="C26" t="s">
@@ -1513,7 +1711,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="6"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1" t="s">
+      <c r="J26" s="4" t="s">
         <v>22</v>
       </c>
       <c r="K26" s="1"/>
@@ -1522,7 +1720,7 @@
       <c r="A27" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>65</v>
       </c>
       <c r="C27" t="s">
@@ -1537,7 +1735,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="6"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1" t="s">
+      <c r="J27" s="4" t="s">
         <v>36</v>
       </c>
       <c r="K27" s="1"/>
@@ -1546,7 +1744,7 @@
       <c r="A28" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -1566,11 +1764,657 @@
         <v>26</v>
       </c>
       <c r="I28"/>
-      <c r="J28" s="9" t="s">
+      <c r="J28" s="14" t="s">
         <v>79</v>
       </c>
       <c r="K28"/>
       <c r="L28"/>
+    </row>
+    <row r="29" spans="1:12" ht="45">
+      <c r="A29" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" ht="30">
+      <c r="A30" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30"/>
+      <c r="J30" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="30">
+      <c r="A31" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="45">
+      <c r="A32" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="31.5">
+      <c r="A33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="47.25">
+      <c r="A34" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="I34" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="47.25">
+      <c r="A35" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="47.25">
+      <c r="A36" t="s">
+        <v>179</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36"/>
+      <c r="I36" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="47.25">
+      <c r="A37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37"/>
+      <c r="I37" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="47.25">
+      <c r="A38" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>143</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38"/>
+      <c r="I38" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="47.25">
+      <c r="A39" t="s">
+        <v>182</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39"/>
+      <c r="I39" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="240">
+      <c r="A40" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>25</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="255">
+      <c r="A41" t="s">
+        <v>184</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" t="s">
+        <v>25</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="45">
+      <c r="A42" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="68.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="64.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="47.25">
+      <c r="A2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" ht="60">
+      <c r="A3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3"/>
+      <c r="I3" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="31.5">
+      <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5"/>
+      <c r="J5" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45">
+      <c r="A6" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45">
+      <c r="A7" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45">
+      <c r="A8" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="90">
+      <c r="A9" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed failed test cases in Profile.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="192">
   <si>
     <t>GET</t>
   </si>
@@ -468,9 +468,6 @@
   </si>
   <si>
     <t>status=404||statusCode=Not Found||errorMessage=User not found.</t>
-  </si>
-  <si>
-    <t>status=200||mediaCategory=image-full||truid=(SYS_USER1)</t>
   </si>
   <si>
     <t>Verify that for the existing truid, Admin API doesn't allow to create same profile again and check the error status</t>
@@ -1030,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="I41" workbookViewId="0">
+      <selection activeCell="L42" sqref="L2:L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1135,7 +1132,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K3" s="1"/>
     </row>
@@ -1772,7 +1769,7 @@
     </row>
     <row r="29" spans="1:12" ht="45">
       <c r="A29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>128</v>
@@ -1801,7 +1798,7 @@
     </row>
     <row r="30" spans="1:12" ht="30">
       <c r="A30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>121</v>
@@ -1822,7 +1819,7 @@
     </row>
     <row r="31" spans="1:12" ht="30">
       <c r="A31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>123</v>
@@ -1848,7 +1845,7 @@
     </row>
     <row r="32" spans="1:12" ht="45">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>129</v>
@@ -1874,7 +1871,7 @@
     </row>
     <row r="33" spans="1:10" ht="31.5">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>136</v>
@@ -1892,7 +1889,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="4"/>
       <c r="I33" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>36</v>
@@ -1900,10 +1897,10 @@
     </row>
     <row r="34" spans="1:10" ht="47.25">
       <c r="A34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
@@ -1920,7 +1917,7 @@
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>138</v>
@@ -1928,7 +1925,7 @@
     </row>
     <row r="35" spans="1:10" ht="47.25">
       <c r="A35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>139</v>
@@ -1949,7 +1946,7 @@
         <v>18</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>150</v>
@@ -1957,7 +1954,7 @@
     </row>
     <row r="36" spans="1:10" ht="47.25">
       <c r="A36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>140</v>
@@ -1973,7 +1970,7 @@
       </c>
       <c r="H36"/>
       <c r="I36" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>36</v>
@@ -1981,7 +1978,7 @@
     </row>
     <row r="37" spans="1:10" ht="47.25">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>141</v>
@@ -1997,7 +1994,7 @@
       </c>
       <c r="H37"/>
       <c r="I37" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>36</v>
@@ -2005,7 +2002,7 @@
     </row>
     <row r="38" spans="1:10" ht="47.25">
       <c r="A38" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>144</v>
@@ -2021,15 +2018,15 @@
       </c>
       <c r="H38"/>
       <c r="I38" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>151</v>
+        <v>172</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="47.25">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>145</v>
@@ -2045,7 +2042,7 @@
       </c>
       <c r="H39"/>
       <c r="I39" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J39" s="4" t="s">
         <v>36</v>
@@ -2053,7 +2050,7 @@
     </row>
     <row r="40" spans="1:10" ht="240">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>146</v>
@@ -2074,7 +2071,7 @@
         <v>58</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J40" s="4" t="s">
         <v>36</v>
@@ -2082,7 +2079,7 @@
     </row>
     <row r="41" spans="1:10" ht="255">
       <c r="A41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>148</v>
@@ -2103,7 +2100,7 @@
         <v>149</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>36</v>
@@ -2111,7 +2108,7 @@
     </row>
     <row r="42" spans="1:10" ht="45">
       <c r="A42" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>129</v>
@@ -2132,7 +2129,7 @@
         <v>134</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>133</v>
@@ -2148,8 +2145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L2:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2206,29 +2203,29 @@
     </row>
     <row r="2" spans="1:12" ht="47.25">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>152</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>153</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
         <v>120</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>127</v>
@@ -2237,40 +2234,40 @@
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3"/>
       <c r="I3" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>157</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>158</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -2286,10 +2283,10 @@
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -2302,15 +2299,15 @@
       </c>
       <c r="F5"/>
       <c r="J5" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -2325,37 +2322,37 @@
         <v>25</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>120</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>150</v>
@@ -2363,10 +2360,10 @@
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -2384,7 +2381,7 @@
         <v>134</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>133</v>
@@ -2392,28 +2389,28 @@
     </row>
     <row r="9" spans="1:12" ht="90">
       <c r="A9" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H9" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>168</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed failed test cases in Profile Module
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Vanilla-Profile" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="185">
   <si>
     <t>GET</t>
   </si>
@@ -74,12 +74,6 @@
     <t>{"firstName": "Project"}</t>
   </si>
   <si>
-    <t>status=200||firstName=Project||lastName=Neon1</t>
-  </si>
-  <si>
-    <t>status=200||interest=computers||interest=science</t>
-  </si>
-  <si>
     <t>status=200</t>
   </si>
   <si>
@@ -104,12 +98,6 @@
     <t>status=200||truid=(SYS_USER1)||truid=(SYS_USER2)</t>
   </si>
   <si>
-    <t>status=413||errorCode=413||errorMessage=Too many TRUIDs provided</t>
-  </si>
-  <si>
-    <t>status=400||errorCode=400||errorMessage=TRUID is missing</t>
-  </si>
-  <si>
     <t>?id=(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2),(SYS_USER1),(SYS_USER2)</t>
   </si>
   <si>
@@ -119,9 +107,6 @@
     <t>/users/user/(SYS_USER1)1</t>
   </si>
   <si>
-    <t>status=404||errorCode=404||errorMessage=User not found.</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
@@ -131,9 +116,6 @@
     <t>/users/user/</t>
   </si>
   <si>
-    <t>status=400||errorCode=400||errorMessage=TRUID is missing.</t>
-  </si>
-  <si>
     <t>{"title": "Project Neon1"}</t>
   </si>
   <si>
@@ -143,9 +125,6 @@
     <t>/users/user/(SYS_USER2)/media</t>
   </si>
   <si>
-    <t>status=404||errorCode=404||errorMessage=Media not found.</t>
-  </si>
-  <si>
     <t>/users/user/(SYS_USER2)/media/image</t>
   </si>
   <si>
@@ -320,18 +299,12 @@
     <t>status=200||truid=(SYS_USER1)||summary=Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test ..... now leading to last chars 1500.</t>
   </si>
   <si>
-    <t>status=400||statusCode=Bad Request||errorMessage=Image Type not set.</t>
-  </si>
-  <si>
     <t>Verify that user is able update only profile title and check no error is displayed throught API.</t>
   </si>
   <si>
     <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=SM||interest=computers||title=Project Neon1</t>
   </si>
   <si>
-    <t>status=400||statusCode=Bad Request||errorMessage=Image Content not set</t>
-  </si>
-  <si>
     <t>{"truid":"(SYS_USER1)","firstName": "Project","lastName": "Neon1","title": "API Automation Tester","role": "QA","primaryInstitution": "Thomson reuters, Bangalore","location": "india", "onboarded": false}</t>
   </si>
   <si>
@@ -353,9 +326,6 @@
     <t>{"truid":"(SYS_USER1)", "onboarded": true}</t>
   </si>
   <si>
-    <t>status=409||statusCode=Conflict||errorMessage=User already exists.</t>
-  </si>
-  <si>
     <t>Verify that for the existing truid, API doesn't allow to create same profile again and check the error status</t>
   </si>
   <si>
@@ -413,9 +383,6 @@
     <t>/users/user/(SYS_USER1)/media/image</t>
   </si>
   <si>
-    <t>status=404||statusCode=Not Found||errorMessage=User not found.</t>
-  </si>
-  <si>
     <t>Verify that for the existing truid, Admin API doesn't allow to create same profile again and check the error status</t>
   </si>
   <si>
@@ -557,17 +524,58 @@
     <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||title=Project Neon2||imageHeight=97||imageWidth=97||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg==</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>status=404||statusCode=404||errorMessage=User not found.</t>
+  </si>
+  <si>
+    <t>status=400||statusCode=400||errorMessage=TRUID is missing.</t>
+  </si>
+  <si>
+    <t>status=413||statusCode=413||errorMessage=Too many TRUIDs provided.</t>
+  </si>
+  <si>
+    <t>status=400||statusCode=400||errorMessage=Image Content not set</t>
+  </si>
+  <si>
+    <t>status=400||statusCode=400||errorMessage=Image Type not set.</t>
+  </si>
+  <si>
+    <t>status=404||statusCode=404||errorMessage=Media not found.</t>
+  </si>
+  <si>
+    <t>status=409||statusCode=409||errorMessage=User already exists.</t>
+  </si>
+  <si>
+    <t>status=200||interest=computers||interest=science||interest=API AUTOMATION</t>
+  </si>
+  <si>
+    <t>OPQA-2679</t>
+  </si>
+  <si>
+    <t>Verify that user is able to edit first name and last name from his own profile page.</t>
+  </si>
+  <si>
+    <t>{"firstName":"ProjectEdited","lastName":"Neon1Edited"}</t>
+  </si>
+  <si>
+    <t>status=200||firstName=ProjectEdited||lastName=Neon1Edited||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
+  </si>
+  <si>
+    <t>status=200||firstName=ProjectEdited||lastName=Neon1Edited</t>
+  </si>
+  <si>
+    <t>OPQA-2679_1</t>
+  </si>
+  <si>
+    <t>{"firstName":"Project","lastName":"Neon1"}</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA||title=Project Neon1||interest=API AUTOMATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -996,26 +1004,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="I38" workbookViewId="0">
-      <selection activeCell="L39" sqref="L2:L39"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="49.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="52.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="96.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="80.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="5" width="90.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="52.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="96.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="80.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="90.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1058,10 +1066,10 @@
     </row>
     <row r="2" spans="1:12" ht="225">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>12</v>
@@ -1073,27 +1081,21 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2"/>
+        <v>21</v>
+      </c>
       <c r="H2" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="I2"/>
+        <v>92</v>
+      </c>
       <c r="J2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2"/>
-      <c r="L2" t="s">
-        <v>181</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1109,19 +1111,16 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>64</v>
+        <v>177</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>178</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1129,33 +1128,34 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1"/>
+      <c r="E4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>179</v>
+      </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="4" t="s">
-        <v>19</v>
+      <c r="J4" s="7" t="s">
+        <v>180</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="31.5">
       <c r="A5" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -1163,841 +1163,704 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="9" t="s">
+        <v>177</v>
+      </c>
       <c r="J5" s="4" t="s">
-        <v>34</v>
+        <v>181</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="31.5">
+    </row>
+    <row r="6" spans="1:12" ht="45">
       <c r="A6" s="9" t="s">
-        <v>73</v>
+        <v>182</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>49</v>
+        <v>178</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4" t="s">
+        <v>183</v>
+      </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="4" t="s">
-        <v>38</v>
+      <c r="J6" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="9" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="I7"/>
-      <c r="J7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>181</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="31.5">
       <c r="A8" s="9" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" ht="31.5">
+      <c r="A9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="31.5">
+      <c r="A10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="19" customFormat="1" ht="31.5">
+      <c r="A11" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11"/>
+      <c r="J11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G8"/>
-      <c r="H8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8"/>
-      <c r="J8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="19" customFormat="1" ht="31.5">
-      <c r="A9" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9"/>
-      <c r="H9" s="20" t="s">
+      <c r="K11"/>
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="1:12" ht="180">
+      <c r="A12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>24</v>
-      </c>
-      <c r="I9"/>
-      <c r="J9" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="180">
-      <c r="A10" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10"/>
-      <c r="G10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="180">
-      <c r="A11" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11"/>
-      <c r="G11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="31.5">
-      <c r="A12" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
-      <c r="F12"/>
       <c r="G12" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H12"/>
-      <c r="I12"/>
       <c r="J12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12"/>
-      <c r="L12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="45">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="180">
       <c r="A13" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13"/>
+      <c r="J13" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="31.5">
+      <c r="A14" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14"/>
+      <c r="J14" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45">
+      <c r="A15" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="K13" s="1"/>
-      <c r="L13" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="30">
-      <c r="A14" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14"/>
-      <c r="H14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I14"/>
-      <c r="J14" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K14"/>
-      <c r="L14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="210">
-      <c r="A15" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15" s="8"/>
-      <c r="I15"/>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="1"/>
       <c r="J15" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="K15"/>
-      <c r="L15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="255">
+        <v>95</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" ht="30">
       <c r="A16" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>55</v>
+        <v>77</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16"/>
+        <v>31</v>
+      </c>
       <c r="H16" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="I16"/>
-      <c r="J16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>172</v>
-      </c>
-      <c r="K16"/>
-      <c r="L16" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="210">
       <c r="A17" s="9" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
       </c>
-      <c r="F17"/>
-      <c r="G17"/>
       <c r="H17" s="8"/>
-      <c r="I17"/>
       <c r="J17" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="K17"/>
-      <c r="L17" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="240">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="255">
       <c r="A18" s="9" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18"/>
+        <v>31</v>
+      </c>
       <c r="H18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18"/>
+        <v>159</v>
+      </c>
       <c r="J18" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="K18"/>
-      <c r="L18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="31.5">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="210">
       <c r="A19" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>65</v>
+        <v>88</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19"/>
-      <c r="H19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19"/>
-      <c r="J19" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="K19"/>
-      <c r="L19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="60">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8"/>
+      <c r="J19" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="240">
       <c r="A20" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>66</v>
+        <v>89</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>48</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20"/>
-      <c r="H20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I20"/>
+        <v>31</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="J20" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="K20"/>
-      <c r="L20" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="31.5">
       <c r="A21" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>61</v>
+        <v>80</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21"/>
-      <c r="G21" s="5"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="60">
+      <c r="A22" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
         <v>34</v>
       </c>
-      <c r="K21"/>
-      <c r="L21" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.75">
-      <c r="A22" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K22" s="1"/>
-      <c r="L22" t="s">
-        <v>181</v>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="31.5">
       <c r="A23" s="9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
         <v>0</v>
       </c>
-      <c r="F23"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="1"/>
+      <c r="G23" s="5"/>
+      <c r="H23"/>
       <c r="J23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K23" s="1"/>
-      <c r="L23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="31.5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="9" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F24"/>
       <c r="G24" s="1"/>
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
       <c r="J24" s="4" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="K24" s="1"/>
-      <c r="L24" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="25" spans="1:12" ht="31.5">
       <c r="A25" s="9" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F25"/>
       <c r="G25" s="1"/>
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="4" t="s">
-        <v>34</v>
+        <v>174</v>
       </c>
       <c r="K25" s="1"/>
-      <c r="L25" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="10" customFormat="1" ht="15.75">
+    </row>
+    <row r="26" spans="1:12" ht="31.5">
       <c r="A26" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
         <v>36</v>
       </c>
-      <c r="G26"/>
-      <c r="H26" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26"/>
-      <c r="J26" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="K26"/>
-      <c r="L26" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="45">
-      <c r="A27" t="s">
-        <v>148</v>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" ht="31.5">
+      <c r="A27" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>113</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>37</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="H27" s="6"/>
       <c r="I27" s="1"/>
       <c r="J27" s="4" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
       <c r="K27" s="1"/>
-      <c r="L27" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="30">
-      <c r="A28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B28" s="5" t="s">
+    </row>
+    <row r="28" spans="1:12" s="10" customFormat="1" ht="15.75">
+      <c r="A28" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28"/>
+      <c r="J28" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K28"/>
+      <c r="L28"/>
+    </row>
+    <row r="29" spans="1:12" ht="45">
+      <c r="A29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" ht="30">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30"/>
+      <c r="J30" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="30">
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="45">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>124</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" t="s">
-        <v>107</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="J28" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="K28"/>
-      <c r="L28" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="30">
-      <c r="A29" t="s">
-        <v>150</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29"/>
-      <c r="H29" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I29"/>
-      <c r="J29" s="4" t="s">
+    </row>
+    <row r="33" spans="1:10" ht="31.5">
+      <c r="A33" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>110</v>
-      </c>
-      <c r="K29"/>
-      <c r="L29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="45">
-      <c r="A30" t="s">
-        <v>151</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" t="s">
-        <v>115</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" t="s">
-        <v>135</v>
-      </c>
-      <c r="G30"/>
-      <c r="H30" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="I30"/>
-      <c r="J30" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="K30"/>
-      <c r="L30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="31.5">
-      <c r="A31" t="s">
-        <v>153</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K31"/>
-      <c r="L31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="47.25">
-      <c r="A32" t="s">
-        <v>155</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="K32"/>
-      <c r="L32" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="47.25">
-      <c r="A33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
@@ -2005,213 +1868,228 @@
       <c r="D33" t="s">
         <v>15</v>
       </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>23</v>
-      </c>
-      <c r="G33"/>
-      <c r="H33" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="4"/>
       <c r="I33" s="9" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="K33"/>
-      <c r="L33" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="47.25">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H34" s="4"/>
       <c r="I34" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34"/>
-      <c r="L34" t="s">
-        <v>181</v>
+        <v>140</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="47.25">
       <c r="A35" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I35" s="9" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K35"/>
-      <c r="L35" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="47.25">
       <c r="A36" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>127</v>
-      </c>
-      <c r="E36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
         <v>0</v>
       </c>
-      <c r="F36"/>
-      <c r="G36"/>
       <c r="H36"/>
       <c r="I36" s="9" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K36"/>
-      <c r="L36" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="47.25">
       <c r="A37" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F37"/>
-      <c r="G37"/>
       <c r="H37"/>
       <c r="I37" s="9" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K37"/>
-      <c r="L37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="240">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="47.25">
       <c r="A38" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
       </c>
       <c r="D38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38"/>
+      <c r="I38" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="47.25">
+      <c r="A39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>121</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39"/>
+      <c r="I39" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="240">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
         <v>16</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E40" t="s">
         <v>11</v>
       </c>
-      <c r="F38" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38"/>
-      <c r="H38" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="K38"/>
-      <c r="L38" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="45">
-      <c r="A39" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s">
-        <v>115</v>
-      </c>
-      <c r="E39" s="9" t="s">
+      <c r="F40" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="45">
+      <c r="A41" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F39" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39"/>
-      <c r="H39" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="K39"/>
-      <c r="L39" t="s">
-        <v>181</v>
+      <c r="F41" t="s">
+        <v>124</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2224,22 +2102,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L2:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="51.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="5" width="30.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="68.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="5" width="64.140625" collapsed="true"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="51.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="68.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="64.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2282,80 +2160,71 @@
     </row>
     <row r="2" spans="1:12" ht="47.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>112</v>
+        <v>175</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
       <c r="I3" s="9" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3" t="s">
-        <v>181</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -2365,171 +2234,140 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>34</v>
+        <v>169</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
       <c r="J5" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>181</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" s="9" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6"/>
+        <v>124</v>
+      </c>
       <c r="H6" s="5" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="9" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G7"/>
+        <v>124</v>
+      </c>
       <c r="H7" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" s="9" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8"/>
+        <v>21</v>
+      </c>
       <c r="H8" s="5" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>181</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="90">
       <c r="A9" s="9" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G9"/>
+        <v>124</v>
+      </c>
       <c r="H9" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="I9"/>
+        <v>162</v>
+      </c>
       <c r="J9" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed profile test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="180">
   <si>
     <t>GET</t>
   </si>
@@ -77,9 +77,6 @@
     <t>status=200</t>
   </si>
   <si>
-    <t>status=200||location=India||primaryInstitution=Thomson Reuters||role=SM</t>
-  </si>
-  <si>
     <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
   </si>
   <si>
@@ -302,9 +299,6 @@
     <t>Verify that user is able update only profile title and check no error is displayed throught API.</t>
   </si>
   <si>
-    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=SM||interest=computers||title=Project Neon1</t>
-  </si>
-  <si>
     <t>{"truid":"(SYS_USER1)","firstName": "Project","lastName": "Neon1","title": "API Automation Tester","role": "QA","primaryInstitution": "Thomson reuters, Bangalore","location": "india", "onboarded": false}</t>
   </si>
   <si>
@@ -419,12 +413,6 @@
     <t>Verify that for the existing truid, user profile is returned using Admin getUser API</t>
   </si>
   <si>
-    <t>Verify that for the inactive truid, user profile is not updated using Admin updateUser API and check the error status</t>
-  </si>
-  <si>
-    <t>Verify that for the existing active truid, user profile is updated using Admin updateUser API</t>
-  </si>
-  <si>
     <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
   </si>
   <si>
@@ -488,12 +476,6 @@
     <t>OPQA-2591_1</t>
   </si>
   <si>
-    <t>OPQA-2592</t>
-  </si>
-  <si>
-    <t>OPQA-2593</t>
-  </si>
-  <si>
     <t>{"imageType": "png","imageHeight":97,"imageWidth":97,"imageContent":"data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg=="}</t>
   </si>
   <si>
@@ -503,12 +485,6 @@
     <t>status=200||truid=(SYS_USER2)||mediaCategory=image-full</t>
   </si>
   <si>
-    <t>{"truid":"(SYS_USER1)","firstName": "Project","lastName": "Neon1","title": "Project Neon1","role": "QA","primaryInstitution": "Thomson reuters, Bangalore","location": "india","onboarded": true}</t>
-  </si>
-  <si>
-    <t>truid=(SYS_USER1)||firstName=Project||lastName=Neon1||title=Project Neon1||primaryInstitution=Thomson Reuters||location=India||summary=I am test user for API Automation||userStatusEntity.truid=(SYS_USER1)||userStatusEntity.active.userState=true||userStatusEntity.deleted.userState=false||userStatusEntity.onboarded.userState=false</t>
-  </si>
-  <si>
     <t>{"interest":["computers","science","API AUTOMATION"]}</t>
   </si>
   <si>
@@ -570,6 +546,15 @@
   </si>
   <si>
     <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA||title=Project Neon1||interest=API AUTOMATION</t>
+  </si>
+  <si>
+    <t>{"location":"India","primaryInstitution":"Thomson Reuters","role":"QA"}</t>
+  </si>
+  <si>
+    <t>status=200||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA||interest=computers||title=Project Neon1</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1051,10 @@
     </row>
     <row r="2" spans="1:12" ht="225">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>12</v>
@@ -1081,21 +1066,21 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1111,16 +1096,16 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="9" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1132,24 +1117,24 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="7" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="31.5">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1164,19 +1149,19 @@
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
       <c r="I5" s="9" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="9" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1188,30 +1173,30 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="4" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
@@ -1221,22 +1206,22 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="31.5">
       <c r="A8" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>0</v>
@@ -1246,16 +1231,16 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="31.5">
       <c r="A9" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -1267,21 +1252,21 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="31.5">
       <c r="A10" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1293,21 +1278,21 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>17</v>
+        <v>177</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>20</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="19" customFormat="1" ht="31.5">
       <c r="A11" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>12</v>
@@ -1319,97 +1304,97 @@
         <v>11</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11"/>
       <c r="H11" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11"/>
       <c r="J11" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K11"/>
       <c r="L11"/>
     </row>
     <row r="12" spans="1:12" ht="180">
       <c r="A12" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12"/>
       <c r="J12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="180">
       <c r="A13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H13"/>
       <c r="J13" s="5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5">
       <c r="A14" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14"/>
       <c r="J14" s="5" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45">
       <c r="A15" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1421,144 +1406,144 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="7" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="210">
       <c r="A17" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
         <v>0</v>
       </c>
       <c r="H17" s="8"/>
       <c r="J17" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="255">
       <c r="A18" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="210">
       <c r="A19" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
         <v>0</v>
       </c>
       <c r="H19" s="8"/>
       <c r="J19" s="7" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="240">
       <c r="A20" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="31.5">
       <c r="A21" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1570,53 +1555,53 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="60">
       <c r="A22" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
         <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="31.5">
       <c r="A23" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
@@ -1624,21 +1609,21 @@
       <c r="G23" s="5"/>
       <c r="H23"/>
       <c r="J23" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>0</v>
@@ -1647,22 +1632,22 @@
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
       <c r="J24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="31.5">
       <c r="A25" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>0</v>
@@ -1671,22 +1656,22 @@
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="4" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="31.5">
       <c r="A26" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>0</v>
@@ -1701,16 +1686,16 @@
     </row>
     <row r="27" spans="1:12" ht="31.5">
       <c r="A27" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>0</v>
@@ -1719,16 +1704,16 @@
       <c r="H27" s="6"/>
       <c r="I27" s="1"/>
       <c r="J27" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:12" s="10" customFormat="1" ht="15.75">
       <c r="A28" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>12</v>
@@ -1740,127 +1725,127 @@
         <v>11</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G28"/>
       <c r="H28" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I28"/>
       <c r="J28" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K28"/>
       <c r="L28"/>
     </row>
     <row r="29" spans="1:12" ht="45">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="4" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:12" ht="30">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>0</v>
       </c>
       <c r="H30"/>
       <c r="J30" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="30">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="45">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="31.5">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
@@ -1875,46 +1860,46 @@
       <c r="G33" s="1"/>
       <c r="H33" s="4"/>
       <c r="I33" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="47.25">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="47.25">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
@@ -1926,24 +1911,24 @@
         <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="47.25">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
@@ -1956,90 +1941,90 @@
       </c>
       <c r="H36"/>
       <c r="I36" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="47.25">
       <c r="A37" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H37"/>
       <c r="I37" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="47.25">
       <c r="A38" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H38"/>
       <c r="I38" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="47.25">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B39" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
         <v>119</v>
-      </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s">
-        <v>121</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H39"/>
       <c r="I39" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="240">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
         <v>12</v>
@@ -2051,45 +2036,45 @@
         <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="45">
       <c r="A41" s="9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F41" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2100,10 +2085,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L2:L9"/>
+      <selection activeCell="L7" sqref="L2:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2160,71 +2145,71 @@
     </row>
     <row r="2" spans="1:12" ht="47.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3"/>
       <c r="I3" s="9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -2234,140 +2219,85 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F5"/>
       <c r="J5" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" s="9" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>96</v>
+        <v>20</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="45">
-      <c r="A8" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="90">
-      <c r="A9" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unused profile test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vanilla-Profile" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="174">
   <si>
     <t>GET</t>
   </si>
@@ -125,9 +125,6 @@
     <t>/users/user/(SYS_USER2)/media/image</t>
   </si>
   <si>
-    <t>/users/user/(SYS_USER2)a/raw/image</t>
-  </si>
-  <si>
     <t>{}</t>
   </si>
   <si>
@@ -161,9 +158,6 @@
     <t>Verify that user is able to update his own profile picture</t>
   </si>
   <si>
-    <t>Verify that for the invalid user id, raw image is not returned and check the error status</t>
-  </si>
-  <si>
     <t>Verify that for the given user id, media image is directly returned using API</t>
   </si>
   <si>
@@ -272,9 +266,6 @@
     <t>OPQA-695</t>
   </si>
   <si>
-    <t>OPQA-697</t>
-  </si>
-  <si>
     <t>OPQA-711</t>
   </si>
   <si>
@@ -356,12 +347,6 @@
     <t>Verify that for the given inactive user id, user image is not returned and check the error status using Vanilla API</t>
   </si>
   <si>
-    <t>Verify that for the given inactive user id, user raw image is not returned and check the error status using Vanilla API</t>
-  </si>
-  <si>
-    <t>/users/user/(SYS_USER1)/raw/image</t>
-  </si>
-  <si>
     <t>/users/user/(SYS_USER1)/media</t>
   </si>
   <si>
@@ -444,9 +429,6 @@
   </si>
   <si>
     <t>OPQA-2581</t>
-  </si>
-  <si>
-    <t>OPQA-2582</t>
   </si>
   <si>
     <t>OPQA-2583</t>
@@ -989,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L41"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1051,10 +1033,10 @@
     </row>
     <row r="2" spans="1:12" ht="225">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>12</v>
@@ -1069,18 +1051,18 @@
         <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1096,16 +1078,16 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1121,20 +1103,20 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="31.5">
       <c r="A5" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1149,19 +1131,19 @@
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
       <c r="I5" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1177,20 +1159,20 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="31.5">
       <c r="A7" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -1206,16 +1188,16 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="31.5">
       <c r="A8" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1231,16 +1213,16 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="31.5">
       <c r="A9" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -1255,18 +1237,18 @@
         <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="31.5">
       <c r="A10" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1281,18 +1263,18 @@
         <v>20</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="19" customFormat="1" ht="31.5">
       <c r="A11" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>12</v>
@@ -1319,10 +1301,10 @@
     </row>
     <row r="12" spans="1:12" ht="180">
       <c r="A12" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1343,10 +1325,10 @@
     </row>
     <row r="13" spans="1:12" ht="180">
       <c r="A13" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1362,15 +1344,15 @@
       </c>
       <c r="H13"/>
       <c r="J13" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5">
       <c r="A14" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1386,15 +1368,15 @@
       </c>
       <c r="H14"/>
       <c r="J14" s="5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45">
       <c r="A15" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1414,16 +1396,16 @@
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="7" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1438,18 +1420,18 @@
         <v>30</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="210">
       <c r="A17" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1462,15 +1444,15 @@
       </c>
       <c r="H17" s="8"/>
       <c r="J17" s="7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="255">
       <c r="A18" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1485,18 +1467,18 @@
         <v>30</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="210">
       <c r="A19" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1509,15 +1491,15 @@
       </c>
       <c r="H19" s="8"/>
       <c r="J19" s="7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="240">
       <c r="A20" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -1532,18 +1514,18 @@
         <v>30</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="31.5">
       <c r="A21" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1561,15 +1543,15 @@
         <v>18</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="60">
       <c r="A22" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -1584,24 +1566,24 @@
         <v>30</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="31.5">
       <c r="A23" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
@@ -1609,15 +1591,15 @@
       <c r="G23" s="5"/>
       <c r="H23"/>
       <c r="J23" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75">
       <c r="A24" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -1632,22 +1614,22 @@
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
       <c r="J24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="31.5">
       <c r="A25" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>0</v>
@@ -1656,16 +1638,16 @@
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="31.5">
       <c r="A26" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -1684,275 +1666,275 @@
       </c>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="31.5">
+    <row r="27" spans="1:12" s="10" customFormat="1" ht="15.75">
       <c r="A27" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27"/>
+      <c r="H27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27"/>
+      <c r="J27" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K27"/>
+      <c r="L27"/>
+    </row>
+    <row r="28" spans="1:12" ht="45">
+      <c r="A28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:12" ht="30">
+      <c r="A29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" s="10" customFormat="1" ht="15.75">
-      <c r="A28" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G28"/>
-      <c r="H28" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28"/>
-      <c r="J28" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="K28"/>
-      <c r="L28"/>
-    </row>
-    <row r="29" spans="1:12" ht="45">
-      <c r="A29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I29" s="1"/>
+      <c r="H29"/>
       <c r="J29" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="K29" s="1"/>
+        <v>104</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="30">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
       </c>
       <c r="D30" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="J30" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H30"/>
-      <c r="J30" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="30">
+    </row>
+    <row r="31" spans="1:12" ht="45">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>100</v>
+        <v>117</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="31.5">
       <c r="A32" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>102</v>
+        <v>133</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" t="s">
-        <v>122</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>158</v>
+        <v>15</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="9" t="s">
+        <v>131</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="31.5">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="47.25">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="H33" s="4"/>
       <c r="I33" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>161</v>
+        <v>131</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="47.25">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H34" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I34" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>110</v>
+        <v>131</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="47.25">
       <c r="A35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H35"/>
       <c r="I35" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="47.25">
       <c r="A36" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H36"/>
       <c r="I36" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="47.25">
       <c r="A37" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
@@ -1965,116 +1947,68 @@
       </c>
       <c r="H37"/>
       <c r="I37" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="47.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="240">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H38"/>
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="I38" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="47.25">
-      <c r="A39" t="s">
-        <v>145</v>
-      </c>
-      <c r="B39" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="45">
+      <c r="A39" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
         <v>117</v>
       </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H39"/>
+      <c r="H39" s="5" t="s">
+        <v>151</v>
+      </c>
       <c r="I39" s="9" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="240">
-      <c r="A40" t="s">
-        <v>146</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C40" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="45">
-      <c r="A41" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B41" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C41" t="s">
-        <v>12</v>
-      </c>
-      <c r="D41" t="s">
-        <v>103</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" t="s">
-        <v>122</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="I41" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2087,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L2:L7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2145,71 +2079,71 @@
     </row>
     <row r="2" spans="1:12" ht="47.25">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3"/>
       <c r="I3" s="9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -2219,70 +2153,70 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F5"/>
       <c r="J5" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="9" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>11</v>
@@ -2291,13 +2225,13 @@
         <v>20</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unused Profile API: /users/user/{TRUID}/image also removed Jira test cases OPQA-502, OPQA-691, OPQA-2581 and added new one:OPQA-2957
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="171">
   <si>
     <t>GET</t>
   </si>
@@ -128,9 +128,6 @@
     <t>{}</t>
   </si>
   <si>
-    <t>/users/user/(SYS_USER2)a/image</t>
-  </si>
-  <si>
     <t>/users/user/(SYS_USER1)a/media</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>Verify that user is able to view his own profile</t>
   </si>
   <si>
-    <t>Verify that user is able to get user image</t>
-  </si>
-  <si>
     <t>Verify that user is able to update his own profile picture</t>
   </si>
   <si>
@@ -170,9 +164,6 @@
     <t>Verify that for the missing truids, bulk profiles data is not returned and validating error status</t>
   </si>
   <si>
-    <t>Verify that for the invalid truids, User Image is not returned and validating error status</t>
-  </si>
-  <si>
     <t>Verify that for the invalid user id, media info is not returned and check media error status</t>
   </si>
   <si>
@@ -245,18 +236,12 @@
     <t>OPQA-500</t>
   </si>
   <si>
-    <t>OPQA-502</t>
-  </si>
-  <si>
     <t>OPQA-503</t>
   </si>
   <si>
     <t>OPQA-505</t>
   </si>
   <si>
-    <t>OPQA-691</t>
-  </si>
-  <si>
     <t>OPQA-693</t>
   </si>
   <si>
@@ -269,9 +254,6 @@
     <t>OPQA-711</t>
   </si>
   <si>
-    <t>OPQA-502_1</t>
-  </si>
-  <si>
     <t>OPQA-500_1</t>
   </si>
   <si>
@@ -344,9 +326,6 @@
     <t>Verify that inactive user is not able to edit  info like title,role,Institution and country using Vanilla API &amp; check the error status.</t>
   </si>
   <si>
-    <t>Verify that for the given inactive user id, user image is not returned and check the error status using Vanilla API</t>
-  </si>
-  <si>
     <t>/users/user/(SYS_USER1)/media</t>
   </si>
   <si>
@@ -428,9 +407,6 @@
     <t>OPQA-2580</t>
   </si>
   <si>
-    <t>OPQA-2581</t>
-  </si>
-  <si>
     <t>OPQA-2583</t>
   </si>
   <si>
@@ -461,9 +437,6 @@
     <t>{"imageType": "png","imageHeight":97,"imageWidth":97,"imageContent":"data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg=="}</t>
   </si>
   <si>
-    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||title=Project Neon2||imageHeight=200||imageWidth=200||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADICAIAAAAiOjnJAAAdqUlEQVR4AezSQREAAAgDIPsHtI6m2GN3kIG5AKiPhViIBWIhFmKBWIiFWCAWYiEWiIVYiAViIRZisc/e2W3HURxxfB9hHmEfYR9hH2EfQY+wb7BAQvwleSXLGINxRAgmEMwROBBC+JBJbDAfiRPyTTjHEC4SckNyldx1fse1/E+7e6YzszvSWrjq1NFZ7Y5GPT2/raquru7ZC7dm/AwuvYHl8v4s7AwWymukJC4O1j9vh8vDsD3gJ69Dk9gxprxufzYH6wEVCJgPFnqhCk3y4liHhWdHoUk4gw7jzA7WgytnB7GWTNFTQw7gJ6/bn83BelDlx2NxADRhRTH4dDYH69spfzsIr0xAh5/hq9uNpogDtgb85HUPEdszo/LZaIlaRQsdrGNI1eZAGnar8O87Ye1CG2hJ3LBjxpaDtT9Z3DnpO9OwdqENSatop4N1nOT5cTgziJV3vFUri4P1041wenCPfjwPaxfakLSKdh4ncbD++3V4eqT7x2ve6XlY8PIk/HV/Da1ysNbP1u/2wo1Z4GdXeXcatu+mTD/bzwPwFaNvtep+pcrB+mQvvDUNr23wos+bBDqWPT97N3GQyM0ZPClI4tcabp4bB/TT/SUviiviunixBnGwXpqEk4Mg/X53t8LxMFQLlvKcOVjESYaUuTNsTywAoSadGIRfzrq1h6uIL4prPFJxsD6c0++pvtolEL49Dzt3J5V/XRfU/2oezlfhkiZwGuKkvYxmIWU6r0J7of35RXGlRycO1pWxbt6Sd/HqGKo099xZvjgIaC5xe753V9sL7c8viitdszhYaHu5NlkEUozvepQLwwBM0mfvxeK3e+HdWUA/L0DpYK1R3pxy21K9OukW0ODv3pv1PDT7x+1wtgo05tFBOD8M/Gryn6/DpVH47iBIr6WOm/bnF4V/dLCOUP51x+6flF91FxOA1lBzh0FCY/n5NAip7yxUxwjK/KK4UgfryNl6cYJhQHlRTxVZqMcpvuOA/hzKX/YDDg79yUbADrWU3aGQkuITc4MXX9R9SZUnSFX5aYmDL7tkMslOUYZwriK5kMbsZkvs3oNXSzlTpVQ9Qni34QnSNRsncy4yS22FwNyo2hp0cIiUTG1+k6k6NeDXezICogrFCMVNooXXZwH9zV5WUTiJkTLlsE7Rm3VCH2bMwcLXEOTGMe8Pxx3wIsCyqrrf73WbChRVKFYqBiumKgYLSkTMw4PwwiTFAqPFR9InR+2R4qqTwJ+ecbBWEHVorJtVb936hz2Wc5FqT3HcqRZUkVvi19gmCSk0huN0JaoW+qf9EMvXdwK+7wdjFKvGJSzefHkjnKoCxz8x0p9IOIzrzTuBnnGwuotsgNxHonxlVxdy7pbKeqzKnS9zNUzI1PidP++TOOBm491ivlOqUOgpC1QZUrEm/pErbeoEjuwuDlaxT3eHTXkpzE+3HKkisBXldIYI5qco2CodLAW1mFeutO9vl4P1zDjvTWlK1TMjlbIo3C4LyQijir/9/6bl1hwLUXLB2CfBYX7N5O+3w/OT8BATfxUkxWeQuUr1zkGQFHqA/nGwlhHSPC37lNgcnlTN8vpG+wqZUkGVyMAaCRcjg59QAivbw/D+XL57EUL9bLo4jL/lGKiSXhyJrRwpOwawWn273pg6WB1Fd1RjqEQVXqgESgVSK9b7Mp3HVAzKCxMi7jh4un33/afHMS6NXs9sVaKcwYSRo3iKFQMp0WAzV/rHweos8i95h2IS8gDrieGilGW7kitM62QYAxaFUN3SVJYlZ5yv2y8CsE/c+BQFOKsVmatYD2bBBMuUf4q1S4TrzTuBnllSHCyNwhjVW2+eGzZ2KGyRJb+hcVxKlRXJlPPvpKwElubyaIDAAhSoysHCMpmJBQtUvgzHVwALwdThTEtU6QvGtSsBRpMQB2v9osxCPvrDvIlFop+tysAinwlAMi2WUtc7uSvkI7BLA3AYeqjk6eT0OV6oEb1xfgF6v4qDpTFgbq7emVqGXQXmQGYlU+X8Pgja7UdBQQwJLM0DcpiQgjwCrHICouAZHawVRGMrjcIKwQTGBue1SkHVucrAYu1Dow+iMVACSeYWKTr4RV2TiL1EFWpDNhkkPgUpTqL8BdaI9yWpeSuODGgVPWP/iObRYw5W95yhBvkN6w7mFXgtvzQZqjgJiyBkirjlKAIKcRqdjwi88JKP1pWi86lu9ulK0JTNEiODcqSvkUH6XxLlnA5W2xyjNJ/Tfc3WHSxT7Z4C+tEcPyhDorvLrTITogbgHAWWGS1W0WDwoFN3HeNBKpXz2NlIjqOUcMWGTcSkMz96P9PCF684g+RgFTLR0jjmhaRk2YKMljKfJBe6TtQkzkjxuIJxHBxsMQEMQwj/+hT2Kcv1azZGIAKlon5RJV9WBmt7KO4L/UPvOVgN6dBCryVTb/hBIWVK0B3boQuVVWJpFbw+ovov35gvNyeoPKOYTsXc8d6ovjrZqJKFi8F6OAVLH+UqN0dLOL7td8/BattruBgJzkVIoQTUsTD6U30ftaB53oH32XlBYmMFG7Ip8wRkLasCNa20de8OpWcqowqVQcVXNpYzJPM/GkgCd/a3xUlGB0tS9gXJDJrYujqhONiMQWqWqIThNm9mFgsXaR/p/c8joLEZdoOX+OoTafHvoJn/Hhfo0cIP5kkoKaevbILYog1x3lVUKVNfUneF5eFSKc5oH5UzuyxzUnbBmgrkRi4t/K8XxuFg2t5Cl5JkDZ8qTV/ymA5WKhqUlc1V70JIjgnZGR7itC6gd0y54ZcB3VLw9EzZaNlck4NVZEu+QLZKVCk53nFhRaGWXIWgfW5Ww/iAjZDiBs/v1jrvVGJL15svQqQ9CvXEjaDnRWq36LEyVQ6W+o4xIF9Z9Wb9ys9Lo/Z4cb/TKZ3z36z1g60ehUJWIi3mvCXYqpOLxAQOOq+9VgqjlILHpuZdhK5qZX2uMKFKNcot5WKVVjectfnmvsHCJlEhzdRkbLEMrHMVr2WrRJVdkWL81CCtOuhzsPjKKrAgFOV1IkIqVubv8k0+357WbC9zeYjdStc0axX1oQo8keIXVUp01ea6xFMxm0D/2EQ4PUZypNmhex4rj9wJNTD15QJwRu+6eUaVTf99ur/mjSq/bI7WZbFEFSqLpdnARJvCLMVhnsfKgyp1UCFDmK9SR2WxCF+MqlZblmHSnhsf4naMT/L4E+0Z0VzUL6qeiibaiZxyqpSg5zB9A3MVfA6WZjPKGRpN1ZXWE++p5EHRTEPOyRA8MThEsLYIyUfJ/5UN08gUj6xRYWHNj7BTtq9YCuFglc2VjJYEtqLid7o7r1bQQtPSCJE4GrAeHx5iUHXz3kWO/Apqj1W82TLzwrARwhIHV+goGS0Hq5D0K5Xz8hVvG6tq4pk7ynRefOM/VjR9JEJefkt19z1/CVdPJjtY3YUbaRPP3NojE7weKzs0I2nvsD3JGxudN3ADptiMOVjts+0dXCGG6tYcByEf0cpiEesAVmyxKJu5qRt/CGKp9jOq52leF/TqBnWLYJdapnPDWqdPb/T0JfTg/WCm7k6LARXXCzsG7SSEWG5aFpwjqJ2rDhGsk801gHLHJ74Zw25Hsz1che1dI9VODcrLe/C+0vRzsiZ9Z1gqyeWwyyNtXqU70bgjyNnDdI6YIsYQyqWVd6s/hUazPSRQYqSk6Uxiy6loryDN++tpuYDmSkBtv4GtElVaylyOvdYrGDNRdTpymtcbNq1AxBY9U04mO1gJXph6U3VTCay4wA0PKKrybYmxBzdkQg5ToHmzoiW447TA8EpWxExy5OKQR12w/UQ+2yO17eba95WDtULtcvxN1X4eMVVnopQ999X2CzkZBT1WqfzKpOet3pnStnw6NdPxWGFO2qx1SEfiV0iZkqZfVRws5jTsi6hFnppEawrtVf4gqlRLrm1FbbYnnsbZHhBpUYzQ/35xoEBZjsTYgu/um69iq6Aqn623LqKvHKySNE2valm6Pi3V46p0TjhKcDeAxbqa+KM/7oVrfVosjUxB4ZCyr/RGMtChT9wVFkTLVIrLzKMvK87x/rKypyrNFh/ef2kcD4otB6t9NouOqwVRy+EbP23Z3URauxUR9EqNt+DvkXsHDV81eEBys2Ro+bST0A/dMlgOFqao/UxF4hN5LZOmbfiakqhvTomsCVziUZvN+XR+przwpfHPT/LCKaYjbU1Yuj4WgnkfPZ/NSXMqHqayVVFIwzi309zXCrV+vmBV2dQCeao5Sf5WK121tZruxPUpE3nE+IuE+BftJrlBVgYVsi8SxlVaKqiKBsBi+Jk//9c+StNpz45tRGkas8VV+ILVzgIuLXqtWJCkvIN2QZLKTXyoJGpzBnWnsoquxi+AdmDLB6d5ChQny8RzMj6AYGzVWa2cjnJgQgplwueChpa+xL67FGZspDIhhUWb9WBpK0ezRngZPVciFw5QYsJ+xWlqn2bMks4px1Rekt9+1ZD2qjxhmoJFD5T6h95LxMEqlORqKXqrADbd4yAbVGrPPjIC2jFb20Bqm78fjdkxS9l8bUkaO1lMFDClE5r8/EhboS4lkCSqtHGXhH4obpriYLXfIiuNvjE/5WX4Oo9FPxBQKnjS+vpTNTO4xGSApQf42ObYcs3amy99YDgGDzSXnhGirpWToK/Jh5b3ptNMvINVjuLpO9wZ+sKEX8uFgW2dEZZJ2fyk0Dk2QrnAFnYrfsrX9eZ895WxVctQkHO4XUTPWBfRV+oiB6v/7DM+ov2OavJcgPVwBhY/7eSE/OBY3iqc2IuViVg+BUnbFWDlKbH8EdTrFweLO6eJGo0iMVFmhHgtr4TqsIKFM4ZUOag93EG21r3KSGCx6hcGFoIqbdk1x6zOls/zWSc4WL1FXXE5pTYwjsXyk/n0osxVef9F/sUti+Xrsv+2XdZD2VZp2rNPW6s1iaobmPO+Pa+vCiScenua0Kmr46rVA/TGyhGVg6UOTdYSJmxBQ2F6EbDKc0TlkYGZxnzXUN4XWNqrsswWdisXSsSs0A/dqXQeUaUHc0hXeJ60g6UhW53ylS2tiFJlqQKy8jZlBb8JsjpD/nAAYizbsw+Ts7TsT4wq8mcos0DlpwlJl3GLDpbWPdercpsJCskgvMEOqTacn3xkuQbBygltYxJMnUwjVqrVHu56qg+59ZbCs8oMKXRTS4nSij9/rNxRPghTYLXYnhp3BivRBnlAQ6SVpmELopFBm8X1hOoMA1uumT5XgRSqR3Ku/0GYbrEQGOr2sIbCJsSrb+dnVGlHkPY7pqISt1i9S2lNgfTdWXkuSLtodMvyE7jEGfDdoWUTqHiuGce9NCG9nq/OYHGsZRbYe+1QHzPrMdYKorrvWC/VQUPco3y95Q40UNdYUndCf5JQxeJjiahCteQm3lP0ZLxsK90ZizFgb2VqXG/eCdd8VLj6V3azijuUvm57SwClPJKCRVGlqNzMVUwVenVSv6foGS00bSfs103BzKWhyOu2sEJrK/oUz7x3EexWvp443W5U1Q16spJskqiyNNWb0/hTUYV2WHsDTFuL+j7qtJbJvGvK0sFac3I1D03ae2FRdbbSHVVWkzpmtNu2IoAFUhaBXZuUGELXIw4Wd/r80O49L6hBaBX2Ejm1FuIqPCC2qk87QQ00VF1ucIVcRXxR/F8H64ipwopgS2LlrpQGlfl6YqwCf/KBtl9btyRPnpKldLCOTqinU+9LL4/yTFU+khKa9lzxHMrVBWtEnTvaPvxCaH9+UVypg3WEQj3diUGu9XltPBpmKfnqPxXfRS2d6ElY8KNAqrXUXxFX6mAdnZCczO8B1eLtRUjpz/GM2Zb/6DKleYRQViRzZdS92t3BWqN8spffAzY6W/4uymKJqu3Kcgrpk5W0jpl01BbTi3WuiqcGs7HMxYq9IUJ7of35RXGlDtaRyltTspRSbFjnSFkrYdDk/t2YNZWyyNlpTpCIqkdLrCvSEh0Haw074vEtR3mx/G6OKC8kAisuZbk5a4yiUCL0dV2Ug7UGwZ29PWWeGErwZZ3vrkpZdqsadLBSFC+wjhmv10VoCe2hVSpEPibiYImqncrcmeKkzgUwGKr3Zj0aJNqQtOq4seVgUZap+6cHza1baEPaKtp5nMTBYhZPQZIp73irHKxV5fWN9Ba+s36LRRvSVr3uFut4CYHRrkXfFoArxlqn0IakVbTTwTqGbB1MyQuUFrYzuLt0d+0D2U7q9VYTzmBZU9XxNT0xmlbRNlHlYH3rxKhCjS2kvJ1VGQWjCjW2HlxxsCx1Lm2Sz/Z1DK/bnu3BFQeLJKdlz634rs1hJEXLc8+m/MmDKw4WEQ+VLRcqfpam/IBpe2Ba4o8zcB6OafVQAgfLhXkbgcVrFwerz6LQWzNZtW+L/I9dOhACAABgIOQPNbW/iRRDYiEWiIVYiAViIRZiIRaIhViIBWIhFmKBWIhVbTs75/3SyQ5F8f92baBYwIYigoL1a0OxY0exK7qCqDwsWMGCIPbeFUWsSN6BwGHInYTvQxf2yZwflnFy0yaf3HsTWX+Hp+npaVbc2NjQLxcWFpRFKNI2m5ubyqKnpyeYdXV11dXV1dTUtLe3o5fb21vr/8d5eBgbG0Ob+BfPyin0qwcwOzur/PT+/r66ujo4ONjc3FxdXd3Q0IABjIyMLC8vX1xc4OMoi05PTycmJlpbW3Wt7u7ulZUVtGb9u0xbW/yM6+vryk+Pj4/aYGZm5n8P1vPz86+wFRcXx4r5+fn6ZUpKirIIRdqmvLxcCb28vGAVo6OjZUeRkZFYsPv7eyXU2dlJs7KyMmXX9fV1VFQUjY+OjowdNTo6ihk55ltbW6uE0E5BQYGvfXx8PNr8/PxUQklJSTTDqM7Pz5XQ2tqa8Z3/swKw7u7uMjIy3N1hnQ4PD82/b9rW5rXZ3d1VFjU1NXktt7e3lUctLS2Orm3DhifjTrCpuLj47e3NqEiCafPDwcL2MkIhtinnD1cvQ+HXwYK3yM3NZS8xMTH19fXj4+MILvBhCQkJLEpMTESsdIBVWlpqc1dwezaw9vf3vd6xqqoKHwHhcmpqCtPs6elBdCsqKhoYGFAenZyceKlKTU1FBJ+cnERQrqys9HaH6m6woKWlpZ8MltT8/LxcDOpbwMISsousrCxAYIRIxDgadHR0OMCi03K7K2MuoIfvHTmioZKSEtZCTvbx8aE8Ojg4wDbQpRERETs7O26wkpOTX19fA7C+EywEAnqLs7MzJYQvzqQkNjaWS0iwHE6L7soB1tDQkMy93ELsBi66Sk5Ojm8ihayczTY2NvqC5R1Yb29vANa3gQVKmFNLJijEIw5jb29PgoUV4krTPdBd0UbOhXOky7y8vGSR44TLKkwJpNLS0rRNenq6L1iIm4yneGAWH4BlgoUU+x+LUCTBgjuRW1ZqcXGRZniWYIFa5Eb6ORQKGe6KYdSYCz0iwxYPobibcNwveKOnPFJQGBLb9AUL9PT19bEphFcJVgBWWCJYTIH5HodzZRG/MoQh+YKF7Io2dFp0V9nZ2bijknPhxRKCLEuZjw8PDyPqKaH+/n6a3dzcKCF52LSBhTMjOqIZTpp/F1gBWPixsLCQTstwV3Nzc2jEMRfwgRxcptWI1KDTuEWDc6WB4/6Ww3OAhR818ZwIUAvAMsHCZUHIIhT9abDwCwDvaAEES5Ffu8Hi5TtO/hUVFTrzo3B68B4sGL/cYOGCJhywIPRISzQegPXV5P3q6ortI74oixAg5I2ABAtZEUKefpOZmUl3hVsxlLrBkr9RwXi4GaC8vDyWYg/w/fHxsbLoX/bunzWOK4oC+BeWQJUqgRASSF0qgdKpFBiXbuzKqVwY7MaR0FdIo0adYPLDA4fNe7uXXU3IBuudwtirmdk3T2fun3PvHd/c3ERxqInFXh4cHCSKl0AMYi0iFrOfbI6uOHXoFYHHx8dNxIIvX740vuzo6Eh4vhOxAlYqOQck3uJYt5G+5JiRqWpigaLkqmiylFhDx7q8vIwbXVtI5sUUfPI0Y0lBLAcnFm4M4U7ECm5vb/sEUE26T+WCXtCXZhbEivLCyuYUZfhBrEXE4qfyFSonpPaGVWLqHKDa48OCWKAWlOND1lcTS425t1iwWoZibJqzBPsnJyc5QHheECu4v78varK7YRDLkxohcfYaGlf8JijXnz59Ojs7y49EIRK9glgJwFNhFD7n84JYJC6VPiVCIhkFiwarJmMBynw55fT0tCFBnDjgn9rijx8/vn379u7dO/63qTHXxAoUZwexlhIrEP8mlOkRJ5jnviYWIAexnhOMuaqJVXxvFM6+cerjx49+VIMTlwdsT6ynp6coaoNYi4gViZwk0f9iIm8yIRMUxCpRE6vufmF+ols20NCXkK7novjs+fl5CmpidbFBihm/ILFEqTo5xZ6CGw/TtAGfP392DEjfisxuPqZoiRQdO4yoI4JR3JUcMTxk8aLUM18zPS0FCE7zvXA3jeApvfcIkT39lKxwfn4uQrIGd60YlbAvaFw598eZcnnWfHV1pZLDmBWKvBbTeRkJ2pqw0ibMS/WnDPQXJNbA6HkfGBjEGhjEGhjEGhgYxBoYxJIAE8GVVq6vr6XTkmpVLXI59U9yTq3Rnlvk5BpR1PmdpUPXWUCX8k8FHOm03JuM2asS2nanDaB8zsfMbQtgAb9vjTS2z7UXbSoauRSMLWy+qVk1MMThlpsaM5GWsuAipHaHKQzMZ9Em3KOuB4JcMQ/88PBA4qfYXVxcUDRcgUihI15Lqp4fNYO3RSwKUKEfRsejZk0d1DfK81qdMDUcomuhtTbHpGS7DdLRRUbKmMYmWM8UZHmlRq8PTKW8n5Ymj9Xnths4iBXEzMQepCmqgLrbHoiVQeoSTNFOxEp9kJlf7e5KW30B1ca3SyyPo45yBRaPoDZzNQ2WXDk2Fb34taZBj4bOB/3VgULNRywklobBP/+Jw8PD/I6bHxn4ns9KVyC7pc1L91W/vKYmk+VxnUoC9sFNqXVyZGrnqxXPFBiaVmZfyjKpKTlXa40SpMnKDx8+mM71ydslljCiLm+pgeRzk8H5PK29BV5NrKIex5hNGxA/KNSbYPHy3GPKjgpT+VwkOn+o7aKZuK8wiOWx7qe4mhZeF9k3sepjlhMrHGrbbDLl4RtjLysMYmUQfhArjYE9sSSSq0GbEZKpxiBWBIXeFYZYiUy/roNoY+/Ecp2vG5DXkNTLS5AututdoRHnzEqAkFTkR8jI6wKmQSwPnxjTTglsPXkCWFOd2c2mbz3EqvPz/RKrBoVp7fJoB/bBDtgHuyGPoaWtNq2n3SUCmF3qNRqZqchsEKtCBq12Ihb8n4nlFl4hN5BAV1PdyGbUYL3XOSwGTAsX0ziItQbHx8cRqdcSS7fn+3VgEvZOLPHQ+w2gCOxELDYbewofh3CkDeWKxoApSzD2b5dYdlZB47efyBBEo57/K8G7okpNLJBt7St4JxzYB2Uf+5AJNvC+hmk7yHiM9yT2yujHCN4nHb2RbZTYPKbLicUI5Qne9MRn3MCvdr9ZYWqpQq6EjKlFbgMTQVxhe8sjK9RsXiSM3NyuxPLEJ/JYe4qQuR1G3Texwo8M4yfA2gaq0e3cxCCWgnwcoqBBfNoMWez0srzm1SuaKV5eXpqvi1CU1xW9mjTiwkz3LyRW89KivPG7QKx+XkCi5WEQqx+ran1TfhRd5491kKWnF2B2K0Lp1ZBOxw62ff/+3Vfn4Z6DMIZhCbGYljwSyudrlyfQ3pJY0jqBV97Du1pkVEzUIWMHiDX6gsxqu7I/hfkhd7u3g1jAtDStColPk/sUaGZBiUPF/Greipb5qlcTS+m3+IrUjLchVtrC+vfw5gGr4cptGXEQywHJboiE8V/zXotntydWLsg9JWppBFXjfsnMlxCLpcwrGHpECN2eWCwoK9hH8SKwYhPcpkW+RR1Lukf5FIlD/98oNP/rCcQLZMqZo6FjiUJwAvzl7u6OSuSyWmtETpsIjZe06duf0HspdqkpFRC+58XU7//wDHCyXJIlAVeuL8hfrE0bjG9vQkOzqfNlGaFNMVP2YfX1pGrPqhQ8oHSHrGBa1T6waj5hekfP+8B/ib/bpQMBAAAAACD/10ZoMFZj1ViN1Vg1VmM1Vo3VWI1VYzVWY9VYjdVYBQInF8S0j+DtAAAAAElFTkSuQmCC</t>
-  </si>
-  <si>
     <t>status=200||truid=(SYS_USER2)||mediaCategory=image-full</t>
   </si>
   <si>
@@ -479,9 +452,6 @@
     <t>{"active": false,"onboarded": true}</t>
   </si>
   <si>
-    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||title=Project Neon2||imageHeight=97||imageWidth=97||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg==</t>
-  </si>
-  <si>
     <t>status=404||statusCode=404||errorMessage=User not found.</t>
   </si>
   <si>
@@ -537,13 +507,34 @@
   </si>
   <si>
     <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA||interest=computers||title=Project Neon1</t>
+  </si>
+  <si>
+    <t>Verify that imageContent is returned for the truid using getUser API</t>
+  </si>
+  <si>
+    <t>?image=yes</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||imageHeight=0||imageWidth=0||imageType=png||imageId=00000000-0000-0000-0000-000000000000||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||imageHeight=0||imageWidth=0||imageType=png||imageId=00000000-0000-0000-0000-000000000000||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADICAIAAAAiOjnJAAAdqUlEQVR4AezSQREAAAgDIPsHtI6m2GN3kIG5AKiPhViIBWIhFmKBWIiFWCAWYiEWiIVYiAViIRZisc/e2W3HURxxfB9hHmEfYR9hH2EfQY+wb7BAQvwleSXLGINxRAgmEMwROBBC+JBJbDAfiRPyTTjHEC4SckNyldx1fse1/E+7e6YzszvSWrjq1NFZ7Y5GPT2/raquru7ZC7dm/AwuvYHl8v4s7AwWymukJC4O1j9vh8vDsD3gJ69Dk9gxprxufzYH6wEVCJgPFnqhCk3y4liHhWdHoUk4gw7jzA7WgytnB7GWTNFTQw7gJ6/bn83BelDlx2NxADRhRTH4dDYH69spfzsIr0xAh5/hq9uNpogDtgb85HUPEdszo/LZaIlaRQsdrGNI1eZAGnar8O87Ye1CG2hJ3LBjxpaDtT9Z3DnpO9OwdqENSatop4N1nOT5cTgziJV3vFUri4P1041wenCPfjwPaxfakLSKdh4ncbD++3V4eqT7x2ve6XlY8PIk/HV/Da1ysNbP1u/2wo1Z4GdXeXcatu+mTD/bzwPwFaNvtep+pcrB+mQvvDUNr23wos+bBDqWPT97N3GQyM0ZPClI4tcabp4bB/TT/SUviiviunixBnGwXpqEk4Mg/X53t8LxMFQLlvKcOVjESYaUuTNsTywAoSadGIRfzrq1h6uIL4prPFJxsD6c0++pvtolEL49Dzt3J5V/XRfU/2oezlfhkiZwGuKkvYxmIWU6r0J7of35RXGlRycO1pWxbt6Sd/HqGKo099xZvjgIaC5xe753V9sL7c8viitdszhYaHu5NlkEUozvepQLwwBM0mfvxeK3e+HdWUA/L0DpYK1R3pxy21K9OukW0ODv3pv1PDT7x+1wtgo05tFBOD8M/Gryn6/DpVH47iBIr6WOm/bnF4V/dLCOUP51x+6flF91FxOA1lBzh0FCY/n5NAip7yxUxwjK/KK4UgfryNl6cYJhQHlRTxVZqMcpvuOA/hzKX/YDDg79yUbADrWU3aGQkuITc4MXX9R9SZUnSFX5aYmDL7tkMslOUYZwriK5kMbsZkvs3oNXSzlTpVQ9Qni34QnSNRsncy4yS22FwNyo2hp0cIiUTG1+k6k6NeDXezICogrFCMVNooXXZwH9zV5WUTiJkTLlsE7Rm3VCH2bMwcLXEOTGMe8Pxx3wIsCyqrrf73WbChRVKFYqBiumKgYLSkTMw4PwwiTFAqPFR9InR+2R4qqTwJ+ecbBWEHVorJtVb936hz2Wc5FqT3HcqRZUkVvi19gmCSk0huN0JaoW+qf9EMvXdwK+7wdjFKvGJSzefHkjnKoCxz8x0p9IOIzrzTuBnnGwuotsgNxHonxlVxdy7pbKeqzKnS9zNUzI1PidP++TOOBm491ivlOqUOgpC1QZUrEm/pErbeoEjuwuDlaxT3eHTXkpzE+3HKkisBXldIYI5qco2CodLAW1mFeutO9vl4P1zDjvTWlK1TMjlbIo3C4LyQijir/9/6bl1hwLUXLB2CfBYX7N5O+3w/OT8BATfxUkxWeQuUr1zkGQFHqA/nGwlhHSPC37lNgcnlTN8vpG+wqZUkGVyMAaCRcjg59QAivbw/D+XL57EUL9bLo4jL/lGKiSXhyJrRwpOwawWn273pg6WB1Fd1RjqEQVXqgESgVSK9b7Mp3HVAzKCxMi7jh4un33/afHMS6NXs9sVaKcwYSRo3iKFQMp0WAzV/rHweos8i95h2IS8gDrieGilGW7kitM62QYAxaFUN3SVJYlZ5yv2y8CsE/c+BQFOKsVmatYD2bBBMuUf4q1S4TrzTuBnllSHCyNwhjVW2+eGzZ2KGyRJb+hcVxKlRXJlPPvpKwElubyaIDAAhSoysHCMpmJBQtUvgzHVwALwdThTEtU6QvGtSsBRpMQB2v9osxCPvrDvIlFop+tysAinwlAMi2WUtc7uSvkI7BLA3AYeqjk6eT0OV6oEb1xfgF6v4qDpTFgbq7emVqGXQXmQGYlU+X8Pgja7UdBQQwJLM0DcpiQgjwCrHICouAZHawVRGMrjcIKwQTGBue1SkHVucrAYu1Dow+iMVACSeYWKTr4RV2TiL1EFWpDNhkkPgUpTqL8BdaI9yWpeSuODGgVPWP/iObRYw5W95yhBvkN6w7mFXgtvzQZqjgJiyBkirjlKAIKcRqdjwi88JKP1pWi86lu9ulK0JTNEiODcqSvkUH6XxLlnA5W2xyjNJ/Tfc3WHSxT7Z4C+tEcPyhDorvLrTITogbgHAWWGS1W0WDwoFN3HeNBKpXz2NlIjqOUcMWGTcSkMz96P9PCF684g+RgFTLR0jjmhaRk2YKMljKfJBe6TtQkzkjxuIJxHBxsMQEMQwj/+hT2Kcv1azZGIAKlon5RJV9WBmt7KO4L/UPvOVgN6dBCryVTb/hBIWVK0B3boQuVVWJpFbw+ovov35gvNyeoPKOYTsXc8d6ovjrZqJKFi8F6OAVLH+UqN0dLOL7td8/BattruBgJzkVIoQTUsTD6U30ftaB53oH32XlBYmMFG7Ip8wRkLasCNa20de8OpWcqowqVQcVXNpYzJPM/GkgCd/a3xUlGB0tS9gXJDJrYujqhONiMQWqWqIThNm9mFgsXaR/p/c8joLEZdoOX+OoTafHvoJn/Hhfo0cIP5kkoKaevbILYog1x3lVUKVNfUneF5eFSKc5oH5UzuyxzUnbBmgrkRi4t/K8XxuFg2t5Cl5JkDZ8qTV/ymA5WKhqUlc1V70JIjgnZGR7itC6gd0y54ZcB3VLw9EzZaNlck4NVZEu+QLZKVCk53nFhRaGWXIWgfW5Ww/iAjZDiBs/v1jrvVGJL15svQqQ9CvXEjaDnRWq36LEyVQ6W+o4xIF9Z9Wb9ys9Lo/Z4cb/TKZ3z36z1g60ehUJWIi3mvCXYqpOLxAQOOq+9VgqjlILHpuZdhK5qZX2uMKFKNcot5WKVVjectfnmvsHCJlEhzdRkbLEMrHMVr2WrRJVdkWL81CCtOuhzsPjKKrAgFOV1IkIqVubv8k0+357WbC9zeYjdStc0axX1oQo8keIXVUp01ea6xFMxm0D/2EQ4PUZypNmhex4rj9wJNTD15QJwRu+6eUaVTf99ur/mjSq/bI7WZbFEFSqLpdnARJvCLMVhnsfKgyp1UCFDmK9SR2WxCF+MqlZblmHSnhsf4naMT/L4E+0Z0VzUL6qeiibaiZxyqpSg5zB9A3MVfA6WZjPKGRpN1ZXWE++p5EHRTEPOyRA8MThEsLYIyUfJ/5UN08gUj6xRYWHNj7BTtq9YCuFglc2VjJYEtqLid7o7r1bQQtPSCJE4GrAeHx5iUHXz3kWO/Apqj1W82TLzwrARwhIHV+goGS0Hq5D0K5Xz8hVvG6tq4pk7ynRefOM/VjR9JEJefkt19z1/CVdPJjtY3YUbaRPP3NojE7weKzs0I2nvsD3JGxudN3ADptiMOVjts+0dXCGG6tYcByEf0cpiEesAVmyxKJu5qRt/CGKp9jOq52leF/TqBnWLYJdapnPDWqdPb/T0JfTg/WCm7k6LARXXCzsG7SSEWG5aFpwjqJ2rDhGsk801gHLHJ74Zw25Hsz1che1dI9VODcrLe/C+0vRzsiZ9Z1gqyeWwyyNtXqU70bgjyNnDdI6YIsYQyqWVd6s/hUazPSRQYqSk6Uxiy6loryDN++tpuYDmSkBtv4GtElVaylyOvdYrGDNRdTpymtcbNq1AxBY9U04mO1gJXph6U3VTCay4wA0PKKrybYmxBzdkQg5ToHmzoiW447TA8EpWxExy5OKQR12w/UQ+2yO17eba95WDtULtcvxN1X4eMVVnopQ999X2CzkZBT1WqfzKpOet3pnStnw6NdPxWGFO2qx1SEfiV0iZkqZfVRws5jTsi6hFnppEawrtVf4gqlRLrm1FbbYnnsbZHhBpUYzQ/35xoEBZjsTYgu/um69iq6Aqn623LqKvHKySNE2valm6Pi3V46p0TjhKcDeAxbqa+KM/7oVrfVosjUxB4ZCyr/RGMtChT9wVFkTLVIrLzKMvK87x/rKypyrNFh/ef2kcD4otB6t9NouOqwVRy+EbP23Z3URauxUR9EqNt+DvkXsHDV81eEBys2Ro+bST0A/dMlgOFqao/UxF4hN5LZOmbfiakqhvTomsCVziUZvN+XR+przwpfHPT/LCKaYjbU1Yuj4WgnkfPZ/NSXMqHqayVVFIwzi309zXCrV+vmBV2dQCeao5Sf5WK121tZruxPUpE3nE+IuE+BftJrlBVgYVsi8SxlVaKqiKBsBi+Jk//9c+StNpz45tRGkas8VV+ILVzgIuLXqtWJCkvIN2QZLKTXyoJGpzBnWnsoquxi+AdmDLB6d5ChQny8RzMj6AYGzVWa2cjnJgQgplwueChpa+xL67FGZspDIhhUWb9WBpK0ezRngZPVciFw5QYsJ+xWlqn2bMks4px1Rekt9+1ZD2qjxhmoJFD5T6h95LxMEqlORqKXqrADbd4yAbVGrPPjIC2jFb20Bqm78fjdkxS9l8bUkaO1lMFDClE5r8/EhboS4lkCSqtHGXhH4obpriYLXfIiuNvjE/5WX4Oo9FPxBQKnjS+vpTNTO4xGSApQf42ObYcs3amy99YDgGDzSXnhGirpWToK/Jh5b3ptNMvINVjuLpO9wZ+sKEX8uFgW2dEZZJ2fyk0Dk2QrnAFnYrfsrX9eZ895WxVctQkHO4XUTPWBfRV+oiB6v/7DM+ov2OavJcgPVwBhY/7eSE/OBY3iqc2IuViVg+BUnbFWDlKbH8EdTrFweLO6eJGo0iMVFmhHgtr4TqsIKFM4ZUOag93EG21r3KSGCx6hcGFoIqbdk1x6zOls/zWSc4WL1FXXE5pTYwjsXyk/n0osxVef9F/sUti+Xrsv+2XdZD2VZp2rNPW6s1iaobmPO+Pa+vCiScenua0Kmr46rVA/TGyhGVg6UOTdYSJmxBQ2F6EbDKc0TlkYGZxnzXUN4XWNqrsswWdisXSsSs0A/dqXQeUaUHc0hXeJ60g6UhW53ylS2tiFJlqQKy8jZlBb8JsjpD/nAAYizbsw+Ts7TsT4wq8mcos0DlpwlJl3GLDpbWPdercpsJCskgvMEOqTacn3xkuQbBygltYxJMnUwjVqrVHu56qg+59ZbCs8oMKXRTS4nSij9/rNxRPghTYLXYnhp3BivRBnlAQ6SVpmELopFBm8X1hOoMA1uumT5XgRSqR3Ku/0GYbrEQGOr2sIbCJsSrb+dnVGlHkPY7pqISt1i9S2lNgfTdWXkuSLtodMvyE7jEGfDdoWUTqHiuGce9NCG9nq/OYHGsZRbYe+1QHzPrMdYKorrvWC/VQUPco3y95Q40UNdYUndCf5JQxeJjiahCteQm3lP0ZLxsK90ZizFgb2VqXG/eCdd8VLj6V3azijuUvm57SwClPJKCRVGlqNzMVUwVenVSv6foGS00bSfs103BzKWhyOu2sEJrK/oUz7x3EexWvp443W5U1Q16spJskqiyNNWb0/hTUYV2WHsDTFuL+j7qtJbJvGvK0sFac3I1D03ae2FRdbbSHVVWkzpmtNu2IoAFUhaBXZuUGELXIw4Wd/r80O49L6hBaBX2Ejm1FuIqPCC2qk87QQ00VF1ucIVcRXxR/F8H64ipwopgS2LlrpQGlfl6YqwCf/KBtl9btyRPnpKldLCOTqinU+9LL4/yTFU+khKa9lzxHMrVBWtEnTvaPvxCaH9+UVypg3WEQj3diUGu9XltPBpmKfnqPxXfRS2d6ElY8KNAqrXUXxFX6mAdnZCczO8B1eLtRUjpz/GM2Zb/6DKleYRQViRzZdS92t3BWqN8spffAzY6W/4uymKJqu3Kcgrpk5W0jpl01BbTi3WuiqcGs7HMxYq9IUJ7of35RXGlDtaRyltTspRSbFjnSFkrYdDk/t2YNZWyyNlpTpCIqkdLrCvSEh0Haw074vEtR3mx/G6OKC8kAisuZbk5a4yiUCL0dV2Ug7UGwZ29PWWeGErwZZ3vrkpZdqsadLBSFC+wjhmv10VoCe2hVSpEPibiYImqncrcmeKkzgUwGKr3Zj0aJNqQtOq4seVgUZap+6cHza1baEPaKtp5nMTBYhZPQZIp73irHKxV5fWN9Ba+s36LRRvSVr3uFut4CYHRrkXfFoArxlqn0IakVbTTwTqGbB1MyQuUFrYzuLt0d+0D2U7q9VYTzmBZU9XxNT0xmlbRNlHlYH3rxKhCjS2kvJ1VGQWjCjW2HlxxsCx1Lm2Sz/Z1DK/bnu3BFQeLJKdlz634rs1hJEXLc8+m/MmDKw4WEQ+VLRcqfpam/IBpe2Ba4o8zcB6OafVQAgfLhXkbgcVrFwerz6LQWzNZtW+L/I9dOhACAABgIOQPNbW/iRRDYiEWiIVYiAViIRZiIRaIhViIBWIhFmKBWIhVbTs75/3SyQ5F8f92baBYwIYigoL1a0OxY0exK7qCqDwsWMGCIPbeFUWsSN6BwGHInYTvQxf2yZwflnFy0yaf3HsTWX+Hp+npaVbc2NjQLxcWFpRFKNI2m5ubyqKnpyeYdXV11dXV1dTUtLe3o5fb21vr/8d5eBgbG0Ob+BfPyin0qwcwOzur/PT+/r66ujo4ONjc3FxdXd3Q0IABjIyMLC8vX1xc4OMoi05PTycmJlpbW3Wt7u7ulZUVtGb9u0xbW/yM6+vryk+Pj4/aYGZm5n8P1vPz86+wFRcXx4r5+fn6ZUpKirIIRdqmvLxcCb28vGAVo6OjZUeRkZFYsPv7eyXU2dlJs7KyMmXX9fV1VFQUjY+OjowdNTo6ihk55ltbW6uE0E5BQYGvfXx8PNr8/PxUQklJSTTDqM7Pz5XQ2tqa8Z3/swKw7u7uMjIy3N1hnQ4PD82/b9rW5rXZ3d1VFjU1NXktt7e3lUctLS2Orm3DhifjTrCpuLj47e3NqEiCafPDwcL2MkIhtinnD1cvQ+HXwYK3yM3NZS8xMTH19fXj4+MILvBhCQkJLEpMTESsdIBVWlpqc1dwezaw9vf3vd6xqqoKHwHhcmpqCtPs6elBdCsqKhoYGFAenZyceKlKTU1FBJ+cnERQrqys9HaH6m6woKWlpZ8MltT8/LxcDOpbwMISsousrCxAYIRIxDgadHR0OMCi03K7K2MuoIfvHTmioZKSEtZCTvbx8aE8Ojg4wDbQpRERETs7O26wkpOTX19fA7C+EywEAnqLs7MzJYQvzqQkNjaWS0iwHE6L7soB1tDQkMy93ELsBi66Sk5Ojm8ihayczTY2NvqC5R1Yb29vANa3gQVKmFNLJijEIw5jb29PgoUV4krTPdBd0UbOhXOky7y8vGSR44TLKkwJpNLS0rRNenq6L1iIm4yneGAWH4BlgoUU+x+LUCTBgjuRW1ZqcXGRZniWYIFa5Eb6ORQKGe6KYdSYCz0iwxYPobibcNwveKOnPFJQGBLb9AUL9PT19bEphFcJVgBWWCJYTIH5HodzZRG/MoQh+YKF7Io2dFp0V9nZ2bijknPhxRKCLEuZjw8PDyPqKaH+/n6a3dzcKCF52LSBhTMjOqIZTpp/F1gBWPixsLCQTstwV3Nzc2jEMRfwgRxcptWI1KDTuEWDc6WB4/6Ww3OAhR818ZwIUAvAMsHCZUHIIhT9abDwCwDvaAEES5Ffu8Hi5TtO/hUVFTrzo3B68B4sGL/cYOGCJhywIPRISzQegPXV5P3q6ortI74oixAg5I2ABAtZEUKefpOZmUl3hVsxlLrBkr9RwXi4GaC8vDyWYg/w/fHxsbLoX/bunzWOK4oC+BeWQJUqgRASSF0qgdKpFBiXbuzKqVwY7MaR0FdIo0adYPLDA4fNe7uXXU3IBuudwtirmdk3T2fun3PvHd/c3ERxqInFXh4cHCSKl0AMYi0iFrOfbI6uOHXoFYHHx8dNxIIvX740vuzo6Eh4vhOxAlYqOQck3uJYt5G+5JiRqWpigaLkqmiylFhDx7q8vIwbXVtI5sUUfPI0Y0lBLAcnFm4M4U7ECm5vb/sEUE26T+WCXtCXZhbEivLCyuYUZfhBrEXE4qfyFSonpPaGVWLqHKDa48OCWKAWlOND1lcTS425t1iwWoZibJqzBPsnJyc5QHheECu4v78varK7YRDLkxohcfYaGlf8JijXnz59Ojs7y49EIRK9glgJwFNhFD7n84JYJC6VPiVCIhkFiwarJmMBynw55fT0tCFBnDjgn9rijx8/vn379u7dO/63qTHXxAoUZwexlhIrEP8mlOkRJ5jnviYWIAexnhOMuaqJVXxvFM6+cerjx49+VIMTlwdsT6ynp6coaoNYi4gViZwk0f9iIm8yIRMUxCpRE6vufmF+ols20NCXkK7novjs+fl5CmpidbFBihm/ILFEqTo5xZ6CGw/TtAGfP392DEjfisxuPqZoiRQdO4yoI4JR3JUcMTxk8aLUM18zPS0FCE7zvXA3jeApvfcIkT39lKxwfn4uQrIGd60YlbAvaFw598eZcnnWfHV1pZLDmBWKvBbTeRkJ2pqw0ibMS/WnDPQXJNbA6HkfGBjEGhjEGhjEGhgYxBoYxJIAE8GVVq6vr6XTkmpVLXI59U9yTq3Rnlvk5BpR1PmdpUPXWUCX8k8FHOm03JuM2asS2nanDaB8zsfMbQtgAb9vjTS2z7UXbSoauRSMLWy+qVk1MMThlpsaM5GWsuAipHaHKQzMZ9Em3KOuB4JcMQ/88PBA4qfYXVxcUDRcgUihI15Lqp4fNYO3RSwKUKEfRsejZk0d1DfK81qdMDUcomuhtTbHpGS7DdLRRUbKmMYmWM8UZHmlRq8PTKW8n5Ymj9Xnths4iBXEzMQepCmqgLrbHoiVQeoSTNFOxEp9kJlf7e5KW30B1ca3SyyPo45yBRaPoDZzNQ2WXDk2Fb34taZBj4bOB/3VgULNRywklobBP/+Jw8PD/I6bHxn4ns9KVyC7pc1L91W/vKYmk+VxnUoC9sFNqXVyZGrnqxXPFBiaVmZfyjKpKTlXa40SpMnKDx8+mM71ydslljCiLm+pgeRzk8H5PK29BV5NrKIex5hNGxA/KNSbYPHy3GPKjgpT+VwkOn+o7aKZuK8wiOWx7qe4mhZeF9k3sepjlhMrHGrbbDLl4RtjLysMYmUQfhArjYE9sSSSq0GbEZKpxiBWBIXeFYZYiUy/roNoY+/Ecp2vG5DXkNTLS5AututdoRHnzEqAkFTkR8jI6wKmQSwPnxjTTglsPXkCWFOd2c2mbz3EqvPz/RKrBoVp7fJoB/bBDtgHuyGPoaWtNq2n3SUCmF3qNRqZqchsEKtCBq12Ihb8n4nlFl4hN5BAV1PdyGbUYL3XOSwGTAsX0ziItQbHx8cRqdcSS7fn+3VgEvZOLPHQ+w2gCOxELDYbewofh3CkDeWKxoApSzD2b5dYdlZB47efyBBEo57/K8G7okpNLJBt7St4JxzYB2Uf+5AJNvC+hmk7yHiM9yT2yujHCN4nHb2RbZTYPKbLicUI5Qne9MRn3MCvdr9ZYWqpQq6EjKlFbgMTQVxhe8sjK9RsXiSM3NyuxPLEJ/JYe4qQuR1G3Texwo8M4yfA2gaq0e3cxCCWgnwcoqBBfNoMWez0srzm1SuaKV5eXpqvi1CU1xW9mjTiwkz3LyRW89KivPG7QKx+XkCi5WEQqx+ran1TfhRd5491kKWnF2B2K0Lp1ZBOxw62ff/+3Vfn4Z6DMIZhCbGYljwSyudrlyfQ3pJY0jqBV97Du1pkVEzUIWMHiDX6gsxqu7I/hfkhd7u3g1jAtDStColPk/sUaGZBiUPF/Greipb5qlcTS+m3+IrUjLchVtrC+vfw5gGr4cptGXEQywHJboiE8V/zXotntydWLsg9JWppBFXjfsnMlxCLpcwrGHpECN2eWCwoK9hH8SKwYhPcpkW+RR1Lukf5FIlD/98oNP/rCcQLZMqZo6FjiUJwAvzl7u6OSuSyWmtETpsIjZe06duf0HspdqkpFRC+58XU7//wDHCyXJIlAVeuL8hfrE0bjG9vQkOzqfNlGaFNMVP2YfX1pGrPqhQ8oHSHrGBa1T6waj5hekfP+8B/ib/bpQMBAAAAACD/10ZoMFZj1ViN1Vg1VmM1Vo3VWI1VYzVWY9VYjdVYBQInF8S0j+DtAAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>OPQA-2957</t>
+  </si>
+  <si>
+    <t>OPQA-2957_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,6 +575,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -648,7 +645,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -677,6 +673,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1033,36 +1030,36 @@
     </row>
     <row r="2" spans="1:12" ht="225">
       <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30">
-      <c r="A3" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>44</v>
+      <c r="A3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1078,16 +1075,16 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="31.5">
-      <c r="A4" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>164</v>
+      <c r="A4" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>154</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1095,7 +1092,7 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
@@ -1103,20 +1100,20 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="7" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="31.5">
-      <c r="A5" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>54</v>
+      <c r="A5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1130,20 +1127,20 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="9" t="s">
-        <v>163</v>
+      <c r="I5" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="45">
-      <c r="A6" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>164</v>
+      <c r="A6" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>154</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1151,7 +1148,7 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F6" t="s">
@@ -1159,20 +1156,20 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="4" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="31.5">
-      <c r="A7" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>39</v>
+      <c r="A7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -1188,16 +1185,16 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="31.5">
-      <c r="A8" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>40</v>
+      <c r="A8" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1213,16 +1210,16 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="31.5">
-      <c r="A9" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>64</v>
+      <c r="A9" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -1237,18 +1234,18 @@
         <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="31.5">
-      <c r="A10" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>66</v>
+      <c r="A10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1263,48 +1260,48 @@
         <v>20</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="19" customFormat="1" ht="31.5">
-      <c r="A11" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="18" customFormat="1" ht="31.5">
+      <c r="A11" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>20</v>
       </c>
       <c r="G11"/>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="19" t="s">
         <v>21</v>
       </c>
       <c r="I11"/>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="19" t="s">
         <v>22</v>
       </c>
       <c r="K11"/>
       <c r="L11"/>
     </row>
     <row r="12" spans="1:12" ht="180">
-      <c r="A12" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>48</v>
+      <c r="A12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1324,11 +1321,11 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="180">
-      <c r="A13" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>49</v>
+      <c r="A13" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1344,15 +1341,15 @@
       </c>
       <c r="H13"/>
       <c r="J13" s="5" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5">
-      <c r="A14" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>50</v>
+      <c r="A14" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1368,15 +1365,15 @@
       </c>
       <c r="H14"/>
       <c r="J14" s="5" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45">
-      <c r="A15" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>90</v>
+      <c r="A15" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1396,16 +1393,16 @@
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="7" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="30">
-      <c r="A16" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>53</v>
+      <c r="A16" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1423,15 +1420,15 @@
         <v>36</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="210">
-      <c r="A17" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>45</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="255">
+      <c r="A17" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1440,45 +1437,51 @@
         <v>33</v>
       </c>
       <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="225.75">
+      <c r="A18" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>167</v>
+      </c>
+      <c r="E18" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="J17" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="255">
-      <c r="A18" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>147</v>
+      <c r="G18" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="210">
-      <c r="A19" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>45</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="240">
+      <c r="A19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1487,45 +1490,51 @@
         <v>33</v>
       </c>
       <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="225.75">
+      <c r="A20" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" t="s">
         <v>0</v>
       </c>
-      <c r="H19" s="8"/>
-      <c r="J19" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="240">
-      <c r="A20" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>42</v>
+      <c r="G20" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="31.5">
-      <c r="A21" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>55</v>
+      <c r="A21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1543,15 +1552,15 @@
         <v>18</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="60">
-      <c r="A22" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>56</v>
+      <c r="A22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -1566,46 +1575,48 @@
         <v>30</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="31.5">
-      <c r="A23" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>51</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75">
+      <c r="A23" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" ht="31.5">
+      <c r="A24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
         <v>37</v>
-      </c>
-      <c r="E23" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23"/>
-      <c r="J23" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75">
-      <c r="A24" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" t="s">
-        <v>34</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>0</v>
@@ -1614,22 +1625,22 @@
       <c r="H24" s="6"/>
       <c r="I24" s="1"/>
       <c r="J24" s="4" t="s">
-        <v>43</v>
+        <v>150</v>
       </c>
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="31.5">
-      <c r="A25" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>52</v>
+      <c r="A25" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>0</v>
@@ -1638,377 +1649,329 @@
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="4" t="s">
-        <v>160</v>
+        <v>19</v>
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="31.5">
-      <c r="A26" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="1" t="s">
+    <row r="26" spans="1:12" s="9" customFormat="1" ht="15.75">
+      <c r="A26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26"/>
+      <c r="H26" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26"/>
+      <c r="J26" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K26"/>
+      <c r="L26"/>
+    </row>
+    <row r="27" spans="1:12" ht="45">
+      <c r="A27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" ht="30">
+      <c r="A28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:12" s="10" customFormat="1" ht="15.75">
-      <c r="A27" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27"/>
-      <c r="H27" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27"/>
-      <c r="J27" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="K27"/>
-      <c r="L27"/>
-    </row>
-    <row r="28" spans="1:12" ht="45">
-      <c r="A28" t="s">
-        <v>128</v>
-      </c>
-      <c r="B28" s="12" t="s">
+      <c r="H28"/>
+      <c r="J28" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" t="s">
-        <v>95</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I28" s="1"/>
-      <c r="J28" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:12" ht="30">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="45">
+      <c r="A30" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>110</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="31.5">
+      <c r="A31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H29"/>
-      <c r="J29" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="30">
-      <c r="A30" t="s">
-        <v>130</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="45">
-      <c r="A31" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" t="s">
-        <v>100</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" t="s">
-        <v>117</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>152</v>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="31.5">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="47.25">
       <c r="A32" t="s">
-        <v>133</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>105</v>
+        <v>128</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>127</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="G32" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="H32" s="4"/>
-      <c r="I32" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>155</v>
+      <c r="I32" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="47.25">
       <c r="A33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>134</v>
+        <v>129</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H33" s="4"/>
-      <c r="I33" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>107</v>
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="47.25">
       <c r="A34" t="s">
-        <v>136</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>108</v>
+        <v>130</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I34" s="9" t="s">
-        <v>131</v>
+        <v>103</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34"/>
+      <c r="I34" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="47.25">
       <c r="A35" t="s">
-        <v>137</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>109</v>
+        <v>131</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="D35" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35"/>
+      <c r="I35" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="240">
+      <c r="A36" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
         <v>16</v>
       </c>
-      <c r="E35" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35"/>
-      <c r="I35" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="47.25">
-      <c r="A36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="45">
+      <c r="A37" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H36"/>
-      <c r="I36" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="47.25">
-      <c r="A37" t="s">
-        <v>139</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" t="s">
-        <v>114</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H37"/>
-      <c r="I37" s="9" t="s">
-        <v>131</v>
+      <c r="H37" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="240">
-      <c r="A38" t="s">
-        <v>140</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="45">
-      <c r="A39" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s">
-        <v>100</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" t="s">
-        <v>117</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2022,7 +1985,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L7" sqref="L2:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2079,71 +2042,71 @@
     </row>
     <row r="2" spans="1:12" ht="47.25">
       <c r="A2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>115</v>
+        <v>133</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>132</v>
+        <v>85</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3"/>
-      <c r="I3" s="9" t="s">
-        <v>132</v>
+      <c r="I3" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>120</v>
+        <v>135</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>113</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -2153,85 +2116,85 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F5"/>
       <c r="J5" s="5" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
-      <c r="A6" s="9" t="s">
-        <v>145</v>
+      <c r="A6" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45">
+      <c r="A7" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="45">
-      <c r="A7" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>145</v>
+        <v>97</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed profile test cases -some test cases removed imageHeight, imageWidth, imageID from getUser API.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Vanilla-Profile" sheetId="1" r:id="rId1"/>
@@ -515,19 +515,19 @@
     <t>?image=yes</t>
   </si>
   <si>
-    <t>status=200||truid=(SYS_USER2)||imageHeight=0||imageWidth=0||imageType=png||imageId=00000000-0000-0000-0000-000000000000||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg==</t>
-  </si>
-  <si>
     <t>/users/user/(SYS_USER2)</t>
   </si>
   <si>
-    <t>status=200||truid=(SYS_USER2)||imageHeight=0||imageWidth=0||imageType=png||imageId=00000000-0000-0000-0000-000000000000||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADICAIAAAAiOjnJAAAdqUlEQVR4AezSQREAAAgDIPsHtI6m2GN3kIG5AKiPhViIBWIhFmKBWIiFWCAWYiEWiIVYiAViIRZisc/e2W3HURxxfB9hHmEfYR9hH2EfQY+wb7BAQvwleSXLGINxRAgmEMwROBBC+JBJbDAfiRPyTTjHEC4SckNyldx1fse1/E+7e6YzszvSWrjq1NFZ7Y5GPT2/raquru7ZC7dm/AwuvYHl8v4s7AwWymukJC4O1j9vh8vDsD3gJ69Dk9gxprxufzYH6wEVCJgPFnqhCk3y4liHhWdHoUk4gw7jzA7WgytnB7GWTNFTQw7gJ6/bn83BelDlx2NxADRhRTH4dDYH69spfzsIr0xAh5/hq9uNpogDtgb85HUPEdszo/LZaIlaRQsdrGNI1eZAGnar8O87Ye1CG2hJ3LBjxpaDtT9Z3DnpO9OwdqENSatop4N1nOT5cTgziJV3vFUri4P1041wenCPfjwPaxfakLSKdh4ncbD++3V4eqT7x2ve6XlY8PIk/HV/Da1ysNbP1u/2wo1Z4GdXeXcatu+mTD/bzwPwFaNvtep+pcrB+mQvvDUNr23wos+bBDqWPT97N3GQyM0ZPClI4tcabp4bB/TT/SUviiviunixBnGwXpqEk4Mg/X53t8LxMFQLlvKcOVjESYaUuTNsTywAoSadGIRfzrq1h6uIL4prPFJxsD6c0++pvtolEL49Dzt3J5V/XRfU/2oezlfhkiZwGuKkvYxmIWU6r0J7of35RXGlRycO1pWxbt6Sd/HqGKo099xZvjgIaC5xe753V9sL7c8viitdszhYaHu5NlkEUozvepQLwwBM0mfvxeK3e+HdWUA/L0DpYK1R3pxy21K9OukW0ODv3pv1PDT7x+1wtgo05tFBOD8M/Gryn6/DpVH47iBIr6WOm/bnF4V/dLCOUP51x+6flF91FxOA1lBzh0FCY/n5NAip7yxUxwjK/KK4UgfryNl6cYJhQHlRTxVZqMcpvuOA/hzKX/YDDg79yUbADrWU3aGQkuITc4MXX9R9SZUnSFX5aYmDL7tkMslOUYZwriK5kMbsZkvs3oNXSzlTpVQ9Qni34QnSNRsncy4yS22FwNyo2hp0cIiUTG1+k6k6NeDXezICogrFCMVNooXXZwH9zV5WUTiJkTLlsE7Rm3VCH2bMwcLXEOTGMe8Pxx3wIsCyqrrf73WbChRVKFYqBiumKgYLSkTMw4PwwiTFAqPFR9InR+2R4qqTwJ+ecbBWEHVorJtVb936hz2Wc5FqT3HcqRZUkVvi19gmCSk0huN0JaoW+qf9EMvXdwK+7wdjFKvGJSzefHkjnKoCxz8x0p9IOIzrzTuBnnGwuotsgNxHonxlVxdy7pbKeqzKnS9zNUzI1PidP++TOOBm491ivlOqUOgpC1QZUrEm/pErbeoEjuwuDlaxT3eHTXkpzE+3HKkisBXldIYI5qco2CodLAW1mFeutO9vl4P1zDjvTWlK1TMjlbIo3C4LyQijir/9/6bl1hwLUXLB2CfBYX7N5O+3w/OT8BATfxUkxWeQuUr1zkGQFHqA/nGwlhHSPC37lNgcnlTN8vpG+wqZUkGVyMAaCRcjg59QAivbw/D+XL57EUL9bLo4jL/lGKiSXhyJrRwpOwawWn273pg6WB1Fd1RjqEQVXqgESgVSK9b7Mp3HVAzKCxMi7jh4un33/afHMS6NXs9sVaKcwYSRo3iKFQMp0WAzV/rHweos8i95h2IS8gDrieGilGW7kitM62QYAxaFUN3SVJYlZ5yv2y8CsE/c+BQFOKsVmatYD2bBBMuUf4q1S4TrzTuBnllSHCyNwhjVW2+eGzZ2KGyRJb+hcVxKlRXJlPPvpKwElubyaIDAAhSoysHCMpmJBQtUvgzHVwALwdThTEtU6QvGtSsBRpMQB2v9osxCPvrDvIlFop+tysAinwlAMi2WUtc7uSvkI7BLA3AYeqjk6eT0OV6oEb1xfgF6v4qDpTFgbq7emVqGXQXmQGYlU+X8Pgja7UdBQQwJLM0DcpiQgjwCrHICouAZHawVRGMrjcIKwQTGBue1SkHVucrAYu1Dow+iMVACSeYWKTr4RV2TiL1EFWpDNhkkPgUpTqL8BdaI9yWpeSuODGgVPWP/iObRYw5W95yhBvkN6w7mFXgtvzQZqjgJiyBkirjlKAIKcRqdjwi88JKP1pWi86lu9ulK0JTNEiODcqSvkUH6XxLlnA5W2xyjNJ/Tfc3WHSxT7Z4C+tEcPyhDorvLrTITogbgHAWWGS1W0WDwoFN3HeNBKpXz2NlIjqOUcMWGTcSkMz96P9PCF684g+RgFTLR0jjmhaRk2YKMljKfJBe6TtQkzkjxuIJxHBxsMQEMQwj/+hT2Kcv1azZGIAKlon5RJV9WBmt7KO4L/UPvOVgN6dBCryVTb/hBIWVK0B3boQuVVWJpFbw+ovov35gvNyeoPKOYTsXc8d6ovjrZqJKFi8F6OAVLH+UqN0dLOL7td8/BattruBgJzkVIoQTUsTD6U30ftaB53oH32XlBYmMFG7Ip8wRkLasCNa20de8OpWcqowqVQcVXNpYzJPM/GkgCd/a3xUlGB0tS9gXJDJrYujqhONiMQWqWqIThNm9mFgsXaR/p/c8joLEZdoOX+OoTafHvoJn/Hhfo0cIP5kkoKaevbILYog1x3lVUKVNfUneF5eFSKc5oH5UzuyxzUnbBmgrkRi4t/K8XxuFg2t5Cl5JkDZ8qTV/ymA5WKhqUlc1V70JIjgnZGR7itC6gd0y54ZcB3VLw9EzZaNlck4NVZEu+QLZKVCk53nFhRaGWXIWgfW5Ww/iAjZDiBs/v1jrvVGJL15svQqQ9CvXEjaDnRWq36LEyVQ6W+o4xIF9Z9Wb9ys9Lo/Z4cb/TKZ3z36z1g60ehUJWIi3mvCXYqpOLxAQOOq+9VgqjlILHpuZdhK5qZX2uMKFKNcot5WKVVjectfnmvsHCJlEhzdRkbLEMrHMVr2WrRJVdkWL81CCtOuhzsPjKKrAgFOV1IkIqVubv8k0+357WbC9zeYjdStc0axX1oQo8keIXVUp01ea6xFMxm0D/2EQ4PUZypNmhex4rj9wJNTD15QJwRu+6eUaVTf99ur/mjSq/bI7WZbFEFSqLpdnARJvCLMVhnsfKgyp1UCFDmK9SR2WxCF+MqlZblmHSnhsf4naMT/L4E+0Z0VzUL6qeiibaiZxyqpSg5zB9A3MVfA6WZjPKGRpN1ZXWE++p5EHRTEPOyRA8MThEsLYIyUfJ/5UN08gUj6xRYWHNj7BTtq9YCuFglc2VjJYEtqLid7o7r1bQQtPSCJE4GrAeHx5iUHXz3kWO/Apqj1W82TLzwrARwhIHV+goGS0Hq5D0K5Xz8hVvG6tq4pk7ynRefOM/VjR9JEJefkt19z1/CVdPJjtY3YUbaRPP3NojE7weKzs0I2nvsD3JGxudN3ADptiMOVjts+0dXCGG6tYcByEf0cpiEesAVmyxKJu5qRt/CGKp9jOq52leF/TqBnWLYJdapnPDWqdPb/T0JfTg/WCm7k6LARXXCzsG7SSEWG5aFpwjqJ2rDhGsk801gHLHJ74Zw25Hsz1che1dI9VODcrLe/C+0vRzsiZ9Z1gqyeWwyyNtXqU70bgjyNnDdI6YIsYQyqWVd6s/hUazPSRQYqSk6Uxiy6loryDN++tpuYDmSkBtv4GtElVaylyOvdYrGDNRdTpymtcbNq1AxBY9U04mO1gJXph6U3VTCay4wA0PKKrybYmxBzdkQg5ToHmzoiW447TA8EpWxExy5OKQR12w/UQ+2yO17eba95WDtULtcvxN1X4eMVVnopQ999X2CzkZBT1WqfzKpOet3pnStnw6NdPxWGFO2qx1SEfiV0iZkqZfVRws5jTsi6hFnppEawrtVf4gqlRLrm1FbbYnnsbZHhBpUYzQ/35xoEBZjsTYgu/um69iq6Aqn623LqKvHKySNE2valm6Pi3V46p0TjhKcDeAxbqa+KM/7oVrfVosjUxB4ZCyr/RGMtChT9wVFkTLVIrLzKMvK87x/rKypyrNFh/ef2kcD4otB6t9NouOqwVRy+EbP23Z3URauxUR9EqNt+DvkXsHDV81eEBys2Ro+bST0A/dMlgOFqao/UxF4hN5LZOmbfiakqhvTomsCVziUZvN+XR+przwpfHPT/LCKaYjbU1Yuj4WgnkfPZ/NSXMqHqayVVFIwzi309zXCrV+vmBV2dQCeao5Sf5WK121tZruxPUpE3nE+IuE+BftJrlBVgYVsi8SxlVaKqiKBsBi+Jk//9c+StNpz45tRGkas8VV+ILVzgIuLXqtWJCkvIN2QZLKTXyoJGpzBnWnsoquxi+AdmDLB6d5ChQny8RzMj6AYGzVWa2cjnJgQgplwueChpa+xL67FGZspDIhhUWb9WBpK0ezRngZPVciFw5QYsJ+xWlqn2bMks4px1Rekt9+1ZD2qjxhmoJFD5T6h95LxMEqlORqKXqrADbd4yAbVGrPPjIC2jFb20Bqm78fjdkxS9l8bUkaO1lMFDClE5r8/EhboS4lkCSqtHGXhH4obpriYLXfIiuNvjE/5WX4Oo9FPxBQKnjS+vpTNTO4xGSApQf42ObYcs3amy99YDgGDzSXnhGirpWToK/Jh5b3ptNMvINVjuLpO9wZ+sKEX8uFgW2dEZZJ2fyk0Dk2QrnAFnYrfsrX9eZ895WxVctQkHO4XUTPWBfRV+oiB6v/7DM+ov2OavJcgPVwBhY/7eSE/OBY3iqc2IuViVg+BUnbFWDlKbH8EdTrFweLO6eJGo0iMVFmhHgtr4TqsIKFM4ZUOag93EG21r3KSGCx6hcGFoIqbdk1x6zOls/zWSc4WL1FXXE5pTYwjsXyk/n0osxVef9F/sUti+Xrsv+2XdZD2VZp2rNPW6s1iaobmPO+Pa+vCiScenua0Kmr46rVA/TGyhGVg6UOTdYSJmxBQ2F6EbDKc0TlkYGZxnzXUN4XWNqrsswWdisXSsSs0A/dqXQeUaUHc0hXeJ60g6UhW53ylS2tiFJlqQKy8jZlBb8JsjpD/nAAYizbsw+Ts7TsT4wq8mcos0DlpwlJl3GLDpbWPdercpsJCskgvMEOqTacn3xkuQbBygltYxJMnUwjVqrVHu56qg+59ZbCs8oMKXRTS4nSij9/rNxRPghTYLXYnhp3BivRBnlAQ6SVpmELopFBm8X1hOoMA1uumT5XgRSqR3Ku/0GYbrEQGOr2sIbCJsSrb+dnVGlHkPY7pqISt1i9S2lNgfTdWXkuSLtodMvyE7jEGfDdoWUTqHiuGce9NCG9nq/OYHGsZRbYe+1QHzPrMdYKorrvWC/VQUPco3y95Q40UNdYUndCf5JQxeJjiahCteQm3lP0ZLxsK90ZizFgb2VqXG/eCdd8VLj6V3azijuUvm57SwClPJKCRVGlqNzMVUwVenVSv6foGS00bSfs103BzKWhyOu2sEJrK/oUz7x3EexWvp443W5U1Q16spJskqiyNNWb0/hTUYV2WHsDTFuL+j7qtJbJvGvK0sFac3I1D03ae2FRdbbSHVVWkzpmtNu2IoAFUhaBXZuUGELXIw4Wd/r80O49L6hBaBX2Ejm1FuIqPCC2qk87QQ00VF1ucIVcRXxR/F8H64ipwopgS2LlrpQGlfl6YqwCf/KBtl9btyRPnpKldLCOTqinU+9LL4/yTFU+khKa9lzxHMrVBWtEnTvaPvxCaH9+UVypg3WEQj3diUGu9XltPBpmKfnqPxXfRS2d6ElY8KNAqrXUXxFX6mAdnZCczO8B1eLtRUjpz/GM2Zb/6DKleYRQViRzZdS92t3BWqN8spffAzY6W/4uymKJqu3Kcgrpk5W0jpl01BbTi3WuiqcGs7HMxYq9IUJ7of35RXGlDtaRyltTspRSbFjnSFkrYdDk/t2YNZWyyNlpTpCIqkdLrCvSEh0Haw074vEtR3mx/G6OKC8kAisuZbk5a4yiUCL0dV2Ug7UGwZ29PWWeGErwZZ3vrkpZdqsadLBSFC+wjhmv10VoCe2hVSpEPibiYImqncrcmeKkzgUwGKr3Zj0aJNqQtOq4seVgUZap+6cHza1baEPaKtp5nMTBYhZPQZIp73irHKxV5fWN9Ba+s36LRRvSVr3uFut4CYHRrkXfFoArxlqn0IakVbTTwTqGbB1MyQuUFrYzuLt0d+0D2U7q9VYTzmBZU9XxNT0xmlbRNlHlYH3rxKhCjS2kvJ1VGQWjCjW2HlxxsCx1Lm2Sz/Z1DK/bnu3BFQeLJKdlz634rs1hJEXLc8+m/MmDKw4WEQ+VLRcqfpam/IBpe2Ba4o8zcB6OafVQAgfLhXkbgcVrFwerz6LQWzNZtW+L/I9dOhACAABgIOQPNbW/iRRDYiEWiIVYiAViIRZiIRaIhViIBWIhFmKBWIhVbTs75/3SyQ5F8f92baBYwIYigoL1a0OxY0exK7qCqDwsWMGCIPbeFUWsSN6BwGHInYTvQxf2yZwflnFy0yaf3HsTWX+Hp+npaVbc2NjQLxcWFpRFKNI2m5ubyqKnpyeYdXV11dXV1dTUtLe3o5fb21vr/8d5eBgbG0Ob+BfPyin0qwcwOzur/PT+/r66ujo4ONjc3FxdXd3Q0IABjIyMLC8vX1xc4OMoi05PTycmJlpbW3Wt7u7ulZUVtGb9u0xbW/yM6+vryk+Pj4/aYGZm5n8P1vPz86+wFRcXx4r5+fn6ZUpKirIIRdqmvLxcCb28vGAVo6OjZUeRkZFYsPv7eyXU2dlJs7KyMmXX9fV1VFQUjY+OjowdNTo6ihk55ltbW6uE0E5BQYGvfXx8PNr8/PxUQklJSTTDqM7Pz5XQ2tqa8Z3/swKw7u7uMjIy3N1hnQ4PD82/b9rW5rXZ3d1VFjU1NXktt7e3lUctLS2Orm3DhifjTrCpuLj47e3NqEiCafPDwcL2MkIhtinnD1cvQ+HXwYK3yM3NZS8xMTH19fXj4+MILvBhCQkJLEpMTESsdIBVWlpqc1dwezaw9vf3vd6xqqoKHwHhcmpqCtPs6elBdCsqKhoYGFAenZyceKlKTU1FBJ+cnERQrqys9HaH6m6woKWlpZ8MltT8/LxcDOpbwMISsousrCxAYIRIxDgadHR0OMCi03K7K2MuoIfvHTmioZKSEtZCTvbx8aE8Ojg4wDbQpRERETs7O26wkpOTX19fA7C+EywEAnqLs7MzJYQvzqQkNjaWS0iwHE6L7soB1tDQkMy93ELsBi66Sk5Ojm8ihayczTY2NvqC5R1Yb29vANa3gQVKmFNLJijEIw5jb29PgoUV4krTPdBd0UbOhXOky7y8vGSR44TLKkwJpNLS0rRNenq6L1iIm4yneGAWH4BlgoUU+x+LUCTBgjuRW1ZqcXGRZniWYIFa5Eb6ORQKGe6KYdSYCz0iwxYPobibcNwveKOnPFJQGBLb9AUL9PT19bEphFcJVgBWWCJYTIH5HodzZRG/MoQh+YKF7Io2dFp0V9nZ2bijknPhxRKCLEuZjw8PDyPqKaH+/n6a3dzcKCF52LSBhTMjOqIZTpp/F1gBWPixsLCQTstwV3Nzc2jEMRfwgRxcptWI1KDTuEWDc6WB4/6Ww3OAhR818ZwIUAvAMsHCZUHIIhT9abDwCwDvaAEES5Ffu8Hi5TtO/hUVFTrzo3B68B4sGL/cYOGCJhywIPRISzQegPXV5P3q6ortI74oixAg5I2ABAtZEUKefpOZmUl3hVsxlLrBkr9RwXi4GaC8vDyWYg/w/fHxsbLoX/bunzWOK4oC+BeWQJUqgRASSF0qgdKpFBiXbuzKqVwY7MaR0FdIo0adYPLDA4fNe7uXXU3IBuudwtirmdk3T2fun3PvHd/c3ERxqInFXh4cHCSKl0AMYi0iFrOfbI6uOHXoFYHHx8dNxIIvX740vuzo6Eh4vhOxAlYqOQck3uJYt5G+5JiRqWpigaLkqmiylFhDx7q8vIwbXVtI5sUUfPI0Y0lBLAcnFm4M4U7ECm5vb/sEUE26T+WCXtCXZhbEivLCyuYUZfhBrEXE4qfyFSonpPaGVWLqHKDa48OCWKAWlOND1lcTS425t1iwWoZibJqzBPsnJyc5QHheECu4v78varK7YRDLkxohcfYaGlf8JijXnz59Ojs7y49EIRK9glgJwFNhFD7n84JYJC6VPiVCIhkFiwarJmMBynw55fT0tCFBnDjgn9rijx8/vn379u7dO/63qTHXxAoUZwexlhIrEP8mlOkRJ5jnviYWIAexnhOMuaqJVXxvFM6+cerjx49+VIMTlwdsT6ynp6coaoNYi4gViZwk0f9iIm8yIRMUxCpRE6vufmF+ols20NCXkK7novjs+fl5CmpidbFBihm/ILFEqTo5xZ6CGw/TtAGfP392DEjfisxuPqZoiRQdO4yoI4JR3JUcMTxk8aLUM18zPS0FCE7zvXA3jeApvfcIkT39lKxwfn4uQrIGd60YlbAvaFw598eZcnnWfHV1pZLDmBWKvBbTeRkJ2pqw0ibMS/WnDPQXJNbA6HkfGBjEGhjEGhjEGhgYxBoYxJIAE8GVVq6vr6XTkmpVLXI59U9yTq3Rnlvk5BpR1PmdpUPXWUCX8k8FHOm03JuM2asS2nanDaB8zsfMbQtgAb9vjTS2z7UXbSoauRSMLWy+qVk1MMThlpsaM5GWsuAipHaHKQzMZ9Em3KOuB4JcMQ/88PBA4qfYXVxcUDRcgUihI15Lqp4fNYO3RSwKUKEfRsejZk0d1DfK81qdMDUcomuhtTbHpGS7DdLRRUbKmMYmWM8UZHmlRq8PTKW8n5Ymj9Xnths4iBXEzMQepCmqgLrbHoiVQeoSTNFOxEp9kJlf7e5KW30B1ca3SyyPo45yBRaPoDZzNQ2WXDk2Fb34taZBj4bOB/3VgULNRywklobBP/+Jw8PD/I6bHxn4ns9KVyC7pc1L91W/vKYmk+VxnUoC9sFNqXVyZGrnqxXPFBiaVmZfyjKpKTlXa40SpMnKDx8+mM71ydslljCiLm+pgeRzk8H5PK29BV5NrKIex5hNGxA/KNSbYPHy3GPKjgpT+VwkOn+o7aKZuK8wiOWx7qe4mhZeF9k3sepjlhMrHGrbbDLl4RtjLysMYmUQfhArjYE9sSSSq0GbEZKpxiBWBIXeFYZYiUy/roNoY+/Ecp2vG5DXkNTLS5AututdoRHnzEqAkFTkR8jI6wKmQSwPnxjTTglsPXkCWFOd2c2mbz3EqvPz/RKrBoVp7fJoB/bBDtgHuyGPoaWtNq2n3SUCmF3qNRqZqchsEKtCBq12Ihb8n4nlFl4hN5BAV1PdyGbUYL3XOSwGTAsX0ziItQbHx8cRqdcSS7fn+3VgEvZOLPHQ+w2gCOxELDYbewofh3CkDeWKxoApSzD2b5dYdlZB47efyBBEo57/K8G7okpNLJBt7St4JxzYB2Uf+5AJNvC+hmk7yHiM9yT2yujHCN4nHb2RbZTYPKbLicUI5Qne9MRn3MCvdr9ZYWqpQq6EjKlFbgMTQVxhe8sjK9RsXiSM3NyuxPLEJ/JYe4qQuR1G3Texwo8M4yfA2gaq0e3cxCCWgnwcoqBBfNoMWez0srzm1SuaKV5eXpqvi1CU1xW9mjTiwkz3LyRW89KivPG7QKx+XkCi5WEQqx+ran1TfhRd5491kKWnF2B2K0Lp1ZBOxw62ff/+3Vfn4Z6DMIZhCbGYljwSyudrlyfQ3pJY0jqBV97Du1pkVEzUIWMHiDX6gsxqu7I/hfkhd7u3g1jAtDStColPk/sUaGZBiUPF/Greipb5qlcTS+m3+IrUjLchVtrC+vfw5gGr4cptGXEQywHJboiE8V/zXotntydWLsg9JWppBFXjfsnMlxCLpcwrGHpECN2eWCwoK9hH8SKwYhPcpkW+RR1Lukf5FIlD/98oNP/rCcQLZMqZo6FjiUJwAvzl7u6OSuSyWmtETpsIjZe06duf0HspdqkpFRC+58XU7//wDHCyXJIlAVeuL8hfrE0bjG9vQkOzqfNlGaFNMVP2YfX1pGrPqhQ8oHSHrGBa1T6waj5hekfP+8B/ib/bpQMBAAAAACD/10ZoMFZj1ViN1Vg1VmM1Vo3VWI1VYzVWY9VYjdVYBQInF8S0j+DtAAAAAElFTkSuQmCC</t>
-  </si>
-  <si>
     <t>OPQA-2957</t>
   </si>
   <si>
     <t>OPQA-2957_1</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADICAIAAAAiOjnJAAAdqUlEQVR4AezSQREAAAgDIPsHtI6m2GN3kIG5AKiPhViIBWIhFmKBWIiFWCAWYiEWiIVYiAViIRZisc/e2W3HURxxfB9hHmEfYR9hH2EfQY+wb7BAQvwleSXLGINxRAgmEMwROBBC+JBJbDAfiRPyTTjHEC4SckNyldx1fse1/E+7e6YzszvSWrjq1NFZ7Y5GPT2/raquru7ZC7dm/AwuvYHl8v4s7AwWymukJC4O1j9vh8vDsD3gJ69Dk9gxprxufzYH6wEVCJgPFnqhCk3y4liHhWdHoUk4gw7jzA7WgytnB7GWTNFTQw7gJ6/bn83BelDlx2NxADRhRTH4dDYH69spfzsIr0xAh5/hq9uNpogDtgb85HUPEdszo/LZaIlaRQsdrGNI1eZAGnar8O87Ye1CG2hJ3LBjxpaDtT9Z3DnpO9OwdqENSatop4N1nOT5cTgziJV3vFUri4P1041wenCPfjwPaxfakLSKdh4ncbD++3V4eqT7x2ve6XlY8PIk/HV/Da1ysNbP1u/2wo1Z4GdXeXcatu+mTD/bzwPwFaNvtep+pcrB+mQvvDUNr23wos+bBDqWPT97N3GQyM0ZPClI4tcabp4bB/TT/SUviiviunixBnGwXpqEk4Mg/X53t8LxMFQLlvKcOVjESYaUuTNsTywAoSadGIRfzrq1h6uIL4prPFJxsD6c0++pvtolEL49Dzt3J5V/XRfU/2oezlfhkiZwGuKkvYxmIWU6r0J7of35RXGlRycO1pWxbt6Sd/HqGKo099xZvjgIaC5xe753V9sL7c8viitdszhYaHu5NlkEUozvepQLwwBM0mfvxeK3e+HdWUA/L0DpYK1R3pxy21K9OukW0ODv3pv1PDT7x+1wtgo05tFBOD8M/Gryn6/DpVH47iBIr6WOm/bnF4V/dLCOUP51x+6flF91FxOA1lBzh0FCY/n5NAip7yxUxwjK/KK4UgfryNl6cYJhQHlRTxVZqMcpvuOA/hzKX/YDDg79yUbADrWU3aGQkuITc4MXX9R9SZUnSFX5aYmDL7tkMslOUYZwriK5kMbsZkvs3oNXSzlTpVQ9Qni34QnSNRsncy4yS22FwNyo2hp0cIiUTG1+k6k6NeDXezICogrFCMVNooXXZwH9zV5WUTiJkTLlsE7Rm3VCH2bMwcLXEOTGMe8Pxx3wIsCyqrrf73WbChRVKFYqBiumKgYLSkTMw4PwwiTFAqPFR9InR+2R4qqTwJ+ecbBWEHVorJtVb936hz2Wc5FqT3HcqRZUkVvi19gmCSk0huN0JaoW+qf9EMvXdwK+7wdjFKvGJSzefHkjnKoCxz8x0p9IOIzrzTuBnnGwuotsgNxHonxlVxdy7pbKeqzKnS9zNUzI1PidP++TOOBm491ivlOqUOgpC1QZUrEm/pErbeoEjuwuDlaxT3eHTXkpzE+3HKkisBXldIYI5qco2CodLAW1mFeutO9vl4P1zDjvTWlK1TMjlbIo3C4LyQijir/9/6bl1hwLUXLB2CfBYX7N5O+3w/OT8BATfxUkxWeQuUr1zkGQFHqA/nGwlhHSPC37lNgcnlTN8vpG+wqZUkGVyMAaCRcjg59QAivbw/D+XL57EUL9bLo4jL/lGKiSXhyJrRwpOwawWn273pg6WB1Fd1RjqEQVXqgESgVSK9b7Mp3HVAzKCxMi7jh4un33/afHMS6NXs9sVaKcwYSRo3iKFQMp0WAzV/rHweos8i95h2IS8gDrieGilGW7kitM62QYAxaFUN3SVJYlZ5yv2y8CsE/c+BQFOKsVmatYD2bBBMuUf4q1S4TrzTuBnllSHCyNwhjVW2+eGzZ2KGyRJb+hcVxKlRXJlPPvpKwElubyaIDAAhSoysHCMpmJBQtUvgzHVwALwdThTEtU6QvGtSsBRpMQB2v9osxCPvrDvIlFop+tysAinwlAMi2WUtc7uSvkI7BLA3AYeqjk6eT0OV6oEb1xfgF6v4qDpTFgbq7emVqGXQXmQGYlU+X8Pgja7UdBQQwJLM0DcpiQgjwCrHICouAZHawVRGMrjcIKwQTGBue1SkHVucrAYu1Dow+iMVACSeYWKTr4RV2TiL1EFWpDNhkkPgUpTqL8BdaI9yWpeSuODGgVPWP/iObRYw5W95yhBvkN6w7mFXgtvzQZqjgJiyBkirjlKAIKcRqdjwi88JKP1pWi86lu9ulK0JTNEiODcqSvkUH6XxLlnA5W2xyjNJ/Tfc3WHSxT7Z4C+tEcPyhDorvLrTITogbgHAWWGS1W0WDwoFN3HeNBKpXz2NlIjqOUcMWGTcSkMz96P9PCF684g+RgFTLR0jjmhaRk2YKMljKfJBe6TtQkzkjxuIJxHBxsMQEMQwj/+hT2Kcv1azZGIAKlon5RJV9WBmt7KO4L/UPvOVgN6dBCryVTb/hBIWVK0B3boQuVVWJpFbw+ovov35gvNyeoPKOYTsXc8d6ovjrZqJKFi8F6OAVLH+UqN0dLOL7td8/BattruBgJzkVIoQTUsTD6U30ftaB53oH32XlBYmMFG7Ip8wRkLasCNa20de8OpWcqowqVQcVXNpYzJPM/GkgCd/a3xUlGB0tS9gXJDJrYujqhONiMQWqWqIThNm9mFgsXaR/p/c8joLEZdoOX+OoTafHvoJn/Hhfo0cIP5kkoKaevbILYog1x3lVUKVNfUneF5eFSKc5oH5UzuyxzUnbBmgrkRi4t/K8XxuFg2t5Cl5JkDZ8qTV/ymA5WKhqUlc1V70JIjgnZGR7itC6gd0y54ZcB3VLw9EzZaNlck4NVZEu+QLZKVCk53nFhRaGWXIWgfW5Ww/iAjZDiBs/v1jrvVGJL15svQqQ9CvXEjaDnRWq36LEyVQ6W+o4xIF9Z9Wb9ys9Lo/Z4cb/TKZ3z36z1g60ehUJWIi3mvCXYqpOLxAQOOq+9VgqjlILHpuZdhK5qZX2uMKFKNcot5WKVVjectfnmvsHCJlEhzdRkbLEMrHMVr2WrRJVdkWL81CCtOuhzsPjKKrAgFOV1IkIqVubv8k0+357WbC9zeYjdStc0axX1oQo8keIXVUp01ea6xFMxm0D/2EQ4PUZypNmhex4rj9wJNTD15QJwRu+6eUaVTf99ur/mjSq/bI7WZbFEFSqLpdnARJvCLMVhnsfKgyp1UCFDmK9SR2WxCF+MqlZblmHSnhsf4naMT/L4E+0Z0VzUL6qeiibaiZxyqpSg5zB9A3MVfA6WZjPKGRpN1ZXWE++p5EHRTEPOyRA8MThEsLYIyUfJ/5UN08gUj6xRYWHNj7BTtq9YCuFglc2VjJYEtqLid7o7r1bQQtPSCJE4GrAeHx5iUHXz3kWO/Apqj1W82TLzwrARwhIHV+goGS0Hq5D0K5Xz8hVvG6tq4pk7ynRefOM/VjR9JEJefkt19z1/CVdPJjtY3YUbaRPP3NojE7weKzs0I2nvsD3JGxudN3ADptiMOVjts+0dXCGG6tYcByEf0cpiEesAVmyxKJu5qRt/CGKp9jOq52leF/TqBnWLYJdapnPDWqdPb/T0JfTg/WCm7k6LARXXCzsG7SSEWG5aFpwjqJ2rDhGsk801gHLHJ74Zw25Hsz1che1dI9VODcrLe/C+0vRzsiZ9Z1gqyeWwyyNtXqU70bgjyNnDdI6YIsYQyqWVd6s/hUazPSRQYqSk6Uxiy6loryDN++tpuYDmSkBtv4GtElVaylyOvdYrGDNRdTpymtcbNq1AxBY9U04mO1gJXph6U3VTCay4wA0PKKrybYmxBzdkQg5ToHmzoiW447TA8EpWxExy5OKQR12w/UQ+2yO17eba95WDtULtcvxN1X4eMVVnopQ999X2CzkZBT1WqfzKpOet3pnStnw6NdPxWGFO2qx1SEfiV0iZkqZfVRws5jTsi6hFnppEawrtVf4gqlRLrm1FbbYnnsbZHhBpUYzQ/35xoEBZjsTYgu/um69iq6Aqn623LqKvHKySNE2valm6Pi3V46p0TjhKcDeAxbqa+KM/7oVrfVosjUxB4ZCyr/RGMtChT9wVFkTLVIrLzKMvK87x/rKypyrNFh/ef2kcD4otB6t9NouOqwVRy+EbP23Z3URauxUR9EqNt+DvkXsHDV81eEBys2Ro+bST0A/dMlgOFqao/UxF4hN5LZOmbfiakqhvTomsCVziUZvN+XR+przwpfHPT/LCKaYjbU1Yuj4WgnkfPZ/NSXMqHqayVVFIwzi309zXCrV+vmBV2dQCeao5Sf5WK121tZruxPUpE3nE+IuE+BftJrlBVgYVsi8SxlVaKqiKBsBi+Jk//9c+StNpz45tRGkas8VV+ILVzgIuLXqtWJCkvIN2QZLKTXyoJGpzBnWnsoquxi+AdmDLB6d5ChQny8RzMj6AYGzVWa2cjnJgQgplwueChpa+xL67FGZspDIhhUWb9WBpK0ezRngZPVciFw5QYsJ+xWlqn2bMks4px1Rekt9+1ZD2qjxhmoJFD5T6h95LxMEqlORqKXqrADbd4yAbVGrPPjIC2jFb20Bqm78fjdkxS9l8bUkaO1lMFDClE5r8/EhboS4lkCSqtHGXhH4obpriYLXfIiuNvjE/5WX4Oo9FPxBQKnjS+vpTNTO4xGSApQf42ObYcs3amy99YDgGDzSXnhGirpWToK/Jh5b3ptNMvINVjuLpO9wZ+sKEX8uFgW2dEZZJ2fyk0Dk2QrnAFnYrfsrX9eZ895WxVctQkHO4XUTPWBfRV+oiB6v/7DM+ov2OavJcgPVwBhY/7eSE/OBY3iqc2IuViVg+BUnbFWDlKbH8EdTrFweLO6eJGo0iMVFmhHgtr4TqsIKFM4ZUOag93EG21r3KSGCx6hcGFoIqbdk1x6zOls/zWSc4WL1FXXE5pTYwjsXyk/n0osxVef9F/sUti+Xrsv+2XdZD2VZp2rNPW6s1iaobmPO+Pa+vCiScenua0Kmr46rVA/TGyhGVg6UOTdYSJmxBQ2F6EbDKc0TlkYGZxnzXUN4XWNqrsswWdisXSsSs0A/dqXQeUaUHc0hXeJ60g6UhW53ylS2tiFJlqQKy8jZlBb8JsjpD/nAAYizbsw+Ts7TsT4wq8mcos0DlpwlJl3GLDpbWPdercpsJCskgvMEOqTacn3xkuQbBygltYxJMnUwjVqrVHu56qg+59ZbCs8oMKXRTS4nSij9/rNxRPghTYLXYnhp3BivRBnlAQ6SVpmELopFBm8X1hOoMA1uumT5XgRSqR3Ku/0GYbrEQGOr2sIbCJsSrb+dnVGlHkPY7pqISt1i9S2lNgfTdWXkuSLtodMvyE7jEGfDdoWUTqHiuGce9NCG9nq/OYHGsZRbYe+1QHzPrMdYKorrvWC/VQUPco3y95Q40UNdYUndCf5JQxeJjiahCteQm3lP0ZLxsK90ZizFgb2VqXG/eCdd8VLj6V3azijuUvm57SwClPJKCRVGlqNzMVUwVenVSv6foGS00bSfs103BzKWhyOu2sEJrK/oUz7x3EexWvp443W5U1Q16spJskqiyNNWb0/hTUYV2WHsDTFuL+j7qtJbJvGvK0sFac3I1D03ae2FRdbbSHVVWkzpmtNu2IoAFUhaBXZuUGELXIw4Wd/r80O49L6hBaBX2Ejm1FuIqPCC2qk87QQ00VF1ucIVcRXxR/F8H64ipwopgS2LlrpQGlfl6YqwCf/KBtl9btyRPnpKldLCOTqinU+9LL4/yTFU+khKa9lzxHMrVBWtEnTvaPvxCaH9+UVypg3WEQj3diUGu9XltPBpmKfnqPxXfRS2d6ElY8KNAqrXUXxFX6mAdnZCczO8B1eLtRUjpz/GM2Zb/6DKleYRQViRzZdS92t3BWqN8spffAzY6W/4uymKJqu3Kcgrpk5W0jpl01BbTi3WuiqcGs7HMxYq9IUJ7of35RXGlDtaRyltTspRSbFjnSFkrYdDk/t2YNZWyyNlpTpCIqkdLrCvSEh0Haw074vEtR3mx/G6OKC8kAisuZbk5a4yiUCL0dV2Ug7UGwZ29PWWeGErwZZ3vrkpZdqsadLBSFC+wjhmv10VoCe2hVSpEPibiYImqncrcmeKkzgUwGKr3Zj0aJNqQtOq4seVgUZap+6cHza1baEPaKtp5nMTBYhZPQZIp73irHKxV5fWN9Ba+s36LRRvSVr3uFut4CYHRrkXfFoArxlqn0IakVbTTwTqGbB1MyQuUFrYzuLt0d+0D2U7q9VYTzmBZU9XxNT0xmlbRNlHlYH3rxKhCjS2kvJ1VGQWjCjW2HlxxsCx1Lm2Sz/Z1DK/bnu3BFQeLJKdlz634rs1hJEXLc8+m/MmDKw4WEQ+VLRcqfpam/IBpe2Ba4o8zcB6OafVQAgfLhXkbgcVrFwerz6LQWzNZtW+L/I9dOhACAABgIOQPNbW/iRRDYiEWiIVYiAViIRZiIRaIhViIBWIhFmKBWIhVbTs75/3SyQ5F8f92baBYwIYigoL1a0OxY0exK7qCqDwsWMGCIPbeFUWsSN6BwGHInYTvQxf2yZwflnFy0yaf3HsTWX+Hp+npaVbc2NjQLxcWFpRFKNI2m5ubyqKnpyeYdXV11dXV1dTUtLe3o5fb21vr/8d5eBgbG0Ob+BfPyin0qwcwOzur/PT+/r66ujo4ONjc3FxdXd3Q0IABjIyMLC8vX1xc4OMoi05PTycmJlpbW3Wt7u7ulZUVtGb9u0xbW/yM6+vryk+Pj4/aYGZm5n8P1vPz86+wFRcXx4r5+fn6ZUpKirIIRdqmvLxcCb28vGAVo6OjZUeRkZFYsPv7eyXU2dlJs7KyMmXX9fV1VFQUjY+OjowdNTo6ihk55ltbW6uE0E5BQYGvfXx8PNr8/PxUQklJSTTDqM7Pz5XQ2tqa8Z3/swKw7u7uMjIy3N1hnQ4PD82/b9rW5rXZ3d1VFjU1NXktt7e3lUctLS2Orm3DhifjTrCpuLj47e3NqEiCafPDwcL2MkIhtinnD1cvQ+HXwYK3yM3NZS8xMTH19fXj4+MILvBhCQkJLEpMTESsdIBVWlpqc1dwezaw9vf3vd6xqqoKHwHhcmpqCtPs6elBdCsqKhoYGFAenZyceKlKTU1FBJ+cnERQrqys9HaH6m6woKWlpZ8MltT8/LxcDOpbwMISsousrCxAYIRIxDgadHR0OMCi03K7K2MuoIfvHTmioZKSEtZCTvbx8aE8Ojg4wDbQpRERETs7O26wkpOTX19fA7C+EywEAnqLs7MzJYQvzqQkNjaWS0iwHE6L7soB1tDQkMy93ELsBi66Sk5Ojm8ihayczTY2NvqC5R1Yb29vANa3gQVKmFNLJijEIw5jb29PgoUV4krTPdBd0UbOhXOky7y8vGSR44TLKkwJpNLS0rRNenq6L1iIm4yneGAWH4BlgoUU+x+LUCTBgjuRW1ZqcXGRZniWYIFa5Eb6ORQKGe6KYdSYCz0iwxYPobibcNwveKOnPFJQGBLb9AUL9PT19bEphFcJVgBWWCJYTIH5HodzZRG/MoQh+YKF7Io2dFp0V9nZ2bijknPhxRKCLEuZjw8PDyPqKaH+/n6a3dzcKCF52LSBhTMjOqIZTpp/F1gBWPixsLCQTstwV3Nzc2jEMRfwgRxcptWI1KDTuEWDc6WB4/6Ww3OAhR818ZwIUAvAMsHCZUHIIhT9abDwCwDvaAEES5Ffu8Hi5TtO/hUVFTrzo3B68B4sGL/cYOGCJhywIPRISzQegPXV5P3q6ortI74oixAg5I2ABAtZEUKefpOZmUl3hVsxlLrBkr9RwXi4GaC8vDyWYg/w/fHxsbLoX/bunzWOK4oC+BeWQJUqgRASSF0qgdKpFBiXbuzKqVwY7MaR0FdIo0adYPLDA4fNe7uXXU3IBuudwtirmdk3T2fun3PvHd/c3ERxqInFXh4cHCSKl0AMYi0iFrOfbI6uOHXoFYHHx8dNxIIvX740vuzo6Eh4vhOxAlYqOQck3uJYt5G+5JiRqWpigaLkqmiylFhDx7q8vIwbXVtI5sUUfPI0Y0lBLAcnFm4M4U7ECm5vb/sEUE26T+WCXtCXZhbEivLCyuYUZfhBrEXE4qfyFSonpPaGVWLqHKDa48OCWKAWlOND1lcTS425t1iwWoZibJqzBPsnJyc5QHheECu4v78varK7YRDLkxohcfYaGlf8JijXnz59Ojs7y49EIRK9glgJwFNhFD7n84JYJC6VPiVCIhkFiwarJmMBynw55fT0tCFBnDjgn9rijx8/vn379u7dO/63qTHXxAoUZwexlhIrEP8mlOkRJ5jnviYWIAexnhOMuaqJVXxvFM6+cerjx49+VIMTlwdsT6ynp6coaoNYi4gViZwk0f9iIm8yIRMUxCpRE6vufmF+ols20NCXkK7novjs+fl5CmpidbFBihm/ILFEqTo5xZ6CGw/TtAGfP392DEjfisxuPqZoiRQdO4yoI4JR3JUcMTxk8aLUM18zPS0FCE7zvXA3jeApvfcIkT39lKxwfn4uQrIGd60YlbAvaFw598eZcnnWfHV1pZLDmBWKvBbTeRkJ2pqw0ibMS/WnDPQXJNbA6HkfGBjEGhjEGhjEGhgYxBoYxJIAE8GVVq6vr6XTkmpVLXI59U9yTq3Rnlvk5BpR1PmdpUPXWUCX8k8FHOm03JuM2asS2nanDaB8zsfMbQtgAb9vjTS2z7UXbSoauRSMLWy+qVk1MMThlpsaM5GWsuAipHaHKQzMZ9Em3KOuB4JcMQ/88PBA4qfYXVxcUDRcgUihI15Lqp4fNYO3RSwKUKEfRsejZk0d1DfK81qdMDUcomuhtTbHpGS7DdLRRUbKmMYmWM8UZHmlRq8PTKW8n5Ymj9Xnths4iBXEzMQepCmqgLrbHoiVQeoSTNFOxEp9kJlf7e5KW30B1ca3SyyPo45yBRaPoDZzNQ2WXDk2Fb34taZBj4bOB/3VgULNRywklobBP/+Jw8PD/I6bHxn4ns9KVyC7pc1L91W/vKYmk+VxnUoC9sFNqXVyZGrnqxXPFBiaVmZfyjKpKTlXa40SpMnKDx8+mM71ydslljCiLm+pgeRzk8H5PK29BV5NrKIex5hNGxA/KNSbYPHy3GPKjgpT+VwkOn+o7aKZuK8wiOWx7qe4mhZeF9k3sepjlhMrHGrbbDLl4RtjLysMYmUQfhArjYE9sSSSq0GbEZKpxiBWBIXeFYZYiUy/roNoY+/Ecp2vG5DXkNTLS5AututdoRHnzEqAkFTkR8jI6wKmQSwPnxjTTglsPXkCWFOd2c2mbz3EqvPz/RKrBoVp7fJoB/bBDtgHuyGPoaWtNq2n3SUCmF3qNRqZqchsEKtCBq12Ihb8n4nlFl4hN5BAV1PdyGbUYL3XOSwGTAsX0ziItQbHx8cRqdcSS7fn+3VgEvZOLPHQ+w2gCOxELDYbewofh3CkDeWKxoApSzD2b5dYdlZB47efyBBEo57/K8G7okpNLJBt7St4JxzYB2Uf+5AJNvC+hmk7yHiM9yT2yujHCN4nHb2RbZTYPKbLicUI5Qne9MRn3MCvdr9ZYWqpQq6EjKlFbgMTQVxhe8sjK9RsXiSM3NyuxPLEJ/JYe4qQuR1G3Texwo8M4yfA2gaq0e3cxCCWgnwcoqBBfNoMWez0srzm1SuaKV5eXpqvi1CU1xW9mjTiwkz3LyRW89KivPG7QKx+XkCi5WEQqx+ran1TfhRd5491kKWnF2B2K0Lp1ZBOxw62ff/+3Vfn4Z6DMIZhCbGYljwSyudrlyfQ3pJY0jqBV97Du1pkVEzUIWMHiDX6gsxqu7I/hfkhd7u3g1jAtDStColPk/sUaGZBiUPF/Greipb5qlcTS+m3+IrUjLchVtrC+vfw5gGr4cptGXEQywHJboiE8V/zXotntydWLsg9JWppBFXjfsnMlxCLpcwrGHpECN2eWCwoK9hH8SKwYhPcpkW+RR1Lukf5FIlD/98oNP/rCcQLZMqZo6FjiUJwAvzl7u6OSuSyWmtETpsIjZe06duf0HspdqkpFRC+58XU7//wDHCyXJIlAVeuL8hfrE0bjG9vQkOzqfNlGaFNMVP2YfX1pGrPqhQ8oHSHrGBa1T6waj5hekfP+8B/ib/bpQMBAAAAACD/10ZoMFZj1ViN1Vg1VmM1Vo3VWI1VYzVWY9VYjdVYBQInF8S0j+DtAAAAAElFTkSuQmCC</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L37"/>
     </sheetView>
   </sheetViews>
@@ -1449,9 +1449,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="225.75">
+    <row r="18" spans="1:12" ht="210.75">
       <c r="A18" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>164</v>
@@ -1460,7 +1460,7 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
@@ -1473,7 +1473,7 @@
         <v>72</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="240">
@@ -1502,9 +1502,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="225.75">
+    <row r="20" spans="1:12" ht="210.75">
       <c r="A20" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>164</v>
@@ -1513,7 +1513,7 @@
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
@@ -1526,7 +1526,7 @@
         <v>79</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="31.5">
@@ -1984,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="L7" sqref="L2:L7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added test cases for Delete Media image Profile APIs. Added tests: OPQA-3176, OPQA-3177
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="176">
   <si>
     <t>GET</t>
   </si>
@@ -528,6 +528,21 @@
   </si>
   <si>
     <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADICAIAAAAiOjnJAAAdqUlEQVR4AezSQREAAAgDIPsHtI6m2GN3kIG5AKiPhViIBWIhFmKBWIiFWCAWYiEWiIVYiAViIRZisc/e2W3HURxxfB9hHmEfYR9hH2EfQY+wb7BAQvwleSXLGINxRAgmEMwROBBC+JBJbDAfiRPyTTjHEC4SckNyldx1fse1/E+7e6YzszvSWrjq1NFZ7Y5GPT2/raquru7ZC7dm/AwuvYHl8v4s7AwWymukJC4O1j9vh8vDsD3gJ69Dk9gxprxufzYH6wEVCJgPFnqhCk3y4liHhWdHoUk4gw7jzA7WgytnB7GWTNFTQw7gJ6/bn83BelDlx2NxADRhRTH4dDYH69spfzsIr0xAh5/hq9uNpogDtgb85HUPEdszo/LZaIlaRQsdrGNI1eZAGnar8O87Ye1CG2hJ3LBjxpaDtT9Z3DnpO9OwdqENSatop4N1nOT5cTgziJV3vFUri4P1041wenCPfjwPaxfakLSKdh4ncbD++3V4eqT7x2ve6XlY8PIk/HV/Da1ysNbP1u/2wo1Z4GdXeXcatu+mTD/bzwPwFaNvtep+pcrB+mQvvDUNr23wos+bBDqWPT97N3GQyM0ZPClI4tcabp4bB/TT/SUviiviunixBnGwXpqEk4Mg/X53t8LxMFQLlvKcOVjESYaUuTNsTywAoSadGIRfzrq1h6uIL4prPFJxsD6c0++pvtolEL49Dzt3J5V/XRfU/2oezlfhkiZwGuKkvYxmIWU6r0J7of35RXGlRycO1pWxbt6Sd/HqGKo099xZvjgIaC5xe753V9sL7c8viitdszhYaHu5NlkEUozvepQLwwBM0mfvxeK3e+HdWUA/L0DpYK1R3pxy21K9OukW0ODv3pv1PDT7x+1wtgo05tFBOD8M/Gryn6/DpVH47iBIr6WOm/bnF4V/dLCOUP51x+6flF91FxOA1lBzh0FCY/n5NAip7yxUxwjK/KK4UgfryNl6cYJhQHlRTxVZqMcpvuOA/hzKX/YDDg79yUbADrWU3aGQkuITc4MXX9R9SZUnSFX5aYmDL7tkMslOUYZwriK5kMbsZkvs3oNXSzlTpVQ9Qni34QnSNRsncy4yS22FwNyo2hp0cIiUTG1+k6k6NeDXezICogrFCMVNooXXZwH9zV5WUTiJkTLlsE7Rm3VCH2bMwcLXEOTGMe8Pxx3wIsCyqrrf73WbChRVKFYqBiumKgYLSkTMw4PwwiTFAqPFR9InR+2R4qqTwJ+ecbBWEHVorJtVb936hz2Wc5FqT3HcqRZUkVvi19gmCSk0huN0JaoW+qf9EMvXdwK+7wdjFKvGJSzefHkjnKoCxz8x0p9IOIzrzTuBnnGwuotsgNxHonxlVxdy7pbKeqzKnS9zNUzI1PidP++TOOBm491ivlOqUOgpC1QZUrEm/pErbeoEjuwuDlaxT3eHTXkpzE+3HKkisBXldIYI5qco2CodLAW1mFeutO9vl4P1zDjvTWlK1TMjlbIo3C4LyQijir/9/6bl1hwLUXLB2CfBYX7N5O+3w/OT8BATfxUkxWeQuUr1zkGQFHqA/nGwlhHSPC37lNgcnlTN8vpG+wqZUkGVyMAaCRcjg59QAivbw/D+XL57EUL9bLo4jL/lGKiSXhyJrRwpOwawWn273pg6WB1Fd1RjqEQVXqgESgVSK9b7Mp3HVAzKCxMi7jh4un33/afHMS6NXs9sVaKcwYSRo3iKFQMp0WAzV/rHweos8i95h2IS8gDrieGilGW7kitM62QYAxaFUN3SVJYlZ5yv2y8CsE/c+BQFOKsVmatYD2bBBMuUf4q1S4TrzTuBnllSHCyNwhjVW2+eGzZ2KGyRJb+hcVxKlRXJlPPvpKwElubyaIDAAhSoysHCMpmJBQtUvgzHVwALwdThTEtU6QvGtSsBRpMQB2v9osxCPvrDvIlFop+tysAinwlAMi2WUtc7uSvkI7BLA3AYeqjk6eT0OV6oEb1xfgF6v4qDpTFgbq7emVqGXQXmQGYlU+X8Pgja7UdBQQwJLM0DcpiQgjwCrHICouAZHawVRGMrjcIKwQTGBue1SkHVucrAYu1Dow+iMVACSeYWKTr4RV2TiL1EFWpDNhkkPgUpTqL8BdaI9yWpeSuODGgVPWP/iObRYw5W95yhBvkN6w7mFXgtvzQZqjgJiyBkirjlKAIKcRqdjwi88JKP1pWi86lu9ulK0JTNEiODcqSvkUH6XxLlnA5W2xyjNJ/Tfc3WHSxT7Z4C+tEcPyhDorvLrTITogbgHAWWGS1W0WDwoFN3HeNBKpXz2NlIjqOUcMWGTcSkMz96P9PCF684g+RgFTLR0jjmhaRk2YKMljKfJBe6TtQkzkjxuIJxHBxsMQEMQwj/+hT2Kcv1azZGIAKlon5RJV9WBmt7KO4L/UPvOVgN6dBCryVTb/hBIWVK0B3boQuVVWJpFbw+ovov35gvNyeoPKOYTsXc8d6ovjrZqJKFi8F6OAVLH+UqN0dLOL7td8/BattruBgJzkVIoQTUsTD6U30ftaB53oH32XlBYmMFG7Ip8wRkLasCNa20de8OpWcqowqVQcVXNpYzJPM/GkgCd/a3xUlGB0tS9gXJDJrYujqhONiMQWqWqIThNm9mFgsXaR/p/c8joLEZdoOX+OoTafHvoJn/Hhfo0cIP5kkoKaevbILYog1x3lVUKVNfUneF5eFSKc5oH5UzuyxzUnbBmgrkRi4t/K8XxuFg2t5Cl5JkDZ8qTV/ymA5WKhqUlc1V70JIjgnZGR7itC6gd0y54ZcB3VLw9EzZaNlck4NVZEu+QLZKVCk53nFhRaGWXIWgfW5Ww/iAjZDiBs/v1jrvVGJL15svQqQ9CvXEjaDnRWq36LEyVQ6W+o4xIF9Z9Wb9ys9Lo/Z4cb/TKZ3z36z1g60ehUJWIi3mvCXYqpOLxAQOOq+9VgqjlILHpuZdhK5qZX2uMKFKNcot5WKVVjectfnmvsHCJlEhzdRkbLEMrHMVr2WrRJVdkWL81CCtOuhzsPjKKrAgFOV1IkIqVubv8k0+357WbC9zeYjdStc0axX1oQo8keIXVUp01ea6xFMxm0D/2EQ4PUZypNmhex4rj9wJNTD15QJwRu+6eUaVTf99ur/mjSq/bI7WZbFEFSqLpdnARJvCLMVhnsfKgyp1UCFDmK9SR2WxCF+MqlZblmHSnhsf4naMT/L4E+0Z0VzUL6qeiibaiZxyqpSg5zB9A3MVfA6WZjPKGRpN1ZXWE++p5EHRTEPOyRA8MThEsLYIyUfJ/5UN08gUj6xRYWHNj7BTtq9YCuFglc2VjJYEtqLid7o7r1bQQtPSCJE4GrAeHx5iUHXz3kWO/Apqj1W82TLzwrARwhIHV+goGS0Hq5D0K5Xz8hVvG6tq4pk7ynRefOM/VjR9JEJefkt19z1/CVdPJjtY3YUbaRPP3NojE7weKzs0I2nvsD3JGxudN3ADptiMOVjts+0dXCGG6tYcByEf0cpiEesAVmyxKJu5qRt/CGKp9jOq52leF/TqBnWLYJdapnPDWqdPb/T0JfTg/WCm7k6LARXXCzsG7SSEWG5aFpwjqJ2rDhGsk801gHLHJ74Zw25Hsz1che1dI9VODcrLe/C+0vRzsiZ9Z1gqyeWwyyNtXqU70bgjyNnDdI6YIsYQyqWVd6s/hUazPSRQYqSk6Uxiy6loryDN++tpuYDmSkBtv4GtElVaylyOvdYrGDNRdTpymtcbNq1AxBY9U04mO1gJXph6U3VTCay4wA0PKKrybYmxBzdkQg5ToHmzoiW447TA8EpWxExy5OKQR12w/UQ+2yO17eba95WDtULtcvxN1X4eMVVnopQ999X2CzkZBT1WqfzKpOet3pnStnw6NdPxWGFO2qx1SEfiV0iZkqZfVRws5jTsi6hFnppEawrtVf4gqlRLrm1FbbYnnsbZHhBpUYzQ/35xoEBZjsTYgu/um69iq6Aqn623LqKvHKySNE2valm6Pi3V46p0TjhKcDeAxbqa+KM/7oVrfVosjUxB4ZCyr/RGMtChT9wVFkTLVIrLzKMvK87x/rKypyrNFh/ef2kcD4otB6t9NouOqwVRy+EbP23Z3URauxUR9EqNt+DvkXsHDV81eEBys2Ro+bST0A/dMlgOFqao/UxF4hN5LZOmbfiakqhvTomsCVziUZvN+XR+przwpfHPT/LCKaYjbU1Yuj4WgnkfPZ/NSXMqHqayVVFIwzi309zXCrV+vmBV2dQCeao5Sf5WK121tZruxPUpE3nE+IuE+BftJrlBVgYVsi8SxlVaKqiKBsBi+Jk//9c+StNpz45tRGkas8VV+ILVzgIuLXqtWJCkvIN2QZLKTXyoJGpzBnWnsoquxi+AdmDLB6d5ChQny8RzMj6AYGzVWa2cjnJgQgplwueChpa+xL67FGZspDIhhUWb9WBpK0ezRngZPVciFw5QYsJ+xWlqn2bMks4px1Rekt9+1ZD2qjxhmoJFD5T6h95LxMEqlORqKXqrADbd4yAbVGrPPjIC2jFb20Bqm78fjdkxS9l8bUkaO1lMFDClE5r8/EhboS4lkCSqtHGXhH4obpriYLXfIiuNvjE/5WX4Oo9FPxBQKnjS+vpTNTO4xGSApQf42ObYcs3amy99YDgGDzSXnhGirpWToK/Jh5b3ptNMvINVjuLpO9wZ+sKEX8uFgW2dEZZJ2fyk0Dk2QrnAFnYrfsrX9eZ895WxVctQkHO4XUTPWBfRV+oiB6v/7DM+ov2OavJcgPVwBhY/7eSE/OBY3iqc2IuViVg+BUnbFWDlKbH8EdTrFweLO6eJGo0iMVFmhHgtr4TqsIKFM4ZUOag93EG21r3KSGCx6hcGFoIqbdk1x6zOls/zWSc4WL1FXXE5pTYwjsXyk/n0osxVef9F/sUti+Xrsv+2XdZD2VZp2rNPW6s1iaobmPO+Pa+vCiScenua0Kmr46rVA/TGyhGVg6UOTdYSJmxBQ2F6EbDKc0TlkYGZxnzXUN4XWNqrsswWdisXSsSs0A/dqXQeUaUHc0hXeJ60g6UhW53ylS2tiFJlqQKy8jZlBb8JsjpD/nAAYizbsw+Ts7TsT4wq8mcos0DlpwlJl3GLDpbWPdercpsJCskgvMEOqTacn3xkuQbBygltYxJMnUwjVqrVHu56qg+59ZbCs8oMKXRTS4nSij9/rNxRPghTYLXYnhp3BivRBnlAQ6SVpmELopFBm8X1hOoMA1uumT5XgRSqR3Ku/0GYbrEQGOr2sIbCJsSrb+dnVGlHkPY7pqISt1i9S2lNgfTdWXkuSLtodMvyE7jEGfDdoWUTqHiuGce9NCG9nq/OYHGsZRbYe+1QHzPrMdYKorrvWC/VQUPco3y95Q40UNdYUndCf5JQxeJjiahCteQm3lP0ZLxsK90ZizFgb2VqXG/eCdd8VLj6V3azijuUvm57SwClPJKCRVGlqNzMVUwVenVSv6foGS00bSfs103BzKWhyOu2sEJrK/oUz7x3EexWvp443W5U1Q16spJskqiyNNWb0/hTUYV2WHsDTFuL+j7qtJbJvGvK0sFac3I1D03ae2FRdbbSHVVWkzpmtNu2IoAFUhaBXZuUGELXIw4Wd/r80O49L6hBaBX2Ejm1FuIqPCC2qk87QQ00VF1ucIVcRXxR/F8H64ipwopgS2LlrpQGlfl6YqwCf/KBtl9btyRPnpKldLCOTqinU+9LL4/yTFU+khKa9lzxHMrVBWtEnTvaPvxCaH9+UVypg3WEQj3diUGu9XltPBpmKfnqPxXfRS2d6ElY8KNAqrXUXxFX6mAdnZCczO8B1eLtRUjpz/GM2Zb/6DKleYRQViRzZdS92t3BWqN8spffAzY6W/4uymKJqu3Kcgrpk5W0jpl01BbTi3WuiqcGs7HMxYq9IUJ7of35RXGlDtaRyltTspRSbFjnSFkrYdDk/t2YNZWyyNlpTpCIqkdLrCvSEh0Haw074vEtR3mx/G6OKC8kAisuZbk5a4yiUCL0dV2Ug7UGwZ29PWWeGErwZZ3vrkpZdqsadLBSFC+wjhmv10VoCe2hVSpEPibiYImqncrcmeKkzgUwGKr3Zj0aJNqQtOq4seVgUZap+6cHza1baEPaKtp5nMTBYhZPQZIp73irHKxV5fWN9Ba+s36LRRvSVr3uFut4CYHRrkXfFoArxlqn0IakVbTTwTqGbB1MyQuUFrYzuLt0d+0D2U7q9VYTzmBZU9XxNT0xmlbRNlHlYH3rxKhCjS2kvJ1VGQWjCjW2HlxxsCx1Lm2Sz/Z1DK/bnu3BFQeLJKdlz634rs1hJEXLc8+m/MmDKw4WEQ+VLRcqfpam/IBpe2Ba4o8zcB6OafVQAgfLhXkbgcVrFwerz6LQWzNZtW+L/I9dOhACAABgIOQPNbW/iRRDYiEWiIVYiAViIRZiIRaIhViIBWIhFmKBWIhVbTs75/3SyQ5F8f92baBYwIYigoL1a0OxY0exK7qCqDwsWMGCIPbeFUWsSN6BwGHInYTvQxf2yZwflnFy0yaf3HsTWX+Hp+npaVbc2NjQLxcWFpRFKNI2m5ubyqKnpyeYdXV11dXV1dTUtLe3o5fb21vr/8d5eBgbG0Ob+BfPyin0qwcwOzur/PT+/r66ujo4ONjc3FxdXd3Q0IABjIyMLC8vX1xc4OMoi05PTycmJlpbW3Wt7u7ulZUVtGb9u0xbW/yM6+vryk+Pj4/aYGZm5n8P1vPz86+wFRcXx4r5+fn6ZUpKirIIRdqmvLxcCb28vGAVo6OjZUeRkZFYsPv7eyXU2dlJs7KyMmXX9fV1VFQUjY+OjowdNTo6ihk55ltbW6uE0E5BQYGvfXx8PNr8/PxUQklJSTTDqM7Pz5XQ2tqa8Z3/swKw7u7uMjIy3N1hnQ4PD82/b9rW5rXZ3d1VFjU1NXktt7e3lUctLS2Orm3DhifjTrCpuLj47e3NqEiCafPDwcL2MkIhtinnD1cvQ+HXwYK3yM3NZS8xMTH19fXj4+MILvBhCQkJLEpMTESsdIBVWlpqc1dwezaw9vf3vd6xqqoKHwHhcmpqCtPs6elBdCsqKhoYGFAenZyceKlKTU1FBJ+cnERQrqys9HaH6m6woKWlpZ8MltT8/LxcDOpbwMISsousrCxAYIRIxDgadHR0OMCi03K7K2MuoIfvHTmioZKSEtZCTvbx8aE8Ojg4wDbQpRERETs7O26wkpOTX19fA7C+EywEAnqLs7MzJYQvzqQkNjaWS0iwHE6L7soB1tDQkMy93ELsBi66Sk5Ojm8ihayczTY2NvqC5R1Yb29vANa3gQVKmFNLJijEIw5jb29PgoUV4krTPdBd0UbOhXOky7y8vGSR44TLKkwJpNLS0rRNenq6L1iIm4yneGAWH4BlgoUU+x+LUCTBgjuRW1ZqcXGRZniWYIFa5Eb6ORQKGe6KYdSYCz0iwxYPobibcNwveKOnPFJQGBLb9AUL9PT19bEphFcJVgBWWCJYTIH5HodzZRG/MoQh+YKF7Io2dFp0V9nZ2bijknPhxRKCLEuZjw8PDyPqKaH+/n6a3dzcKCF52LSBhTMjOqIZTpp/F1gBWPixsLCQTstwV3Nzc2jEMRfwgRxcptWI1KDTuEWDc6WB4/6Ww3OAhR818ZwIUAvAMsHCZUHIIhT9abDwCwDvaAEES5Ffu8Hi5TtO/hUVFTrzo3B68B4sGL/cYOGCJhywIPRISzQegPXV5P3q6ortI74oixAg5I2ABAtZEUKefpOZmUl3hVsxlLrBkr9RwXi4GaC8vDyWYg/w/fHxsbLoX/bunzWOK4oC+BeWQJUqgRASSF0qgdKpFBiXbuzKqVwY7MaR0FdIo0adYPLDA4fNe7uXXU3IBuudwtirmdk3T2fun3PvHd/c3ERxqInFXh4cHCSKl0AMYi0iFrOfbI6uOHXoFYHHx8dNxIIvX740vuzo6Eh4vhOxAlYqOQck3uJYt5G+5JiRqWpigaLkqmiylFhDx7q8vIwbXVtI5sUUfPI0Y0lBLAcnFm4M4U7ECm5vb/sEUE26T+WCXtCXZhbEivLCyuYUZfhBrEXE4qfyFSonpPaGVWLqHKDa48OCWKAWlOND1lcTS425t1iwWoZibJqzBPsnJyc5QHheECu4v78varK7YRDLkxohcfYaGlf8JijXnz59Ojs7y49EIRK9glgJwFNhFD7n84JYJC6VPiVCIhkFiwarJmMBynw55fT0tCFBnDjgn9rijx8/vn379u7dO/63qTHXxAoUZwexlhIrEP8mlOkRJ5jnviYWIAexnhOMuaqJVXxvFM6+cerjx49+VIMTlwdsT6ynp6coaoNYi4gViZwk0f9iIm8yIRMUxCpRE6vufmF+ols20NCXkK7novjs+fl5CmpidbFBihm/ILFEqTo5xZ6CGw/TtAGfP392DEjfisxuPqZoiRQdO4yoI4JR3JUcMTxk8aLUM18zPS0FCE7zvXA3jeApvfcIkT39lKxwfn4uQrIGd60YlbAvaFw598eZcnnWfHV1pZLDmBWKvBbTeRkJ2pqw0ibMS/WnDPQXJNbA6HkfGBjEGhjEGhjEGhgYxBoYxJIAE8GVVq6vr6XTkmpVLXI59U9yTq3Rnlvk5BpR1PmdpUPXWUCX8k8FHOm03JuM2asS2nanDaB8zsfMbQtgAb9vjTS2z7UXbSoauRSMLWy+qVk1MMThlpsaM5GWsuAipHaHKQzMZ9Em3KOuB4JcMQ/88PBA4qfYXVxcUDRcgUihI15Lqp4fNYO3RSwKUKEfRsejZk0d1DfK81qdMDUcomuhtTbHpGS7DdLRRUbKmMYmWM8UZHmlRq8PTKW8n5Ymj9Xnths4iBXEzMQepCmqgLrbHoiVQeoSTNFOxEp9kJlf7e5KW30B1ca3SyyPo45yBRaPoDZzNQ2WXDk2Fb34taZBj4bOB/3VgULNRywklobBP/+Jw8PD/I6bHxn4ns9KVyC7pc1L91W/vKYmk+VxnUoC9sFNqXVyZGrnqxXPFBiaVmZfyjKpKTlXa40SpMnKDx8+mM71ydslljCiLm+pgeRzk8H5PK29BV5NrKIex5hNGxA/KNSbYPHy3GPKjgpT+VwkOn+o7aKZuK8wiOWx7qe4mhZeF9k3sepjlhMrHGrbbDLl4RtjLysMYmUQfhArjYE9sSSSq0GbEZKpxiBWBIXeFYZYiUy/roNoY+/Ecp2vG5DXkNTLS5AututdoRHnzEqAkFTkR8jI6wKmQSwPnxjTTglsPXkCWFOd2c2mbz3EqvPz/RKrBoVp7fJoB/bBDtgHuyGPoaWtNq2n3SUCmF3qNRqZqchsEKtCBq12Ihb8n4nlFl4hN5BAV1PdyGbUYL3XOSwGTAsX0ziItQbHx8cRqdcSS7fn+3VgEvZOLPHQ+w2gCOxELDYbewofh3CkDeWKxoApSzD2b5dYdlZB47efyBBEo57/K8G7okpNLJBt7St4JxzYB2Uf+5AJNvC+hmk7yHiM9yT2yujHCN4nHb2RbZTYPKbLicUI5Qne9MRn3MCvdr9ZYWqpQq6EjKlFbgMTQVxhe8sjK9RsXiSM3NyuxPLEJ/JYe4qQuR1G3Texwo8M4yfA2gaq0e3cxCCWgnwcoqBBfNoMWez0srzm1SuaKV5eXpqvi1CU1xW9mjTiwkz3LyRW89KivPG7QKx+XkCi5WEQqx+ran1TfhRd5491kKWnF2B2K0Lp1ZBOxw62ff/+3Vfn4Z6DMIZhCbGYljwSyudrlyfQ3pJY0jqBV97Du1pkVEzUIWMHiDX6gsxqu7I/hfkhd7u3g1jAtDStColPk/sUaGZBiUPF/Greipb5qlcTS+m3+IrUjLchVtrC+vfw5gGr4cptGXEQywHJboiE8V/zXotntydWLsg9JWppBFXjfsnMlxCLpcwrGHpECN2eWCwoK9hH8SKwYhPcpkW+RR1Lukf5FIlD/98oNP/rCcQLZMqZo6FjiUJwAvzl7u6OSuSyWmtETpsIjZe06duf0HspdqkpFRC+58XU7//wDHCyXJIlAVeuL8hfrE0bjG9vQkOzqfNlGaFNMVP2YfX1pGrPqhQ8oHSHrGBa1T6waj5hekfP+8B/ib/bpQMBAAAAACD/10ZoMFZj1ViN1Vg1VmM1Vo3VWI1VYzVWY9VYjdVYBQInF8S0j+DtAAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Verify that imageUrl is not returned in Get User Profile API once media image is deleted using Vanilla API</t>
+  </si>
+  <si>
+    <t>Verify that user media image is deleted using Vanilla Profile API</t>
+  </si>
+  <si>
+    <t>OPQA-3176</t>
+  </si>
+  <si>
+    <t>OPQA-3177</t>
   </si>
 </sst>
 </file>
@@ -968,10 +983,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L37"/>
+    <sheetView tabSelected="1" topLeftCell="I34" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1476,38 +1491,37 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="240">
+    <row r="19" spans="1:12" ht="32.25">
       <c r="A19" s="8" t="s">
-        <v>79</v>
+        <v>174</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>41</v>
+        <v>171</v>
+      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="210.75">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="32.25">
       <c r="A20" s="8" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -1518,129 +1532,132 @@
       <c r="E20" t="s">
         <v>0</v>
       </c>
-      <c r="G20" s="20" t="s">
-        <v>165</v>
-      </c>
+      <c r="G20" s="20"/>
       <c r="H20" s="7"/>
       <c r="I20" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="240">
+      <c r="A21" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="J20" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="31.5">
-      <c r="A21" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>52</v>
+      <c r="B21" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
       </c>
       <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="210.75">
+      <c r="A22" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="31.5">
+      <c r="A23" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="60">
-      <c r="A22" s="8" t="s">
+    <row r="24" spans="1:12" ht="60">
+      <c r="A24" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B24" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>11</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F24" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75">
-      <c r="A23" s="8" t="s">
+    <row r="25" spans="1:12" ht="15.75">
+      <c r="A25" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
         <v>34</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="1:12" ht="31.5">
-      <c r="A24" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:12" ht="31.5">
-      <c r="A25" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" t="s">
-        <v>35</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>0</v>
@@ -1649,202 +1666,196 @@
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="4" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:12" s="9" customFormat="1" ht="15.75">
+    <row r="26" spans="1:12" ht="31.5">
       <c r="A26" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26"/>
-      <c r="H26" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I26"/>
-      <c r="J26" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K26"/>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" ht="45">
-      <c r="A27" t="s">
-        <v>121</v>
+        <v>76</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" ht="31.5">
+      <c r="A27" s="8" t="s">
+        <v>77</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="4" t="s">
-        <v>85</v>
-      </c>
+      <c r="H27" s="6"/>
       <c r="I27" s="1"/>
       <c r="J27" s="4" t="s">
-        <v>151</v>
+        <v>19</v>
       </c>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="30">
-      <c r="A28" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" t="s">
-        <v>87</v>
+    <row r="28" spans="1:12" s="9" customFormat="1" ht="15.75">
+      <c r="A28" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28"/>
-      <c r="J28" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="30">
+        <v>11</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28"/>
+      <c r="J28" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="K28"/>
+      <c r="L28"/>
+    </row>
+    <row r="29" spans="1:12" ht="45">
       <c r="A29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>88</v>
+        <v>121</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>92</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>11</v>
+        <v>89</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="F29" t="s">
         <v>20</v>
       </c>
+      <c r="G29" s="1"/>
       <c r="H29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" ht="30">
+      <c r="A30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30"/>
+      <c r="J30" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="30">
+      <c r="A31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J31" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="45">
-      <c r="A30" t="s">
+    <row r="32" spans="1:12" ht="45">
+      <c r="A32" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
         <v>94</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F32" t="s">
         <v>110</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J32" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="31.5">
-      <c r="A31" t="s">
+    <row r="33" spans="1:10" ht="31.5">
+      <c r="A33" t="s">
         <v>126</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B33" s="11" t="s">
         <v>99</v>
-      </c>
-      <c r="C31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="47.25">
-      <c r="A32" t="s">
-        <v>128</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H32" s="4"/>
-      <c r="I32" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="47.25">
-      <c r="A33" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
@@ -1852,15 +1863,12 @@
       <c r="D33" t="s">
         <v>15</v>
       </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="E33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="4"/>
       <c r="I33" s="8" t="s">
         <v>124</v>
       </c>
@@ -1870,45 +1878,54 @@
     </row>
     <row r="34" spans="1:10" ht="47.25">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H34"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H34" s="4"/>
       <c r="I34" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="J34" s="4" t="s">
-        <v>150</v>
+      <c r="J34" s="7" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="47.25">
       <c r="A35" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>107</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35"/>
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I35" s="8" t="s">
         <v>124</v>
       </c>
@@ -1916,61 +1933,109 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="240">
+    <row r="36" spans="1:10" ht="47.25">
       <c r="A36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" t="s">
-        <v>11</v>
-      </c>
-      <c r="F36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36"/>
       <c r="I36" s="8" t="s">
         <v>124</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="45">
-      <c r="A37" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>93</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="47.25">
+      <c r="A37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" t="s">
-        <v>110</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>142</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37"/>
       <c r="I37" s="8" t="s">
         <v>124</v>
       </c>
       <c r="J37" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="240">
+      <c r="A38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="45">
+      <c r="A39" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>94</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" t="s">
+        <v>110</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deleted Vanilla CreateUserAPI test case (below). OPQA-2574:Verify that for the existing truid, API doesn't allow to create same profile again and check the error status
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="174">
   <si>
     <t>GET</t>
   </si>
@@ -284,18 +284,12 @@
     <t>Verify that for the existing active truid, updateOnboardedStatus API works as expected.</t>
   </si>
   <si>
-    <t>/users/user</t>
-  </si>
-  <si>
     <t>status=200||truid=(SYS_USER1)||onboarded=true</t>
   </si>
   <si>
     <t>{"truid":"(SYS_USER1)", "onboarded": true}</t>
   </si>
   <si>
-    <t>Verify that for the existing truid, API doesn't allow to create same profile again and check the error status</t>
-  </si>
-  <si>
     <t>Verify that for the existing active truid, update active status  using  updateUserStatus of Admin API works as expected.</t>
   </si>
   <si>
@@ -380,9 +374,6 @@
     <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
   </si>
   <si>
-    <t>OPQA-2574</t>
-  </si>
-  <si>
     <t>OPQA-2575</t>
   </si>
   <si>
@@ -543,6 +534,9 @@
   </si>
   <si>
     <t>OPQA-3177</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)</t>
   </si>
 </sst>
 </file>
@@ -983,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I34" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L39"/>
+      <selection activeCell="L2" sqref="L2:L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1090,16 +1084,16 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1115,11 +1109,11 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -1143,19 +1137,19 @@
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
       <c r="I5" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1171,11 +1165,11 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -1200,7 +1194,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -1225,7 +1219,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K8" s="1"/>
     </row>
@@ -1249,10 +1243,10 @@
         <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="31.5">
@@ -1275,10 +1269,10 @@
         <v>20</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="18" customFormat="1" ht="31.5">
@@ -1356,7 +1350,7 @@
       </c>
       <c r="H13"/>
       <c r="J13" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5">
@@ -1380,7 +1374,7 @@
       </c>
       <c r="H14"/>
       <c r="J14" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45">
@@ -1408,7 +1402,7 @@
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="K15" s="1"/>
     </row>
@@ -1435,7 +1429,7 @@
         <v>36</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="255">
@@ -1458,45 +1452,45 @@
         <v>30</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="210.75">
       <c r="A18" s="8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="8" t="s">
         <v>72</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="32.25">
       <c r="A19" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1505,7 +1499,10 @@
         <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>171</v>
+        <v>168</v>
+      </c>
+      <c r="F19" t="s">
+        <v>173</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="7"/>
@@ -1518,16 +1515,16 @@
     </row>
     <row r="20" spans="1:12" ht="32.25">
       <c r="A20" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
@@ -1535,10 +1532,10 @@
       <c r="G20" s="20"/>
       <c r="H20" s="7"/>
       <c r="I20" s="8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="240">
@@ -1564,34 +1561,34 @@
         <v>41</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="210.75">
       <c r="A22" s="8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="8" t="s">
         <v>79</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="31.5">
@@ -1617,7 +1614,7 @@
         <v>18</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="60">
@@ -1643,7 +1640,7 @@
         <v>54</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75">
@@ -1690,7 +1687,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="1"/>
       <c r="J26" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K26" s="1"/>
     </row>
@@ -1748,41 +1745,33 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" ht="45">
+    <row r="29" spans="1:12" ht="30">
       <c r="A29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>92</v>
+        <v>119</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I29" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29"/>
       <c r="J29" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="K29" s="1"/>
+        <v>96</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="30">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -1791,122 +1780,130 @@
         <v>87</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H30"/>
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="J30" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="30">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="45">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>91</v>
+        <v>108</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="31.5">
       <c r="A32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="47.25">
+      <c r="A33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" t="s">
-        <v>94</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" t="s">
-        <v>110</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="31.5">
-      <c r="A33" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>99</v>
-      </c>
       <c r="C33" t="s">
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="H33" s="4"/>
       <c r="I33" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>145</v>
+        <v>121</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="47.25">
       <c r="A34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H34" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I34" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>101</v>
+        <v>121</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="47.25">
       <c r="A35" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>102</v>
@@ -1915,128 +1912,99 @@
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35"/>
       <c r="I35" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="47.25">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H36"/>
       <c r="I36" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="47.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="240">
       <c r="A37" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H37"/>
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="I37" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="240">
-      <c r="A38" t="s">
-        <v>132</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>106</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="45">
+      <c r="A38" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" t="s">
+        <v>92</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>41</v>
+        <v>108</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="45">
-      <c r="A39" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s">
         <v>94</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" t="s">
-        <v>110</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2107,71 +2075,71 @@
     </row>
     <row r="2" spans="1:12" ht="47.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3"/>
       <c r="I3" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -2181,70 +2149,70 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F5"/>
       <c r="J5" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>11</v>
@@ -2253,13 +2221,13 @@
         <v>20</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2testcases in Profile & added validations for discoverable field. Tests added in Profile: OPQA-3289, OPQA-3288
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vanilla-Profile" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="184">
   <si>
     <t>GET</t>
   </si>
@@ -284,259 +284,289 @@
     <t>Verify that for the existing active truid, updateOnboardedStatus API works as expected.</t>
   </si>
   <si>
+    <t>Verify that for the existing active truid, update active status  using  updateUserStatus of Admin API works as expected.</t>
+  </si>
+  <si>
+    <t>/admin/users/user/(SYS_USER1)/status</t>
+  </si>
+  <si>
+    <t>{"truid": "(SYS_USER1)","active": true,"onboarded": false}</t>
+  </si>
+  <si>
+    <t>Verify that for the inactive user id, user profile is not returned and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>?id=(SYS_USER1),(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project||lastName=Neon2||location=India||truid=(SYS_USER2)||location=INdia||primaryInstitution=Thomson reuters||role=QA</t>
+  </si>
+  <si>
+    <t>Verify that inactive user is not able to edit  info like title,role,Institution and country using Vanilla API &amp; check the error status.</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER1)/media</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user media info is not returned and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user media image is not returned and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user image is not updated and check the error status using Vanilla API</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER1)/media/image</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, Admin API doesn't allow to create same profile again and check the error status</t>
+  </si>
+  <si>
+    <t>/admin/users/user</t>
+  </si>
+  <si>
+    <t>Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>/admin/users/user/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>Verify that for the invalid user id, user profile is not returned using Admin API and check the error status</t>
+  </si>
+  <si>
+    <t>/admin/users/user/(SYS_USER1)1</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, user status is updated using Admin updateUserStatus API</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, user status is returned using Admin getUserStatus API</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, user profile is returned using Admin getUser API</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
+  </si>
+  <si>
+    <t>OPQA-2575</t>
+  </si>
+  <si>
+    <t>OPQA-2576</t>
+  </si>
+  <si>
+    <t>OPQA-2577</t>
+  </si>
+  <si>
+    <t>OPQA-2577_1</t>
+  </si>
+  <si>
+    <t>OPQA-2578</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id in the bulk list, user profile is not returned and check the bulk profiles in the response using Vanilla API</t>
+  </si>
+  <si>
+    <t>OPQA-2579</t>
+  </si>
+  <si>
+    <t>OPQA-2580</t>
+  </si>
+  <si>
+    <t>OPQA-2583</t>
+  </si>
+  <si>
+    <t>OPQA-2584</t>
+  </si>
+  <si>
+    <t>OPQA-2585</t>
+  </si>
+  <si>
+    <t>OPQA-2587</t>
+  </si>
+  <si>
+    <t>OPQA-2588</t>
+  </si>
+  <si>
+    <t>OPQA-2589</t>
+  </si>
+  <si>
+    <t>OPQA-2590</t>
+  </si>
+  <si>
+    <t>OPQA-2591</t>
+  </si>
+  <si>
+    <t>OPQA-2591_1</t>
+  </si>
+  <si>
+    <t>{"imageType": "png","imageHeight":97,"imageWidth":97,"imageContent":"data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg=="}</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||mediaCategory=image-full</t>
+  </si>
+  <si>
+    <t>{"interest":["computers","science","API AUTOMATION"]}</t>
+  </si>
+  <si>
+    <t>{"active": false,"onboarded": true}</t>
+  </si>
+  <si>
+    <t>status=404||statusCode=404||errorMessage=User not found.</t>
+  </si>
+  <si>
+    <t>status=400||statusCode=400||errorMessage=TRUID is missing.</t>
+  </si>
+  <si>
+    <t>status=413||statusCode=413||errorMessage=Too many TRUIDs provided.</t>
+  </si>
+  <si>
+    <t>status=400||statusCode=400||errorMessage=Image Content not set</t>
+  </si>
+  <si>
+    <t>status=400||statusCode=400||errorMessage=Image Type not set.</t>
+  </si>
+  <si>
+    <t>status=404||statusCode=404||errorMessage=Media not found.</t>
+  </si>
+  <si>
+    <t>status=409||statusCode=409||errorMessage=User already exists.</t>
+  </si>
+  <si>
+    <t>status=200||interest=computers||interest=science||interest=API AUTOMATION</t>
+  </si>
+  <si>
+    <t>OPQA-2679</t>
+  </si>
+  <si>
+    <t>Verify that user is able to edit first name and last name from his own profile page.</t>
+  </si>
+  <si>
+    <t>{"firstName":"ProjectEdited","lastName":"Neon1Edited"}</t>
+  </si>
+  <si>
+    <t>status=200||firstName=ProjectEdited||lastName=Neon1Edited||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
+  </si>
+  <si>
+    <t>status=200||firstName=ProjectEdited||lastName=Neon1Edited</t>
+  </si>
+  <si>
+    <t>OPQA-2679_1</t>
+  </si>
+  <si>
+    <t>{"firstName":"Project","lastName":"Neon1"}</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA||title=Project Neon1||interest=API AUTOMATION</t>
+  </si>
+  <si>
+    <t>{"location":"India","primaryInstitution":"Thomson Reuters","role":"QA"}</t>
+  </si>
+  <si>
+    <t>status=200||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
+  </si>
+  <si>
+    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA||interest=computers||title=Project Neon1</t>
+  </si>
+  <si>
+    <t>Verify that imageContent is returned for the truid using getUser API</t>
+  </si>
+  <si>
+    <t>?image=yes</t>
+  </si>
+  <si>
+    <t>/users/user/(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>OPQA-2957</t>
+  </si>
+  <si>
+    <t>OPQA-2957_1</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADICAIAAAAiOjnJAAAdqUlEQVR4AezSQREAAAgDIPsHtI6m2GN3kIG5AKiPhViIBWIhFmKBWIiFWCAWYiEWiIVYiAViIRZisc/e2W3HURxxfB9hHmEfYR9hH2EfQY+wb7BAQvwleSXLGINxRAgmEMwROBBC+JBJbDAfiRPyTTjHEC4SckNyldx1fse1/E+7e6YzszvSWrjq1NFZ7Y5GPT2/raquru7ZC7dm/AwuvYHl8v4s7AwWymukJC4O1j9vh8vDsD3gJ69Dk9gxprxufzYH6wEVCJgPFnqhCk3y4liHhWdHoUk4gw7jzA7WgytnB7GWTNFTQw7gJ6/bn83BelDlx2NxADRhRTH4dDYH69spfzsIr0xAh5/hq9uNpogDtgb85HUPEdszo/LZaIlaRQsdrGNI1eZAGnar8O87Ye1CG2hJ3LBjxpaDtT9Z3DnpO9OwdqENSatop4N1nOT5cTgziJV3vFUri4P1041wenCPfjwPaxfakLSKdh4ncbD++3V4eqT7x2ve6XlY8PIk/HV/Da1ysNbP1u/2wo1Z4GdXeXcatu+mTD/bzwPwFaNvtep+pcrB+mQvvDUNr23wos+bBDqWPT97N3GQyM0ZPClI4tcabp4bB/TT/SUviiviunixBnGwXpqEk4Mg/X53t8LxMFQLlvKcOVjESYaUuTNsTywAoSadGIRfzrq1h6uIL4prPFJxsD6c0++pvtolEL49Dzt3J5V/XRfU/2oezlfhkiZwGuKkvYxmIWU6r0J7of35RXGlRycO1pWxbt6Sd/HqGKo099xZvjgIaC5xe753V9sL7c8viitdszhYaHu5NlkEUozvepQLwwBM0mfvxeK3e+HdWUA/L0DpYK1R3pxy21K9OukW0ODv3pv1PDT7x+1wtgo05tFBOD8M/Gryn6/DpVH47iBIr6WOm/bnF4V/dLCOUP51x+6flF91FxOA1lBzh0FCY/n5NAip7yxUxwjK/KK4UgfryNl6cYJhQHlRTxVZqMcpvuOA/hzKX/YDDg79yUbADrWU3aGQkuITc4MXX9R9SZUnSFX5aYmDL7tkMslOUYZwriK5kMbsZkvs3oNXSzlTpVQ9Qni34QnSNRsncy4yS22FwNyo2hp0cIiUTG1+k6k6NeDXezICogrFCMVNooXXZwH9zV5WUTiJkTLlsE7Rm3VCH2bMwcLXEOTGMe8Pxx3wIsCyqrrf73WbChRVKFYqBiumKgYLSkTMw4PwwiTFAqPFR9InR+2R4qqTwJ+ecbBWEHVorJtVb936hz2Wc5FqT3HcqRZUkVvi19gmCSk0huN0JaoW+qf9EMvXdwK+7wdjFKvGJSzefHkjnKoCxz8x0p9IOIzrzTuBnnGwuotsgNxHonxlVxdy7pbKeqzKnS9zNUzI1PidP++TOOBm491ivlOqUOgpC1QZUrEm/pErbeoEjuwuDlaxT3eHTXkpzE+3HKkisBXldIYI5qco2CodLAW1mFeutO9vl4P1zDjvTWlK1TMjlbIo3C4LyQijir/9/6bl1hwLUXLB2CfBYX7N5O+3w/OT8BATfxUkxWeQuUr1zkGQFHqA/nGwlhHSPC37lNgcnlTN8vpG+wqZUkGVyMAaCRcjg59QAivbw/D+XL57EUL9bLo4jL/lGKiSXhyJrRwpOwawWn273pg6WB1Fd1RjqEQVXqgESgVSK9b7Mp3HVAzKCxMi7jh4un33/afHMS6NXs9sVaKcwYSRo3iKFQMp0WAzV/rHweos8i95h2IS8gDrieGilGW7kitM62QYAxaFUN3SVJYlZ5yv2y8CsE/c+BQFOKsVmatYD2bBBMuUf4q1S4TrzTuBnllSHCyNwhjVW2+eGzZ2KGyRJb+hcVxKlRXJlPPvpKwElubyaIDAAhSoysHCMpmJBQtUvgzHVwALwdThTEtU6QvGtSsBRpMQB2v9osxCPvrDvIlFop+tysAinwlAMi2WUtc7uSvkI7BLA3AYeqjk6eT0OV6oEb1xfgF6v4qDpTFgbq7emVqGXQXmQGYlU+X8Pgja7UdBQQwJLM0DcpiQgjwCrHICouAZHawVRGMrjcIKwQTGBue1SkHVucrAYu1Dow+iMVACSeYWKTr4RV2TiL1EFWpDNhkkPgUpTqL8BdaI9yWpeSuODGgVPWP/iObRYw5W95yhBvkN6w7mFXgtvzQZqjgJiyBkirjlKAIKcRqdjwi88JKP1pWi86lu9ulK0JTNEiODcqSvkUH6XxLlnA5W2xyjNJ/Tfc3WHSxT7Z4C+tEcPyhDorvLrTITogbgHAWWGS1W0WDwoFN3HeNBKpXz2NlIjqOUcMWGTcSkMz96P9PCF684g+RgFTLR0jjmhaRk2YKMljKfJBe6TtQkzkjxuIJxHBxsMQEMQwj/+hT2Kcv1azZGIAKlon5RJV9WBmt7KO4L/UPvOVgN6dBCryVTb/hBIWVK0B3boQuVVWJpFbw+ovov35gvNyeoPKOYTsXc8d6ovjrZqJKFi8F6OAVLH+UqN0dLOL7td8/BattruBgJzkVIoQTUsTD6U30ftaB53oH32XlBYmMFG7Ip8wRkLasCNa20de8OpWcqowqVQcVXNpYzJPM/GkgCd/a3xUlGB0tS9gXJDJrYujqhONiMQWqWqIThNm9mFgsXaR/p/c8joLEZdoOX+OoTafHvoJn/Hhfo0cIP5kkoKaevbILYog1x3lVUKVNfUneF5eFSKc5oH5UzuyxzUnbBmgrkRi4t/K8XxuFg2t5Cl5JkDZ8qTV/ymA5WKhqUlc1V70JIjgnZGR7itC6gd0y54ZcB3VLw9EzZaNlck4NVZEu+QLZKVCk53nFhRaGWXIWgfW5Ww/iAjZDiBs/v1jrvVGJL15svQqQ9CvXEjaDnRWq36LEyVQ6W+o4xIF9Z9Wb9ys9Lo/Z4cb/TKZ3z36z1g60ehUJWIi3mvCXYqpOLxAQOOq+9VgqjlILHpuZdhK5qZX2uMKFKNcot5WKVVjectfnmvsHCJlEhzdRkbLEMrHMVr2WrRJVdkWL81CCtOuhzsPjKKrAgFOV1IkIqVubv8k0+357WbC9zeYjdStc0axX1oQo8keIXVUp01ea6xFMxm0D/2EQ4PUZypNmhex4rj9wJNTD15QJwRu+6eUaVTf99ur/mjSq/bI7WZbFEFSqLpdnARJvCLMVhnsfKgyp1UCFDmK9SR2WxCF+MqlZblmHSnhsf4naMT/L4E+0Z0VzUL6qeiibaiZxyqpSg5zB9A3MVfA6WZjPKGRpN1ZXWE++p5EHRTEPOyRA8MThEsLYIyUfJ/5UN08gUj6xRYWHNj7BTtq9YCuFglc2VjJYEtqLid7o7r1bQQtPSCJE4GrAeHx5iUHXz3kWO/Apqj1W82TLzwrARwhIHV+goGS0Hq5D0K5Xz8hVvG6tq4pk7ynRefOM/VjR9JEJefkt19z1/CVdPJjtY3YUbaRPP3NojE7weKzs0I2nvsD3JGxudN3ADptiMOVjts+0dXCGG6tYcByEf0cpiEesAVmyxKJu5qRt/CGKp9jOq52leF/TqBnWLYJdapnPDWqdPb/T0JfTg/WCm7k6LARXXCzsG7SSEWG5aFpwjqJ2rDhGsk801gHLHJ74Zw25Hsz1che1dI9VODcrLe/C+0vRzsiZ9Z1gqyeWwyyNtXqU70bgjyNnDdI6YIsYQyqWVd6s/hUazPSRQYqSk6Uxiy6loryDN++tpuYDmSkBtv4GtElVaylyOvdYrGDNRdTpymtcbNq1AxBY9U04mO1gJXph6U3VTCay4wA0PKKrybYmxBzdkQg5ToHmzoiW447TA8EpWxExy5OKQR12w/UQ+2yO17eba95WDtULtcvxN1X4eMVVnopQ999X2CzkZBT1WqfzKpOet3pnStnw6NdPxWGFO2qx1SEfiV0iZkqZfVRws5jTsi6hFnppEawrtVf4gqlRLrm1FbbYnnsbZHhBpUYzQ/35xoEBZjsTYgu/um69iq6Aqn623LqKvHKySNE2valm6Pi3V46p0TjhKcDeAxbqa+KM/7oVrfVosjUxB4ZCyr/RGMtChT9wVFkTLVIrLzKMvK87x/rKypyrNFh/ef2kcD4otB6t9NouOqwVRy+EbP23Z3URauxUR9EqNt+DvkXsHDV81eEBys2Ro+bST0A/dMlgOFqao/UxF4hN5LZOmbfiakqhvTomsCVziUZvN+XR+przwpfHPT/LCKaYjbU1Yuj4WgnkfPZ/NSXMqHqayVVFIwzi309zXCrV+vmBV2dQCeao5Sf5WK121tZruxPUpE3nE+IuE+BftJrlBVgYVsi8SxlVaKqiKBsBi+Jk//9c+StNpz45tRGkas8VV+ILVzgIuLXqtWJCkvIN2QZLKTXyoJGpzBnWnsoquxi+AdmDLB6d5ChQny8RzMj6AYGzVWa2cjnJgQgplwueChpa+xL67FGZspDIhhUWb9WBpK0ezRngZPVciFw5QYsJ+xWlqn2bMks4px1Rekt9+1ZD2qjxhmoJFD5T6h95LxMEqlORqKXqrADbd4yAbVGrPPjIC2jFb20Bqm78fjdkxS9l8bUkaO1lMFDClE5r8/EhboS4lkCSqtHGXhH4obpriYLXfIiuNvjE/5WX4Oo9FPxBQKnjS+vpTNTO4xGSApQf42ObYcs3amy99YDgGDzSXnhGirpWToK/Jh5b3ptNMvINVjuLpO9wZ+sKEX8uFgW2dEZZJ2fyk0Dk2QrnAFnYrfsrX9eZ895WxVctQkHO4XUTPWBfRV+oiB6v/7DM+ov2OavJcgPVwBhY/7eSE/OBY3iqc2IuViVg+BUnbFWDlKbH8EdTrFweLO6eJGo0iMVFmhHgtr4TqsIKFM4ZUOag93EG21r3KSGCx6hcGFoIqbdk1x6zOls/zWSc4WL1FXXE5pTYwjsXyk/n0osxVef9F/sUti+Xrsv+2XdZD2VZp2rNPW6s1iaobmPO+Pa+vCiScenua0Kmr46rVA/TGyhGVg6UOTdYSJmxBQ2F6EbDKc0TlkYGZxnzXUN4XWNqrsswWdisXSsSs0A/dqXQeUaUHc0hXeJ60g6UhW53ylS2tiFJlqQKy8jZlBb8JsjpD/nAAYizbsw+Ts7TsT4wq8mcos0DlpwlJl3GLDpbWPdercpsJCskgvMEOqTacn3xkuQbBygltYxJMnUwjVqrVHu56qg+59ZbCs8oMKXRTS4nSij9/rNxRPghTYLXYnhp3BivRBnlAQ6SVpmELopFBm8X1hOoMA1uumT5XgRSqR3Ku/0GYbrEQGOr2sIbCJsSrb+dnVGlHkPY7pqISt1i9S2lNgfTdWXkuSLtodMvyE7jEGfDdoWUTqHiuGce9NCG9nq/OYHGsZRbYe+1QHzPrMdYKorrvWC/VQUPco3y95Q40UNdYUndCf5JQxeJjiahCteQm3lP0ZLxsK90ZizFgb2VqXG/eCdd8VLj6V3azijuUvm57SwClPJKCRVGlqNzMVUwVenVSv6foGS00bSfs103BzKWhyOu2sEJrK/oUz7x3EexWvp443W5U1Q16spJskqiyNNWb0/hTUYV2WHsDTFuL+j7qtJbJvGvK0sFac3I1D03ae2FRdbbSHVVWkzpmtNu2IoAFUhaBXZuUGELXIw4Wd/r80O49L6hBaBX2Ejm1FuIqPCC2qk87QQ00VF1ucIVcRXxR/F8H64ipwopgS2LlrpQGlfl6YqwCf/KBtl9btyRPnpKldLCOTqinU+9LL4/yTFU+khKa9lzxHMrVBWtEnTvaPvxCaH9+UVypg3WEQj3diUGu9XltPBpmKfnqPxXfRS2d6ElY8KNAqrXUXxFX6mAdnZCczO8B1eLtRUjpz/GM2Zb/6DKleYRQViRzZdS92t3BWqN8spffAzY6W/4uymKJqu3Kcgrpk5W0jpl01BbTi3WuiqcGs7HMxYq9IUJ7of35RXGlDtaRyltTspRSbFjnSFkrYdDk/t2YNZWyyNlpTpCIqkdLrCvSEh0Haw074vEtR3mx/G6OKC8kAisuZbk5a4yiUCL0dV2Ug7UGwZ29PWWeGErwZZ3vrkpZdqsadLBSFC+wjhmv10VoCe2hVSpEPibiYImqncrcmeKkzgUwGKr3Zj0aJNqQtOq4seVgUZap+6cHza1baEPaKtp5nMTBYhZPQZIp73irHKxV5fWN9Ba+s36LRRvSVr3uFut4CYHRrkXfFoArxlqn0IakVbTTwTqGbB1MyQuUFrYzuLt0d+0D2U7q9VYTzmBZU9XxNT0xmlbRNlHlYH3rxKhCjS2kvJ1VGQWjCjW2HlxxsCx1Lm2Sz/Z1DK/bnu3BFQeLJKdlz634rs1hJEXLc8+m/MmDKw4WEQ+VLRcqfpam/IBpe2Ba4o8zcB6OafVQAgfLhXkbgcVrFwerz6LQWzNZtW+L/I9dOhACAABgIOQPNbW/iRRDYiEWiIVYiAViIRZiIRaIhViIBWIhFmKBWIhVbTs75/3SyQ5F8f92baBYwIYigoL1a0OxY0exK7qCqDwsWMGCIPbeFUWsSN6BwGHInYTvQxf2yZwflnFy0yaf3HsTWX+Hp+npaVbc2NjQLxcWFpRFKNI2m5ubyqKnpyeYdXV11dXV1dTUtLe3o5fb21vr/8d5eBgbG0Ob+BfPyin0qwcwOzur/PT+/r66ujo4ONjc3FxdXd3Q0IABjIyMLC8vX1xc4OMoi05PTycmJlpbW3Wt7u7ulZUVtGb9u0xbW/yM6+vryk+Pj4/aYGZm5n8P1vPz86+wFRcXx4r5+fn6ZUpKirIIRdqmvLxcCb28vGAVo6OjZUeRkZFYsPv7eyXU2dlJs7KyMmXX9fV1VFQUjY+OjowdNTo6ihk55ltbW6uE0E5BQYGvfXx8PNr8/PxUQklJSTTDqM7Pz5XQ2tqa8Z3/swKw7u7uMjIy3N1hnQ4PD82/b9rW5rXZ3d1VFjU1NXktt7e3lUctLS2Orm3DhifjTrCpuLj47e3NqEiCafPDwcL2MkIhtinnD1cvQ+HXwYK3yM3NZS8xMTH19fXj4+MILvBhCQkJLEpMTESsdIBVWlpqc1dwezaw9vf3vd6xqqoKHwHhcmpqCtPs6elBdCsqKhoYGFAenZyceKlKTU1FBJ+cnERQrqys9HaH6m6woKWlpZ8MltT8/LxcDOpbwMISsousrCxAYIRIxDgadHR0OMCi03K7K2MuoIfvHTmioZKSEtZCTvbx8aE8Ojg4wDbQpRERETs7O26wkpOTX19fA7C+EywEAnqLs7MzJYQvzqQkNjaWS0iwHE6L7soB1tDQkMy93ELsBi66Sk5Ojm8ihayczTY2NvqC5R1Yb29vANa3gQVKmFNLJijEIw5jb29PgoUV4krTPdBd0UbOhXOky7y8vGSR44TLKkwJpNLS0rRNenq6L1iIm4yneGAWH4BlgoUU+x+LUCTBgjuRW1ZqcXGRZniWYIFa5Eb6ORQKGe6KYdSYCz0iwxYPobibcNwveKOnPFJQGBLb9AUL9PT19bEphFcJVgBWWCJYTIH5HodzZRG/MoQh+YKF7Io2dFp0V9nZ2bijknPhxRKCLEuZjw8PDyPqKaH+/n6a3dzcKCF52LSBhTMjOqIZTpp/F1gBWPixsLCQTstwV3Nzc2jEMRfwgRxcptWI1KDTuEWDc6WB4/6Ww3OAhR818ZwIUAvAMsHCZUHIIhT9abDwCwDvaAEES5Ffu8Hi5TtO/hUVFTrzo3B68B4sGL/cYOGCJhywIPRISzQegPXV5P3q6ortI74oixAg5I2ABAtZEUKefpOZmUl3hVsxlLrBkr9RwXi4GaC8vDyWYg/w/fHxsbLoX/bunzWOK4oC+BeWQJUqgRASSF0qgdKpFBiXbuzKqVwY7MaR0FdIo0adYPLDA4fNe7uXXU3IBuudwtirmdk3T2fun3PvHd/c3ERxqInFXh4cHCSKl0AMYi0iFrOfbI6uOHXoFYHHx8dNxIIvX740vuzo6Eh4vhOxAlYqOQck3uJYt5G+5JiRqWpigaLkqmiylFhDx7q8vIwbXVtI5sUUfPI0Y0lBLAcnFm4M4U7ECm5vb/sEUE26T+WCXtCXZhbEivLCyuYUZfhBrEXE4qfyFSonpPaGVWLqHKDa48OCWKAWlOND1lcTS425t1iwWoZibJqzBPsnJyc5QHheECu4v78varK7YRDLkxohcfYaGlf8JijXnz59Ojs7y49EIRK9glgJwFNhFD7n84JYJC6VPiVCIhkFiwarJmMBynw55fT0tCFBnDjgn9rijx8/vn379u7dO/63qTHXxAoUZwexlhIrEP8mlOkRJ5jnviYWIAexnhOMuaqJVXxvFM6+cerjx49+VIMTlwdsT6ynp6coaoNYi4gViZwk0f9iIm8yIRMUxCpRE6vufmF+ols20NCXkK7novjs+fl5CmpidbFBihm/ILFEqTo5xZ6CGw/TtAGfP392DEjfisxuPqZoiRQdO4yoI4JR3JUcMTxk8aLUM18zPS0FCE7zvXA3jeApvfcIkT39lKxwfn4uQrIGd60YlbAvaFw598eZcnnWfHV1pZLDmBWKvBbTeRkJ2pqw0ibMS/WnDPQXJNbA6HkfGBjEGhjEGhjEGhgYxBoYxJIAE8GVVq6vr6XTkmpVLXI59U9yTq3Rnlvk5BpR1PmdpUPXWUCX8k8FHOm03JuM2asS2nanDaB8zsfMbQtgAb9vjTS2z7UXbSoauRSMLWy+qVk1MMThlpsaM5GWsuAipHaHKQzMZ9Em3KOuB4JcMQ/88PBA4qfYXVxcUDRcgUihI15Lqp4fNYO3RSwKUKEfRsejZk0d1DfK81qdMDUcomuhtTbHpGS7DdLRRUbKmMYmWM8UZHmlRq8PTKW8n5Ymj9Xnths4iBXEzMQepCmqgLrbHoiVQeoSTNFOxEp9kJlf7e5KW30B1ca3SyyPo45yBRaPoDZzNQ2WXDk2Fb34taZBj4bOB/3VgULNRywklobBP/+Jw8PD/I6bHxn4ns9KVyC7pc1L91W/vKYmk+VxnUoC9sFNqXVyZGrnqxXPFBiaVmZfyjKpKTlXa40SpMnKDx8+mM71ydslljCiLm+pgeRzk8H5PK29BV5NrKIex5hNGxA/KNSbYPHy3GPKjgpT+VwkOn+o7aKZuK8wiOWx7qe4mhZeF9k3sepjlhMrHGrbbDLl4RtjLysMYmUQfhArjYE9sSSSq0GbEZKpxiBWBIXeFYZYiUy/roNoY+/Ecp2vG5DXkNTLS5AututdoRHnzEqAkFTkR8jI6wKmQSwPnxjTTglsPXkCWFOd2c2mbz3EqvPz/RKrBoVp7fJoB/bBDtgHuyGPoaWtNq2n3SUCmF3qNRqZqchsEKtCBq12Ihb8n4nlFl4hN5BAV1PdyGbUYL3XOSwGTAsX0ziItQbHx8cRqdcSS7fn+3VgEvZOLPHQ+w2gCOxELDYbewofh3CkDeWKxoApSzD2b5dYdlZB47efyBBEo57/K8G7okpNLJBt7St4JxzYB2Uf+5AJNvC+hmk7yHiM9yT2yujHCN4nHb2RbZTYPKbLicUI5Qne9MRn3MCvdr9ZYWqpQq6EjKlFbgMTQVxhe8sjK9RsXiSM3NyuxPLEJ/JYe4qQuR1G3Texwo8M4yfA2gaq0e3cxCCWgnwcoqBBfNoMWez0srzm1SuaKV5eXpqvi1CU1xW9mjTiwkz3LyRW89KivPG7QKx+XkCi5WEQqx+ran1TfhRd5491kKWnF2B2K0Lp1ZBOxw62ff/+3Vfn4Z6DMIZhCbGYljwSyudrlyfQ3pJY0jqBV97Du1pkVEzUIWMHiDX6gsxqu7I/hfkhd7u3g1jAtDStColPk/sUaGZBiUPF/Greipb5qlcTS+m3+IrUjLchVtrC+vfw5gGr4cptGXEQywHJboiE8V/zXotntydWLsg9JWppBFXjfsnMlxCLpcwrGHpECN2eWCwoK9hH8SKwYhPcpkW+RR1Lukf5FIlD/98oNP/rCcQLZMqZo6FjiUJwAvzl7u6OSuSyWmtETpsIjZe06duf0HspdqkpFRC+58XU7//wDHCyXJIlAVeuL8hfrE0bjG9vQkOzqfNlGaFNMVP2YfX1pGrPqhQ8oHSHrGBa1T6waj5hekfP+8B/ib/bpQMBAAAAACD/10ZoMFZj1ViN1Vg1VmM1Vo3VWI1VYzVWY9VYjdVYBQInF8S0j+DtAAAAAElFTkSuQmCC</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>Verify that imageUrl is not returned in Get User Profile API once media image is deleted using Vanilla API</t>
+  </si>
+  <si>
+    <t>Verify that user media image is deleted using Vanilla Profile API</t>
+  </si>
+  <si>
+    <t>OPQA-3176</t>
+  </si>
+  <si>
+    <t>OPQA-3177</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||onboarded=true||discoverable=true</t>
+  </si>
+  <si>
+    <t>truid=(SYS_USER1)||active=false||deleted=false||onboarded=false||discoverable=false</t>
+  </si>
+  <si>
+    <t>truid=(SYS_USER1)||firstName=Project||lastName=Neon1||title=Project Neon1||primaryInstitution=Thomson Reuters||location=India||summary=I am test user for API Automation||active=true||deleted=false||onboarded=false||discoverable=false</t>
+  </si>
+  <si>
+    <t>truid=(SYS_USER1)||active=true||deleted=false||onboarded=false||discoverable=false</t>
+  </si>
+  <si>
+    <t>{"onboarded": true}</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "onboarded": false}</t>
+  </si>
+  <si>
+    <t>{"active": false}</t>
+  </si>
+  <si>
+    <t>{"active": true}</t>
+  </si>
+  <si>
     <t>status=200||truid=(SYS_USER1)||onboarded=true</t>
   </si>
   <si>
-    <t>{"truid":"(SYS_USER1)", "onboarded": true}</t>
-  </si>
-  <si>
-    <t>Verify that for the existing active truid, update active status  using  updateUserStatus of Admin API works as expected.</t>
-  </si>
-  <si>
-    <t>/admin/users/user/(SYS_USER1)/status</t>
-  </si>
-  <si>
-    <t>status=200||truid=(SYS_USER1)||active=false||deleted=false||onboarded=false</t>
-  </si>
-  <si>
-    <t>status=200||truid=(SYS_USER1)||active=true||deleted=false||onboarded=false</t>
-  </si>
-  <si>
-    <t>{"truid": "(SYS_USER1)","active": true,"onboarded": false}</t>
+    <t>OPQA-2590_1</t>
+  </si>
+  <si>
+    <t>truid=(SYS_USER1)||active=true||deleted=false||onboarded=true||discoverable=true</t>
   </si>
   <si>
     <t>status=200||truid=(SYS_USER1)||onboarded=false</t>
   </si>
   <si>
-    <t>Verify that for the inactive user id, user profile is not returned and check the error status using Vanilla API</t>
-  </si>
-  <si>
-    <t>?id=(SYS_USER1),(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>status=200||firstName=Project||lastName=Neon2||location=India||truid=(SYS_USER2)||location=INdia||primaryInstitution=Thomson reuters||role=QA</t>
-  </si>
-  <si>
-    <t>Verify that inactive user is not able to edit  info like title,role,Institution and country using Vanilla API &amp; check the error status.</t>
-  </si>
-  <si>
-    <t>/users/user/(SYS_USER1)/media</t>
-  </si>
-  <si>
-    <t>Verify that for the given inactive user id, user media info is not returned and check the error status using Vanilla API</t>
-  </si>
-  <si>
-    <t>Verify that for the given inactive user id, user media image is not returned and check the error status using Vanilla API</t>
-  </si>
-  <si>
-    <t>Verify that for the given inactive user id, user image is not updated and check the error status using Vanilla API</t>
-  </si>
-  <si>
-    <t>/users/user/(SYS_USER1)/media/image</t>
-  </si>
-  <si>
-    <t>Verify that for the existing truid, Admin API doesn't allow to create same profile again and check the error status</t>
-  </si>
-  <si>
-    <t>/admin/users/user</t>
-  </si>
-  <si>
-    <t>Content-Type=application/json</t>
-  </si>
-  <si>
-    <t>/admin/users/user/(SYS_USER1)</t>
-  </si>
-  <si>
-    <t>truid=(SYS_USER1)||firstName=Project||lastName=Neon1||title=Project Neon1||primaryInstitution=Thomson Reuters||location=India||summary=I am test user for API Automation||active=true||deleted=false||onboarded=false</t>
-  </si>
-  <si>
-    <t>Verify that for the invalid user id, user profile is not returned using Admin API and check the error status</t>
-  </si>
-  <si>
-    <t>/admin/users/user/(SYS_USER1)1</t>
-  </si>
-  <si>
-    <t>truid=(SYS_USER1)||active=true||deleted=false||onboarded=false</t>
-  </si>
-  <si>
-    <t>status=200||truid=(SYS_USER1)||active=false||deleted=false||onboarded=true</t>
-  </si>
-  <si>
-    <t>Verify that for the existing truid, user status is updated using Admin updateUserStatus API</t>
-  </si>
-  <si>
-    <t>Verify that for the existing truid, user status is returned using Admin getUserStatus API</t>
-  </si>
-  <si>
-    <t>Verify that for the existing truid, user profile is returned using Admin getUser API</t>
-  </si>
-  <si>
-    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
-  </si>
-  <si>
-    <t>OPQA-2575</t>
-  </si>
-  <si>
-    <t>OPQA-2576</t>
-  </si>
-  <si>
-    <t>OPQA-2577</t>
-  </si>
-  <si>
-    <t>OPQA-2577_1</t>
-  </si>
-  <si>
-    <t>OPQA-2578</t>
-  </si>
-  <si>
-    <t>Verify that for the given inactive user id in the bulk list, user profile is not returned and check the bulk profiles in the response using Vanilla API</t>
-  </si>
-  <si>
-    <t>OPQA-2579</t>
-  </si>
-  <si>
-    <t>OPQA-2580</t>
-  </si>
-  <si>
-    <t>OPQA-2583</t>
-  </si>
-  <si>
-    <t>OPQA-2584</t>
-  </si>
-  <si>
-    <t>OPQA-2585</t>
-  </si>
-  <si>
-    <t>OPQA-2587</t>
-  </si>
-  <si>
-    <t>OPQA-2588</t>
-  </si>
-  <si>
-    <t>OPQA-2589</t>
-  </si>
-  <si>
-    <t>OPQA-2590</t>
-  </si>
-  <si>
-    <t>OPQA-2591</t>
-  </si>
-  <si>
-    <t>OPQA-2591_1</t>
-  </si>
-  <si>
-    <t>{"imageType": "png","imageHeight":97,"imageWidth":97,"imageContent":"data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg=="}</t>
-  </si>
-  <si>
-    <t>status=200||truid=(SYS_USER2)||mediaCategory=image-full</t>
-  </si>
-  <si>
-    <t>{"interest":["computers","science","API AUTOMATION"]}</t>
-  </si>
-  <si>
-    <t>{"active": true,"onboarded": false}</t>
-  </si>
-  <si>
-    <t>{"active": false,"onboarded": false}</t>
-  </si>
-  <si>
-    <t>{"active": false,"onboarded": true}</t>
-  </si>
-  <si>
-    <t>status=404||statusCode=404||errorMessage=User not found.</t>
-  </si>
-  <si>
-    <t>status=400||statusCode=400||errorMessage=TRUID is missing.</t>
-  </si>
-  <si>
-    <t>status=413||statusCode=413||errorMessage=Too many TRUIDs provided.</t>
-  </si>
-  <si>
-    <t>status=400||statusCode=400||errorMessage=Image Content not set</t>
-  </si>
-  <si>
-    <t>status=400||statusCode=400||errorMessage=Image Type not set.</t>
-  </si>
-  <si>
-    <t>status=404||statusCode=404||errorMessage=Media not found.</t>
-  </si>
-  <si>
-    <t>status=409||statusCode=409||errorMessage=User already exists.</t>
-  </si>
-  <si>
-    <t>status=200||interest=computers||interest=science||interest=API AUTOMATION</t>
-  </si>
-  <si>
-    <t>OPQA-2679</t>
-  </si>
-  <si>
-    <t>Verify that user is able to edit first name and last name from his own profile page.</t>
-  </si>
-  <si>
-    <t>{"firstName":"ProjectEdited","lastName":"Neon1Edited"}</t>
-  </si>
-  <si>
-    <t>status=200||firstName=ProjectEdited||lastName=Neon1Edited||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
-  </si>
-  <si>
-    <t>status=200||firstName=ProjectEdited||lastName=Neon1Edited</t>
-  </si>
-  <si>
-    <t>OPQA-2679_1</t>
-  </si>
-  <si>
-    <t>{"firstName":"Project","lastName":"Neon1"}</t>
-  </si>
-  <si>
-    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA||title=Project Neon1||interest=API AUTOMATION</t>
-  </si>
-  <si>
-    <t>{"location":"India","primaryInstitution":"Thomson Reuters","role":"QA"}</t>
-  </si>
-  <si>
-    <t>status=200||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
-  </si>
-  <si>
-    <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA||interest=computers||title=Project Neon1</t>
-  </si>
-  <si>
-    <t>Verify that imageContent is returned for the truid using getUser API</t>
-  </si>
-  <si>
-    <t>?image=yes</t>
-  </si>
-  <si>
-    <t>/users/user/(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>OPQA-2957</t>
-  </si>
-  <si>
-    <t>OPQA-2957_1</t>
-  </si>
-  <si>
-    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg==</t>
-  </si>
-  <si>
-    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADICAIAAAAiOjnJAAAdqUlEQVR4AezSQREAAAgDIPsHtI6m2GN3kIG5AKiPhViIBWIhFmKBWIiFWCAWYiEWiIVYiAViIRZisc/e2W3HURxxfB9hHmEfYR9hH2EfQY+wb7BAQvwleSXLGINxRAgmEMwROBBC+JBJbDAfiRPyTTjHEC4SckNyldx1fse1/E+7e6YzszvSWrjq1NFZ7Y5GPT2/raquru7ZC7dm/AwuvYHl8v4s7AwWymukJC4O1j9vh8vDsD3gJ69Dk9gxprxufzYH6wEVCJgPFnqhCk3y4liHhWdHoUk4gw7jzA7WgytnB7GWTNFTQw7gJ6/bn83BelDlx2NxADRhRTH4dDYH69spfzsIr0xAh5/hq9uNpogDtgb85HUPEdszo/LZaIlaRQsdrGNI1eZAGnar8O87Ye1CG2hJ3LBjxpaDtT9Z3DnpO9OwdqENSatop4N1nOT5cTgziJV3vFUri4P1041wenCPfjwPaxfakLSKdh4ncbD++3V4eqT7x2ve6XlY8PIk/HV/Da1ysNbP1u/2wo1Z4GdXeXcatu+mTD/bzwPwFaNvtep+pcrB+mQvvDUNr23wos+bBDqWPT97N3GQyM0ZPClI4tcabp4bB/TT/SUviiviunixBnGwXpqEk4Mg/X53t8LxMFQLlvKcOVjESYaUuTNsTywAoSadGIRfzrq1h6uIL4prPFJxsD6c0++pvtolEL49Dzt3J5V/XRfU/2oezlfhkiZwGuKkvYxmIWU6r0J7of35RXGlRycO1pWxbt6Sd/HqGKo099xZvjgIaC5xe753V9sL7c8viitdszhYaHu5NlkEUozvepQLwwBM0mfvxeK3e+HdWUA/L0DpYK1R3pxy21K9OukW0ODv3pv1PDT7x+1wtgo05tFBOD8M/Gryn6/DpVH47iBIr6WOm/bnF4V/dLCOUP51x+6flF91FxOA1lBzh0FCY/n5NAip7yxUxwjK/KK4UgfryNl6cYJhQHlRTxVZqMcpvuOA/hzKX/YDDg79yUbADrWU3aGQkuITc4MXX9R9SZUnSFX5aYmDL7tkMslOUYZwriK5kMbsZkvs3oNXSzlTpVQ9Qni34QnSNRsncy4yS22FwNyo2hp0cIiUTG1+k6k6NeDXezICogrFCMVNooXXZwH9zV5WUTiJkTLlsE7Rm3VCH2bMwcLXEOTGMe8Pxx3wIsCyqrrf73WbChRVKFYqBiumKgYLSkTMw4PwwiTFAqPFR9InR+2R4qqTwJ+ecbBWEHVorJtVb936hz2Wc5FqT3HcqRZUkVvi19gmCSk0huN0JaoW+qf9EMvXdwK+7wdjFKvGJSzefHkjnKoCxz8x0p9IOIzrzTuBnnGwuotsgNxHonxlVxdy7pbKeqzKnS9zNUzI1PidP++TOOBm491ivlOqUOgpC1QZUrEm/pErbeoEjuwuDlaxT3eHTXkpzE+3HKkisBXldIYI5qco2CodLAW1mFeutO9vl4P1zDjvTWlK1TMjlbIo3C4LyQijir/9/6bl1hwLUXLB2CfBYX7N5O+3w/OT8BATfxUkxWeQuUr1zkGQFHqA/nGwlhHSPC37lNgcnlTN8vpG+wqZUkGVyMAaCRcjg59QAivbw/D+XL57EUL9bLo4jL/lGKiSXhyJrRwpOwawWn273pg6WB1Fd1RjqEQVXqgESgVSK9b7Mp3HVAzKCxMi7jh4un33/afHMS6NXs9sVaKcwYSRo3iKFQMp0WAzV/rHweos8i95h2IS8gDrieGilGW7kitM62QYAxaFUN3SVJYlZ5yv2y8CsE/c+BQFOKsVmatYD2bBBMuUf4q1S4TrzTuBnllSHCyNwhjVW2+eGzZ2KGyRJb+hcVxKlRXJlPPvpKwElubyaIDAAhSoysHCMpmJBQtUvgzHVwALwdThTEtU6QvGtSsBRpMQB2v9osxCPvrDvIlFop+tysAinwlAMi2WUtc7uSvkI7BLA3AYeqjk6eT0OV6oEb1xfgF6v4qDpTFgbq7emVqGXQXmQGYlU+X8Pgja7UdBQQwJLM0DcpiQgjwCrHICouAZHawVRGMrjcIKwQTGBue1SkHVucrAYu1Dow+iMVACSeYWKTr4RV2TiL1EFWpDNhkkPgUpTqL8BdaI9yWpeSuODGgVPWP/iObRYw5W95yhBvkN6w7mFXgtvzQZqjgJiyBkirjlKAIKcRqdjwi88JKP1pWi86lu9ulK0JTNEiODcqSvkUH6XxLlnA5W2xyjNJ/Tfc3WHSxT7Z4C+tEcPyhDorvLrTITogbgHAWWGS1W0WDwoFN3HeNBKpXz2NlIjqOUcMWGTcSkMz96P9PCF684g+RgFTLR0jjmhaRk2YKMljKfJBe6TtQkzkjxuIJxHBxsMQEMQwj/+hT2Kcv1azZGIAKlon5RJV9WBmt7KO4L/UPvOVgN6dBCryVTb/hBIWVK0B3boQuVVWJpFbw+ovov35gvNyeoPKOYTsXc8d6ovjrZqJKFi8F6OAVLH+UqN0dLOL7td8/BattruBgJzkVIoQTUsTD6U30ftaB53oH32XlBYmMFG7Ip8wRkLasCNa20de8OpWcqowqVQcVXNpYzJPM/GkgCd/a3xUlGB0tS9gXJDJrYujqhONiMQWqWqIThNm9mFgsXaR/p/c8joLEZdoOX+OoTafHvoJn/Hhfo0cIP5kkoKaevbILYog1x3lVUKVNfUneF5eFSKc5oH5UzuyxzUnbBmgrkRi4t/K8XxuFg2t5Cl5JkDZ8qTV/ymA5WKhqUlc1V70JIjgnZGR7itC6gd0y54ZcB3VLw9EzZaNlck4NVZEu+QLZKVCk53nFhRaGWXIWgfW5Ww/iAjZDiBs/v1jrvVGJL15svQqQ9CvXEjaDnRWq36LEyVQ6W+o4xIF9Z9Wb9ys9Lo/Z4cb/TKZ3z36z1g60ehUJWIi3mvCXYqpOLxAQOOq+9VgqjlILHpuZdhK5qZX2uMKFKNcot5WKVVjectfnmvsHCJlEhzdRkbLEMrHMVr2WrRJVdkWL81CCtOuhzsPjKKrAgFOV1IkIqVubv8k0+357WbC9zeYjdStc0axX1oQo8keIXVUp01ea6xFMxm0D/2EQ4PUZypNmhex4rj9wJNTD15QJwRu+6eUaVTf99ur/mjSq/bI7WZbFEFSqLpdnARJvCLMVhnsfKgyp1UCFDmK9SR2WxCF+MqlZblmHSnhsf4naMT/L4E+0Z0VzUL6qeiibaiZxyqpSg5zB9A3MVfA6WZjPKGRpN1ZXWE++p5EHRTEPOyRA8MThEsLYIyUfJ/5UN08gUj6xRYWHNj7BTtq9YCuFglc2VjJYEtqLid7o7r1bQQtPSCJE4GrAeHx5iUHXz3kWO/Apqj1W82TLzwrARwhIHV+goGS0Hq5D0K5Xz8hVvG6tq4pk7ynRefOM/VjR9JEJefkt19z1/CVdPJjtY3YUbaRPP3NojE7weKzs0I2nvsD3JGxudN3ADptiMOVjts+0dXCGG6tYcByEf0cpiEesAVmyxKJu5qRt/CGKp9jOq52leF/TqBnWLYJdapnPDWqdPb/T0JfTg/WCm7k6LARXXCzsG7SSEWG5aFpwjqJ2rDhGsk801gHLHJ74Zw25Hsz1che1dI9VODcrLe/C+0vRzsiZ9Z1gqyeWwyyNtXqU70bgjyNnDdI6YIsYQyqWVd6s/hUazPSRQYqSk6Uxiy6loryDN++tpuYDmSkBtv4GtElVaylyOvdYrGDNRdTpymtcbNq1AxBY9U04mO1gJXph6U3VTCay4wA0PKKrybYmxBzdkQg5ToHmzoiW447TA8EpWxExy5OKQR12w/UQ+2yO17eba95WDtULtcvxN1X4eMVVnopQ999X2CzkZBT1WqfzKpOet3pnStnw6NdPxWGFO2qx1SEfiV0iZkqZfVRws5jTsi6hFnppEawrtVf4gqlRLrm1FbbYnnsbZHhBpUYzQ/35xoEBZjsTYgu/um69iq6Aqn623LqKvHKySNE2valm6Pi3V46p0TjhKcDeAxbqa+KM/7oVrfVosjUxB4ZCyr/RGMtChT9wVFkTLVIrLzKMvK87x/rKypyrNFh/ef2kcD4otB6t9NouOqwVRy+EbP23Z3URauxUR9EqNt+DvkXsHDV81eEBys2Ro+bST0A/dMlgOFqao/UxF4hN5LZOmbfiakqhvTomsCVziUZvN+XR+przwpfHPT/LCKaYjbU1Yuj4WgnkfPZ/NSXMqHqayVVFIwzi309zXCrV+vmBV2dQCeao5Sf5WK121tZruxPUpE3nE+IuE+BftJrlBVgYVsi8SxlVaKqiKBsBi+Jk//9c+StNpz45tRGkas8VV+ILVzgIuLXqtWJCkvIN2QZLKTXyoJGpzBnWnsoquxi+AdmDLB6d5ChQny8RzMj6AYGzVWa2cjnJgQgplwueChpa+xL67FGZspDIhhUWb9WBpK0ezRngZPVciFw5QYsJ+xWlqn2bMks4px1Rekt9+1ZD2qjxhmoJFD5T6h95LxMEqlORqKXqrADbd4yAbVGrPPjIC2jFb20Bqm78fjdkxS9l8bUkaO1lMFDClE5r8/EhboS4lkCSqtHGXhH4obpriYLXfIiuNvjE/5WX4Oo9FPxBQKnjS+vpTNTO4xGSApQf42ObYcs3amy99YDgGDzSXnhGirpWToK/Jh5b3ptNMvINVjuLpO9wZ+sKEX8uFgW2dEZZJ2fyk0Dk2QrnAFnYrfsrX9eZ895WxVctQkHO4XUTPWBfRV+oiB6v/7DM+ov2OavJcgPVwBhY/7eSE/OBY3iqc2IuViVg+BUnbFWDlKbH8EdTrFweLO6eJGo0iMVFmhHgtr4TqsIKFM4ZUOag93EG21r3KSGCx6hcGFoIqbdk1x6zOls/zWSc4WL1FXXE5pTYwjsXyk/n0osxVef9F/sUti+Xrsv+2XdZD2VZp2rNPW6s1iaobmPO+Pa+vCiScenua0Kmr46rVA/TGyhGVg6UOTdYSJmxBQ2F6EbDKc0TlkYGZxnzXUN4XWNqrsswWdisXSsSs0A/dqXQeUaUHc0hXeJ60g6UhW53ylS2tiFJlqQKy8jZlBb8JsjpD/nAAYizbsw+Ts7TsT4wq8mcos0DlpwlJl3GLDpbWPdercpsJCskgvMEOqTacn3xkuQbBygltYxJMnUwjVqrVHu56qg+59ZbCs8oMKXRTS4nSij9/rNxRPghTYLXYnhp3BivRBnlAQ6SVpmELopFBm8X1hOoMA1uumT5XgRSqR3Ku/0GYbrEQGOr2sIbCJsSrb+dnVGlHkPY7pqISt1i9S2lNgfTdWXkuSLtodMvyE7jEGfDdoWUTqHiuGce9NCG9nq/OYHGsZRbYe+1QHzPrMdYKorrvWC/VQUPco3y95Q40UNdYUndCf5JQxeJjiahCteQm3lP0ZLxsK90ZizFgb2VqXG/eCdd8VLj6V3azijuUvm57SwClPJKCRVGlqNzMVUwVenVSv6foGS00bSfs103BzKWhyOu2sEJrK/oUz7x3EexWvp443W5U1Q16spJskqiyNNWb0/hTUYV2WHsDTFuL+j7qtJbJvGvK0sFac3I1D03ae2FRdbbSHVVWkzpmtNu2IoAFUhaBXZuUGELXIw4Wd/r80O49L6hBaBX2Ejm1FuIqPCC2qk87QQ00VF1ucIVcRXxR/F8H64ipwopgS2LlrpQGlfl6YqwCf/KBtl9btyRPnpKldLCOTqinU+9LL4/yTFU+khKa9lzxHMrVBWtEnTvaPvxCaH9+UVypg3WEQj3diUGu9XltPBpmKfnqPxXfRS2d6ElY8KNAqrXUXxFX6mAdnZCczO8B1eLtRUjpz/GM2Zb/6DKleYRQViRzZdS92t3BWqN8spffAzY6W/4uymKJqu3Kcgrpk5W0jpl01BbTi3WuiqcGs7HMxYq9IUJ7of35RXGlDtaRyltTspRSbFjnSFkrYdDk/t2YNZWyyNlpTpCIqkdLrCvSEh0Haw074vEtR3mx/G6OKC8kAisuZbk5a4yiUCL0dV2Ug7UGwZ29PWWeGErwZZ3vrkpZdqsadLBSFC+wjhmv10VoCe2hVSpEPibiYImqncrcmeKkzgUwGKr3Zj0aJNqQtOq4seVgUZap+6cHza1baEPaKtp5nMTBYhZPQZIp73irHKxV5fWN9Ba+s36LRRvSVr3uFut4CYHRrkXfFoArxlqn0IakVbTTwTqGbB1MyQuUFrYzuLt0d+0D2U7q9VYTzmBZU9XxNT0xmlbRNlHlYH3rxKhCjS2kvJ1VGQWjCjW2HlxxsCx1Lm2Sz/Z1DK/bnu3BFQeLJKdlz634rs1hJEXLc8+m/MmDKw4WEQ+VLRcqfpam/IBpe2Ba4o8zcB6OafVQAgfLhXkbgcVrFwerz6LQWzNZtW+L/I9dOhACAABgIOQPNbW/iRRDYiEWiIVYiAViIRZiIRaIhViIBWIhFmKBWIhVbTs75/3SyQ5F8f92baBYwIYigoL1a0OxY0exK7qCqDwsWMGCIPbeFUWsSN6BwGHInYTvQxf2yZwflnFy0yaf3HsTWX+Hp+npaVbc2NjQLxcWFpRFKNI2m5ubyqKnpyeYdXV11dXV1dTUtLe3o5fb21vr/8d5eBgbG0Ob+BfPyin0qwcwOzur/PT+/r66ujo4ONjc3FxdXd3Q0IABjIyMLC8vX1xc4OMoi05PTycmJlpbW3Wt7u7ulZUVtGb9u0xbW/yM6+vryk+Pj4/aYGZm5n8P1vPz86+wFRcXx4r5+fn6ZUpKirIIRdqmvLxcCb28vGAVo6OjZUeRkZFYsPv7eyXU2dlJs7KyMmXX9fV1VFQUjY+OjowdNTo6ihk55ltbW6uE0E5BQYGvfXx8PNr8/PxUQklJSTTDqM7Pz5XQ2tqa8Z3/swKw7u7uMjIy3N1hnQ4PD82/b9rW5rXZ3d1VFjU1NXktt7e3lUctLS2Orm3DhifjTrCpuLj47e3NqEiCafPDwcL2MkIhtinnD1cvQ+HXwYK3yM3NZS8xMTH19fXj4+MILvBhCQkJLEpMTESsdIBVWlpqc1dwezaw9vf3vd6xqqoKHwHhcmpqCtPs6elBdCsqKhoYGFAenZyceKlKTU1FBJ+cnERQrqys9HaH6m6woKWlpZ8MltT8/LxcDOpbwMISsousrCxAYIRIxDgadHR0OMCi03K7K2MuoIfvHTmioZKSEtZCTvbx8aE8Ojg4wDbQpRERETs7O26wkpOTX19fA7C+EywEAnqLs7MzJYQvzqQkNjaWS0iwHE6L7soB1tDQkMy93ELsBi66Sk5Ojm8ihayczTY2NvqC5R1Yb29vANa3gQVKmFNLJijEIw5jb29PgoUV4krTPdBd0UbOhXOky7y8vGSR44TLKkwJpNLS0rRNenq6L1iIm4yneGAWH4BlgoUU+x+LUCTBgjuRW1ZqcXGRZniWYIFa5Eb6ORQKGe6KYdSYCz0iwxYPobibcNwveKOnPFJQGBLb9AUL9PT19bEphFcJVgBWWCJYTIH5HodzZRG/MoQh+YKF7Io2dFp0V9nZ2bijknPhxRKCLEuZjw8PDyPqKaH+/n6a3dzcKCF52LSBhTMjOqIZTpp/F1gBWPixsLCQTstwV3Nzc2jEMRfwgRxcptWI1KDTuEWDc6WB4/6Ww3OAhR818ZwIUAvAMsHCZUHIIhT9abDwCwDvaAEES5Ffu8Hi5TtO/hUVFTrzo3B68B4sGL/cYOGCJhywIPRISzQegPXV5P3q6ortI74oixAg5I2ABAtZEUKefpOZmUl3hVsxlLrBkr9RwXi4GaC8vDyWYg/w/fHxsbLoX/bunzWOK4oC+BeWQJUqgRASSF0qgdKpFBiXbuzKqVwY7MaR0FdIo0adYPLDA4fNe7uXXU3IBuudwtirmdk3T2fun3PvHd/c3ERxqInFXh4cHCSKl0AMYi0iFrOfbI6uOHXoFYHHx8dNxIIvX740vuzo6Eh4vhOxAlYqOQck3uJYt5G+5JiRqWpigaLkqmiylFhDx7q8vIwbXVtI5sUUfPI0Y0lBLAcnFm4M4U7ECm5vb/sEUE26T+WCXtCXZhbEivLCyuYUZfhBrEXE4qfyFSonpPaGVWLqHKDa48OCWKAWlOND1lcTS425t1iwWoZibJqzBPsnJyc5QHheECu4v78varK7YRDLkxohcfYaGlf8JijXnz59Ojs7y49EIRK9glgJwFNhFD7n84JYJC6VPiVCIhkFiwarJmMBynw55fT0tCFBnDjgn9rijx8/vn379u7dO/63qTHXxAoUZwexlhIrEP8mlOkRJ5jnviYWIAexnhOMuaqJVXxvFM6+cerjx49+VIMTlwdsT6ynp6coaoNYi4gViZwk0f9iIm8yIRMUxCpRE6vufmF+ols20NCXkK7novjs+fl5CmpidbFBihm/ILFEqTo5xZ6CGw/TtAGfP392DEjfisxuPqZoiRQdO4yoI4JR3JUcMTxk8aLUM18zPS0FCE7zvXA3jeApvfcIkT39lKxwfn4uQrIGd60YlbAvaFw598eZcnnWfHV1pZLDmBWKvBbTeRkJ2pqw0ibMS/WnDPQXJNbA6HkfGBjEGhjEGhjEGhgYxBoYxJIAE8GVVq6vr6XTkmpVLXI59U9yTq3Rnlvk5BpR1PmdpUPXWUCX8k8FHOm03JuM2asS2nanDaB8zsfMbQtgAb9vjTS2z7UXbSoauRSMLWy+qVk1MMThlpsaM5GWsuAipHaHKQzMZ9Em3KOuB4JcMQ/88PBA4qfYXVxcUDRcgUihI15Lqp4fNYO3RSwKUKEfRsejZk0d1DfK81qdMDUcomuhtTbHpGS7DdLRRUbKmMYmWM8UZHmlRq8PTKW8n5Ymj9Xnths4iBXEzMQepCmqgLrbHoiVQeoSTNFOxEp9kJlf7e5KW30B1ca3SyyPo45yBRaPoDZzNQ2WXDk2Fb34taZBj4bOB/3VgULNRywklobBP/+Jw8PD/I6bHxn4ns9KVyC7pc1L91W/vKYmk+VxnUoC9sFNqXVyZGrnqxXPFBiaVmZfyjKpKTlXa40SpMnKDx8+mM71ydslljCiLm+pgeRzk8H5PK29BV5NrKIex5hNGxA/KNSbYPHy3GPKjgpT+VwkOn+o7aKZuK8wiOWx7qe4mhZeF9k3sepjlhMrHGrbbDLl4RtjLysMYmUQfhArjYE9sSSSq0GbEZKpxiBWBIXeFYZYiUy/roNoY+/Ecp2vG5DXkNTLS5AututdoRHnzEqAkFTkR8jI6wKmQSwPnxjTTglsPXkCWFOd2c2mbz3EqvPz/RKrBoVp7fJoB/bBDtgHuyGPoaWtNq2n3SUCmF3qNRqZqchsEKtCBq12Ihb8n4nlFl4hN5BAV1PdyGbUYL3XOSwGTAsX0ziItQbHx8cRqdcSS7fn+3VgEvZOLPHQ+w2gCOxELDYbewofh3CkDeWKxoApSzD2b5dYdlZB47efyBBEo57/K8G7okpNLJBt7St4JxzYB2Uf+5AJNvC+hmk7yHiM9yT2yujHCN4nHb2RbZTYPKbLicUI5Qne9MRn3MCvdr9ZYWqpQq6EjKlFbgMTQVxhe8sjK9RsXiSM3NyuxPLEJ/JYe4qQuR1G3Texwo8M4yfA2gaq0e3cxCCWgnwcoqBBfNoMWez0srzm1SuaKV5eXpqvi1CU1xW9mjTiwkz3LyRW89KivPG7QKx+XkCi5WEQqx+ran1TfhRd5491kKWnF2B2K0Lp1ZBOxw62ff/+3Vfn4Z6DMIZhCbGYljwSyudrlyfQ3pJY0jqBV97Du1pkVEzUIWMHiDX6gsxqu7I/hfkhd7u3g1jAtDStColPk/sUaGZBiUPF/Greipb5qlcTS+m3+IrUjLchVtrC+vfw5gGr4cptGXEQywHJboiE8V/zXotntydWLsg9JWppBFXjfsnMlxCLpcwrGHpECN2eWCwoK9hH8SKwYhPcpkW+RR1Lukf5FIlD/98oNP/rCcQLZMqZo6FjiUJwAvzl7u6OSuSyWmtETpsIjZe06duf0HspdqkpFRC+58XU7//wDHCyXJIlAVeuL8hfrE0bjG9vQkOzqfNlGaFNMVP2YfX1pGrPqhQ8oHSHrGBa1T6waj5hekfP+8B/ib/bpQMBAAAAACD/10ZoMFZj1ViN1Vg1VmM1Vo3VWI1VYzVWY9VYjdVYBQInF8S0j+DtAAAAAElFTkSuQmCC</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>Verify that imageUrl is not returned in Get User Profile API once media image is deleted using Vanilla API</t>
-  </si>
-  <si>
-    <t>Verify that user media image is deleted using Vanilla Profile API</t>
-  </si>
-  <si>
-    <t>OPQA-3176</t>
-  </si>
-  <si>
-    <t>OPQA-3177</t>
-  </si>
-  <si>
-    <t>X-1P-User=(SYS_USER2)</t>
+    <t>status=200||truid=(SYS_USER1)||active.userState=false||deleted.userState=false||onboarded.userState=false||discoverable.userState=false</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||active.userState=true||deleted.userState=false||onboarded.userState=false||discoverable.userState=false</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||active.userState=false||deleted.userState=false||onboarded.userState=true||discoverable.userState=false</t>
+  </si>
+  <si>
+    <t>Verify that for the given truid, on changing active status, discoverable status also changed accordingly using  updateUserStatus of Admin API.</t>
+  </si>
+  <si>
+    <t>OPQA-2576_1</t>
+  </si>
+  <si>
+    <t>OPQA-3288</t>
+  </si>
+  <si>
+    <t>Verify that for the existing truid, on changing the onboarding status, discoverable status also updated accordingly using Vanilla update onboarding user API</t>
+  </si>
+  <si>
+    <t>OPQA-3289</t>
   </si>
 </sst>
 </file>
@@ -977,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I34" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L38"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1084,16 +1114,16 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="8" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1109,11 +1139,11 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="7" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -1137,19 +1167,19 @@
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
       <c r="I5" s="8" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="8" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1165,11 +1195,11 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="4" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -1194,7 +1224,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -1219,7 +1249,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="K8" s="1"/>
     </row>
@@ -1243,10 +1273,10 @@
         <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="31.5">
@@ -1269,10 +1299,10 @@
         <v>20</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="18" customFormat="1" ht="31.5">
@@ -1350,7 +1380,7 @@
       </c>
       <c r="H13"/>
       <c r="J13" s="5" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5">
@@ -1374,7 +1404,7 @@
       </c>
       <c r="H14"/>
       <c r="J14" s="5" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45">
@@ -1402,7 +1432,7 @@
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="7" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="K15" s="1"/>
     </row>
@@ -1429,7 +1459,7 @@
         <v>36</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="255">
@@ -1452,45 +1482,45 @@
         <v>30</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="210.75">
       <c r="A18" s="8" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="8" t="s">
         <v>72</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="32.25">
       <c r="A19" s="8" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1499,10 +1529,10 @@
         <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F19" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="7"/>
@@ -1515,16 +1545,16 @@
     </row>
     <row r="20" spans="1:12" ht="32.25">
       <c r="A20" s="8" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
@@ -1532,10 +1562,10 @@
       <c r="G20" s="20"/>
       <c r="H20" s="7"/>
       <c r="I20" s="8" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="240">
@@ -1561,34 +1591,34 @@
         <v>41</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="210.75">
       <c r="A22" s="8" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="8" t="s">
         <v>79</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="31.5">
@@ -1614,7 +1644,7 @@
         <v>18</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="60">
@@ -1640,7 +1670,7 @@
         <v>54</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75">
@@ -1687,7 +1717,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="1"/>
       <c r="J26" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="K26" s="1"/>
     </row>
@@ -1747,7 +1777,7 @@
     </row>
     <row r="29" spans="1:12" ht="30">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>86</v>
@@ -1763,12 +1793,12 @@
       </c>
       <c r="H29"/>
       <c r="J29" s="4" t="s">
-        <v>96</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="30">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>88</v>
@@ -1786,225 +1816,246 @@
         <v>20</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>90</v>
+        <v>169</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>89</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="45">
       <c r="A31" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="31.5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="45">
       <c r="A32" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>97</v>
+        <v>181</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="47.25">
+      <c r="H32"/>
+      <c r="J32" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="31.5">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="G33" s="1"/>
       <c r="H33" s="4"/>
       <c r="I33" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>99</v>
+        <v>113</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="47.25">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>17</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" s="4"/>
       <c r="I34" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>142</v>
+        <v>113</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="47.25">
       <c r="A35" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>101</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35"/>
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I35" s="8" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="47.25">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H36"/>
       <c r="I36" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="47.25">
+      <c r="A37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37"/>
+      <c r="I37" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="240">
+      <c r="A38" t="s">
         <v>121</v>
       </c>
-      <c r="J36" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="240">
-      <c r="A37" t="s">
-        <v>129</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B38" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
         <v>16</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>11</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F38" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="7" t="s">
+      <c r="H38" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I37" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="45">
-      <c r="A38" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" t="s">
-        <v>92</v>
-      </c>
-      <c r="E38" s="8" t="s">
+      <c r="I38" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="45">
+      <c r="A39" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>90</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F38" t="s">
-        <v>108</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>94</v>
+      <c r="F39" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2015,10 +2066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L2:L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2026,7 +2077,7 @@
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="51.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="30.42578125" style="5" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -2075,71 +2126,71 @@
     </row>
     <row r="2" spans="1:12" ht="47.25">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="60">
+    <row r="3" spans="1:12" ht="75">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3"/>
       <c r="I3" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>110</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -2149,70 +2200,70 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F5"/>
       <c r="J5" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45">
       <c r="A6" s="8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="4" t="s">
-        <v>114</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>11</v>
@@ -2221,13 +2272,81 @@
         <v>20</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>94</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30">
+      <c r="A8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45">
+      <c r="A9" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9"/>
+      <c r="J9" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10"/>
+      <c r="J10" s="5" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed profile failed testcases
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="183">
   <si>
     <t>GET</t>
   </si>
@@ -507,9 +507,6 @@
   </si>
   <si>
     <t>X-1P-User=(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>status=200||truid=(SYS_USER1)||onboarded=true||discoverable=true</t>
   </si>
   <si>
     <t>truid=(SYS_USER1)||active=false||deleted=false||onboarded=false||discoverable=false</t>
@@ -1009,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1793,7 +1790,7 @@
       </c>
       <c r="H29"/>
       <c r="J29" s="4" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="30">
@@ -1816,10 +1813,10 @@
         <v>20</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="45">
@@ -1842,18 +1839,18 @@
         <v>103</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="45">
       <c r="A32" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
@@ -1866,7 +1863,7 @@
       </c>
       <c r="H32"/>
       <c r="J32" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="31.5">
@@ -2049,13 +2046,13 @@
         <v>103</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>113</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2068,8 +2065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2176,7 +2173,7 @@
         <v>114</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
@@ -2222,7 +2219,7 @@
       </c>
       <c r="F5"/>
       <c r="J5" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45">
@@ -2249,7 +2246,7 @@
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
@@ -2278,12 +2275,12 @@
         <v>126</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>88</v>
@@ -2301,18 +2298,18 @@
         <v>20</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45">
       <c r="A9" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -2325,12 +2322,12 @@
       </c>
       <c r="F9"/>
       <c r="J9" s="4" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>108</v>
@@ -2346,7 +2343,7 @@
       </c>
       <c r="F10"/>
       <c r="J10" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed profile failed tests.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Vanilla-Profile" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="184">
   <si>
     <t>GET</t>
   </si>
@@ -308,9 +308,6 @@
     <t>/users/user/(SYS_USER1)/media</t>
   </si>
   <si>
-    <t>Verify that for the given inactive user id, user media info is not returned and check the error status using Vanilla API</t>
-  </si>
-  <si>
     <t>Verify that for the given inactive user id, user media image is not returned and check the error status using Vanilla API</t>
   </si>
   <si>
@@ -564,6 +561,12 @@
   </si>
   <si>
     <t>OPQA-3289</t>
+  </si>
+  <si>
+    <t>Verify that for the given inactive user id, user's available  media info is returned using Vanilla API</t>
+  </si>
+  <si>
+    <t>status=200||mediaCategory=image-full||truid=(SYS_USER1)</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L39"/>
     </sheetView>
   </sheetViews>
@@ -1111,16 +1114,16 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1136,11 +1139,11 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -1164,19 +1167,19 @@
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
       <c r="I5" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1192,11 +1195,11 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K6" s="1"/>
     </row>
@@ -1221,7 +1224,7 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -1246,7 +1249,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K8" s="1"/>
     </row>
@@ -1270,10 +1273,10 @@
         <v>20</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="31.5">
@@ -1296,10 +1299,10 @@
         <v>20</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="18" customFormat="1" ht="31.5">
@@ -1377,7 +1380,7 @@
       </c>
       <c r="H13"/>
       <c r="J13" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="31.5">
@@ -1401,7 +1404,7 @@
       </c>
       <c r="H14"/>
       <c r="J14" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45">
@@ -1429,7 +1432,7 @@
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K15" s="1"/>
     </row>
@@ -1456,7 +1459,7 @@
         <v>36</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="255">
@@ -1479,45 +1482,45 @@
         <v>30</v>
       </c>
       <c r="H17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="210.75">
       <c r="A18" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E18" t="s">
         <v>0</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="8" t="s">
         <v>72</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="32.25">
       <c r="A19" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1526,10 +1529,10 @@
         <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="7"/>
@@ -1542,16 +1545,16 @@
     </row>
     <row r="20" spans="1:12" ht="32.25">
       <c r="A20" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
@@ -1559,10 +1562,10 @@
       <c r="G20" s="20"/>
       <c r="H20" s="7"/>
       <c r="I20" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="240">
@@ -1588,34 +1591,34 @@
         <v>41</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="210.75">
       <c r="A22" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="8" t="s">
         <v>79</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="31.5">
@@ -1641,7 +1644,7 @@
         <v>18</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="60">
@@ -1667,7 +1670,7 @@
         <v>54</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75">
@@ -1714,7 +1717,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="1"/>
       <c r="J26" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K26" s="1"/>
     </row>
@@ -1774,7 +1777,7 @@
     </row>
     <row r="29" spans="1:12" ht="30">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>86</v>
@@ -1790,12 +1793,12 @@
       </c>
       <c r="H29"/>
       <c r="J29" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="30">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>88</v>
@@ -1813,15 +1816,15 @@
         <v>20</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="45">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>89</v>
@@ -1836,21 +1839,21 @@
         <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="45">
       <c r="A32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
@@ -1863,12 +1866,12 @@
       </c>
       <c r="H32"/>
       <c r="J32" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="31.5">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>92</v>
@@ -1886,18 +1889,18 @@
       <c r="G33" s="1"/>
       <c r="H33" s="4"/>
       <c r="I33" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="47.25">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
@@ -1914,7 +1917,7 @@
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>94</v>
@@ -1922,7 +1925,7 @@
     </row>
     <row r="35" spans="1:10" ht="47.25">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>95</v>
@@ -1943,18 +1946,18 @@
         <v>17</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="47.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="31.5">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>97</v>
+        <v>182</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
@@ -1967,42 +1970,42 @@
       </c>
       <c r="H36"/>
       <c r="I36" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="47.25">
       <c r="A37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H37"/>
       <c r="I37" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="240">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
@@ -2020,15 +2023,15 @@
         <v>41</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="45">
       <c r="A39" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>89</v>
@@ -2043,16 +2046,16 @@
         <v>11</v>
       </c>
       <c r="F39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2065,7 +2068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="L10" sqref="L2:L10"/>
     </sheetView>
   </sheetViews>
@@ -2123,71 +2126,71 @@
     </row>
     <row r="2" spans="1:12" ht="47.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>101</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>102</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
         <v>85</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="75">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3"/>
       <c r="I3" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="31.5">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>105</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>106</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -2197,16 +2200,16 @@
       <c r="H4" s="4"/>
       <c r="I4" s="1"/>
       <c r="J4" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -2219,15 +2222,15 @@
       </c>
       <c r="F5"/>
       <c r="J5" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -2239,22 +2242,22 @@
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -2272,15 +2275,15 @@
         <v>91</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>88</v>
@@ -2298,18 +2301,18 @@
         <v>20</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45">
       <c r="A9" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -2322,15 +2325,15 @@
       </c>
       <c r="F9"/>
       <c r="J9" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
       <c r="A10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -2343,7 +2346,7 @@
       </c>
       <c r="F10"/>
       <c r="J10" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test case OPQA-4602 for Profile. Modified 1 test case in Project container.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="188">
   <si>
     <t>GET</t>
   </si>
@@ -567,6 +567,18 @@
   </si>
   <si>
     <t>status=200||mediaCategory=image-full||truid=(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>Verify that for the given invalid UUID for truid, Admin API doesn't allow to create profile and check the error status using Create User API</t>
+  </si>
+  <si>
+    <t>{"truid" : "a650ce83-12345-bbbb","firstName": "Project","lastName": "NeonX","title": "API Automation Tester","role": "QA","primaryInstitution": "Thomson reuters, Bangalore","location": "india", "onboarded": false}</t>
+  </si>
+  <si>
+    <t>status=400||statusCode=400||errorMessage=TRUID is invalid.</t>
+  </si>
+  <si>
+    <t>OPQA-4602</t>
   </si>
 </sst>
 </file>
@@ -2066,10 +2078,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L2:L10"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2155,82 +2167,90 @@
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="75">
+    <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" ht="75">
+      <c r="A4" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>103</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="F3"/>
-      <c r="I3" s="8" t="s">
+      <c r="F4"/>
+      <c r="I4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="31.5">
-      <c r="A4" t="s">
+    <row r="5" spans="1:12" ht="31.5">
+      <c r="A5" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>105</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="30">
-      <c r="A5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5"/>
-      <c r="J5" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="45">
-      <c r="A6" s="8" t="s">
-        <v>125</v>
+      <c r="F5" s="4"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="30">
+      <c r="A6" t="s">
+        <v>124</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -2238,23 +2258,17 @@
       <c r="D6" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="4" t="s">
-        <v>176</v>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6"/>
+      <c r="J6" s="5" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>106</v>
@@ -2269,50 +2283,51 @@
         <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>125</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="I7" s="8"/>
       <c r="J7" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="30">
-      <c r="A8" t="s">
-        <v>178</v>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45">
+      <c r="A8" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>166</v>
+      <c r="H8" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="45">
-      <c r="A9" s="8" t="s">
-        <v>181</v>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" t="s">
+        <v>178</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>180</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -2321,31 +2336,57 @@
         <v>87</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9"/>
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="J9" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12" ht="45">
+      <c r="A10" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10"/>
+      <c r="J10" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" t="s">
         <v>171</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F10"/>
-      <c r="J10" s="5" t="s">
+      <c r="F11"/>
+      <c r="J11" s="5" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Profile test cases and removed invalid tests: OPQA-693, OPQA-2583
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileTestData.xlsx
+++ b/src/test/test-data/ProfileTestData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UC196992\Git\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="179">
   <si>
     <t>GET</t>
   </si>
@@ -68,9 +73,6 @@
     <t>/users/user/(SYS_USER1)/image</t>
   </si>
   <si>
-    <t>{"location":"India","primaryInstitution":"Thomson Reuters","role":"SM"}</t>
-  </si>
-  <si>
     <t>{"firstName": "Project"}</t>
   </si>
   <si>
@@ -113,15 +115,9 @@
     <t>/users/user/</t>
   </si>
   <si>
-    <t>{"title": "Project Neon1"}</t>
-  </si>
-  <si>
     <t>/users/user/(SYS_USER2)/image</t>
   </si>
   <si>
-    <t>/users/user/(SYS_USER2)/media</t>
-  </si>
-  <si>
     <t>/users/user/(SYS_USER2)/media/image</t>
   </si>
   <si>
@@ -137,15 +133,9 @@
     <t>Verify that for the missing truid, user profile is not returned and check the error status</t>
   </si>
   <si>
-    <t>Verify that for the given user id, media info is returned</t>
-  </si>
-  <si>
     <t>{"imageType": "png","imageHeight":200,"imageWidth":200,"imageContent":"data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADICAIAAAAiOjnJAAAdqUlEQVR4AezSQREAAAgDIPsHtI6m2GN3kIG5AKiPhViIBWIhFmKBWIiFWCAWYiEWiIVYiAViIRZisc/e2W3HURxxfB9hHmEfYR9hH2EfQY+wb7BAQvwleSXLGINxRAgmEMwROBBC+JBJbDAfiRPyTTjHEC4SckNyldx1fse1/E+7e6YzszvSWrjq1NFZ7Y5GPT2/raquru7ZC7dm/AwuvYHl8v4s7AwWymukJC4O1j9vh8vDsD3gJ69Dk9gxprxufzYH6wEVCJgPFnqhCk3y4liHhWdHoUk4gw7jzA7WgytnB7GWTNFTQw7gJ6/bn83BelDlx2NxADRhRTH4dDYH69spfzsIr0xAh5/hq9uNpogDtgb85HUPEdszo/LZaIlaRQsdrGNI1eZAGnar8O87Ye1CG2hJ3LBjxpaDtT9Z3DnpO9OwdqENSatop4N1nOT5cTgziJV3vFUri4P1041wenCPfjwPaxfakLSKdh4ncbD++3V4eqT7x2ve6XlY8PIk/HV/Da1ysNbP1u/2wo1Z4GdXeXcatu+mTD/bzwPwFaNvtep+pcrB+mQvvDUNr23wos+bBDqWPT97N3GQyM0ZPClI4tcabp4bB/TT/SUviiviunixBnGwXpqEk4Mg/X53t8LxMFQLlvKcOVjESYaUuTNsTywAoSadGIRfzrq1h6uIL4prPFJxsD6c0++pvtolEL49Dzt3J5V/XRfU/2oezlfhkiZwGuKkvYxmIWU6r0J7of35RXGlRycO1pWxbt6Sd/HqGKo099xZvjgIaC5xe753V9sL7c8viitdszhYaHu5NlkEUozvepQLwwBM0mfvxeK3e+HdWUA/L0DpYK1R3pxy21K9OukW0ODv3pv1PDT7x+1wtgo05tFBOD8M/Gryn6/DpVH47iBIr6WOm/bnF4V/dLCOUP51x+6flF91FxOA1lBzh0FCY/n5NAip7yxUxwjK/KK4UgfryNl6cYJhQHlRTxVZqMcpvuOA/hzKX/YDDg79yUbADrWU3aGQkuITc4MXX9R9SZUnSFX5aYmDL7tkMslOUYZwriK5kMbsZkvs3oNXSzlTpVQ9Qni34QnSNRsncy4yS22FwNyo2hp0cIiUTG1+k6k6NeDXezICogrFCMVNooXXZwH9zV5WUTiJkTLlsE7Rm3VCH2bMwcLXEOTGMe8Pxx3wIsCyqrrf73WbChRVKFYqBiumKgYLSkTMw4PwwiTFAqPFR9InR+2R4qqTwJ+ecbBWEHVorJtVb936hz2Wc5FqT3HcqRZUkVvi19gmCSk0huN0JaoW+qf9EMvXdwK+7wdjFKvGJSzefHkjnKoCxz8x0p9IOIzrzTuBnnGwuotsgNxHonxlVxdy7pbKeqzKnS9zNUzI1PidP++TOOBm491ivlOqUOgpC1QZUrEm/pErbeoEjuwuDlaxT3eHTXkpzE+3HKkisBXldIYI5qco2CodLAW1mFeutO9vl4P1zDjvTWlK1TMjlbIo3C4LyQijir/9/6bl1hwLUXLB2CfBYX7N5O+3w/OT8BATfxUkxWeQuUr1zkGQFHqA/nGwlhHSPC37lNgcnlTN8vpG+wqZUkGVyMAaCRcjg59QAivbw/D+XL57EUL9bLo4jL/lGKiSXhyJrRwpOwawWn273pg6WB1Fd1RjqEQVXqgESgVSK9b7Mp3HVAzKCxMi7jh4un33/afHMS6NXs9sVaKcwYSRo3iKFQMp0WAzV/rHweos8i95h2IS8gDrieGilGW7kitM62QYAxaFUN3SVJYlZ5yv2y8CsE/c+BQFOKsVmatYD2bBBMuUf4q1S4TrzTuBnllSHCyNwhjVW2+eGzZ2KGyRJb+hcVxKlRXJlPPvpKwElubyaIDAAhSoysHCMpmJBQtUvgzHVwALwdThTEtU6QvGtSsBRpMQB2v9osxCPvrDvIlFop+tysAinwlAMi2WUtc7uSvkI7BLA3AYeqjk6eT0OV6oEb1xfgF6v4qDpTFgbq7emVqGXQXmQGYlU+X8Pgja7UdBQQwJLM0DcpiQgjwCrHICouAZHawVRGMrjcIKwQTGBue1SkHVucrAYu1Dow+iMVACSeYWKTr4RV2TiL1EFWpDNhkkPgUpTqL8BdaI9yWpeSuODGgVPWP/iObRYw5W95yhBvkN6w7mFXgtvzQZqjgJiyBkirjlKAIKcRqdjwi88JKP1pWi86lu9ulK0JTNEiODcqSvkUH6XxLlnA5W2xyjNJ/Tfc3WHSxT7Z4C+tEcPyhDorvLrTITogbgHAWWGS1W0WDwoFN3HeNBKpXz2NlIjqOUcMWGTcSkMz96P9PCF684g+RgFTLR0jjmhaRk2YKMljKfJBe6TtQkzkjxuIJxHBxsMQEMQwj/+hT2Kcv1azZGIAKlon5RJV9WBmt7KO4L/UPvOVgN6dBCryVTb/hBIWVK0B3boQuVVWJpFbw+ovov35gvNyeoPKOYTsXc8d6ovjrZqJKFi8F6OAVLH+UqN0dLOL7td8/BattruBgJzkVIoQTUsTD6U30ftaB53oH32XlBYmMFG7Ip8wRkLasCNa20de8OpWcqowqVQcVXNpYzJPM/GkgCd/a3xUlGB0tS9gXJDJrYujqhONiMQWqWqIThNm9mFgsXaR/p/c8joLEZdoOX+OoTafHvoJn/Hhfo0cIP5kkoKaevbILYog1x3lVUKVNfUneF5eFSKc5oH5UzuyxzUnbBmgrkRi4t/K8XxuFg2t5Cl5JkDZ8qTV/ymA5WKhqUlc1V70JIjgnZGR7itC6gd0y54ZcB3VLw9EzZaNlck4NVZEu+QLZKVCk53nFhRaGWXIWgfW5Ww/iAjZDiBs/v1jrvVGJL15svQqQ9CvXEjaDnRWq36LEyVQ6W+o4xIF9Z9Wb9ys9Lo/Z4cb/TKZ3z36z1g60ehUJWIi3mvCXYqpOLxAQOOq+9VgqjlILHpuZdhK5qZX2uMKFKNcot5WKVVjectfnmvsHCJlEhzdRkbLEMrHMVr2WrRJVdkWL81CCtOuhzsPjKKrAgFOV1IkIqVubv8k0+357WbC9zeYjdStc0axX1oQo8keIXVUp01ea6xFMxm0D/2EQ4PUZypNmhex4rj9wJNTD15QJwRu+6eUaVTf99ur/mjSq/bI7WZbFEFSqLpdnARJvCLMVhnsfKgyp1UCFDmK9SR2WxCF+MqlZblmHSnhsf4naMT/L4E+0Z0VzUL6qeiibaiZxyqpSg5zB9A3MVfA6WZjPKGRpN1ZXWE++p5EHRTEPOyRA8MThEsLYIyUfJ/5UN08gUj6xRYWHNj7BTtq9YCuFglc2VjJYEtqLid7o7r1bQQtPSCJE4GrAeHx5iUHXz3kWO/Apqj1W82TLzwrARwhIHV+goGS0Hq5D0K5Xz8hVvG6tq4pk7ynRefOM/VjR9JEJefkt19z1/CVdPJjtY3YUbaRPP3NojE7weKzs0I2nvsD3JGxudN3ADptiMOVjts+0dXCGG6tYcByEf0cpiEesAVmyxKJu5qRt/CGKp9jOq52leF/TqBnWLYJdapnPDWqdPb/T0JfTg/WCm7k6LARXXCzsG7SSEWG5aFpwjqJ2rDhGsk801gHLHJ74Zw25Hsz1che1dI9VODcrLe/C+0vRzsiZ9Z1gqyeWwyyNtXqU70bgjyNnDdI6YIsYQyqWVd6s/hUazPSRQYqSk6Uxiy6loryDN++tpuYDmSkBtv4GtElVaylyOvdYrGDNRdTpymtcbNq1AxBY9U04mO1gJXph6U3VTCay4wA0PKKrybYmxBzdkQg5ToHmzoiW447TA8EpWxExy5OKQR12w/UQ+2yO17eba95WDtULtcvxN1X4eMVVnopQ999X2CzkZBT1WqfzKpOet3pnStnw6NdPxWGFO2qx1SEfiV0iZkqZfVRws5jTsi6hFnppEawrtVf4gqlRLrm1FbbYnnsbZHhBpUYzQ/35xoEBZjsTYgu/um69iq6Aqn623LqKvHKySNE2valm6Pi3V46p0TjhKcDeAxbqa+KM/7oVrfVosjUxB4ZCyr/RGMtChT9wVFkTLVIrLzKMvK87x/rKypyrNFh/ef2kcD4otB6t9NouOqwVRy+EbP23Z3URauxUR9EqNt+DvkXsHDV81eEBys2Ro+bST0A/dMlgOFqao/UxF4hN5LZOmbfiakqhvTomsCVziUZvN+XR+przwpfHPT/LCKaYjbU1Yuj4WgnkfPZ/NSXMqHqayVVFIwzi309zXCrV+vmBV2dQCeao5Sf5WK121tZruxPUpE3nE+IuE+BftJrlBVgYVsi8SxlVaKqiKBsBi+Jk//9c+StNpz45tRGkas8VV+ILVzgIuLXqtWJCkvIN2QZLKTXyoJGpzBnWnsoquxi+AdmDLB6d5ChQny8RzMj6AYGzVWa2cjnJgQgplwueChpa+xL67FGZspDIhhUWb9WBpK0ezRngZPVciFw5QYsJ+xWlqn2bMks4px1Rekt9+1ZD2qjxhmoJFD5T6h95LxMEqlORqKXqrADbd4yAbVGrPPjIC2jFb20Bqm78fjdkxS9l8bUkaO1lMFDClE5r8/EhboS4lkCSqtHGXhH4obpriYLXfIiuNvjE/5WX4Oo9FPxBQKnjS+vpTNTO4xGSApQf42ObYcs3amy99YDgGDzSXnhGirpWToK/Jh5b3ptNMvINVjuLpO9wZ+sKEX8uFgW2dEZZJ2fyk0Dk2QrnAFnYrfsrX9eZ895WxVctQkHO4XUTPWBfRV+oiB6v/7DM+ov2OavJcgPVwBhY/7eSE/OBY3iqc2IuViVg+BUnbFWDlKbH8EdTrFweLO6eJGo0iMVFmhHgtr4TqsIKFM4ZUOag93EG21r3KSGCx6hcGFoIqbdk1x6zOls/zWSc4WL1FXXE5pTYwjsXyk/n0osxVef9F/sUti+Xrsv+2XdZD2VZp2rNPW6s1iaobmPO+Pa+vCiScenua0Kmr46rVA/TGyhGVg6UOTdYSJmxBQ2F6EbDKc0TlkYGZxnzXUN4XWNqrsswWdisXSsSs0A/dqXQeUaUHc0hXeJ60g6UhW53ylS2tiFJlqQKy8jZlBb8JsjpD/nAAYizbsw+Ts7TsT4wq8mcos0DlpwlJl3GLDpbWPdercpsJCskgvMEOqTacn3xkuQbBygltYxJMnUwjVqrVHu56qg+59ZbCs8oMKXRTS4nSij9/rNxRPghTYLXYnhp3BivRBnlAQ6SVpmELopFBm8X1hOoMA1uumT5XgRSqR3Ku/0GYbrEQGOr2sIbCJsSrb+dnVGlHkPY7pqISt1i9S2lNgfTdWXkuSLtodMvyE7jEGfDdoWUTqHiuGce9NCG9nq/OYHGsZRbYe+1QHzPrMdYKorrvWC/VQUPco3y95Q40UNdYUndCf5JQxeJjiahCteQm3lP0ZLxsK90ZizFgb2VqXG/eCdd8VLj6V3azijuUvm57SwClPJKCRVGlqNzMVUwVenVSv6foGS00bSfs103BzKWhyOu2sEJrK/oUz7x3EexWvp443W5U1Q16spJskqiyNNWb0/hTUYV2WHsDTFuL+j7qtJbJvGvK0sFac3I1D03ae2FRdbbSHVVWkzpmtNu2IoAFUhaBXZuUGELXIw4Wd/r80O49L6hBaBX2Ejm1FuIqPCC2qk87QQ00VF1ucIVcRXxR/F8H64ipwopgS2LlrpQGlfl6YqwCf/KBtl9btyRPnpKldLCOTqinU+9LL4/yTFU+khKa9lzxHMrVBWtEnTvaPvxCaH9+UVypg3WEQj3diUGu9XltPBpmKfnqPxXfRS2d6ElY8KNAqrXUXxFX6mAdnZCczO8B1eLtRUjpz/GM2Zb/6DKleYRQViRzZdS92t3BWqN8spffAzY6W/4uymKJqu3Kcgrpk5W0jpl01BbTi3WuiqcGs7HMxYq9IUJ7of35RXGlDtaRyltTspRSbFjnSFkrYdDk/t2YNZWyyNlpTpCIqkdLrCvSEh0Haw074vEtR3mx/G6OKC8kAisuZbk5a4yiUCL0dV2Ug7UGwZ29PWWeGErwZZ3vrkpZdqsadLBSFC+wjhmv10VoCe2hVSpEPibiYImqncrcmeKkzgUwGKr3Zj0aJNqQtOq4seVgUZap+6cHza1baEPaKtp5nMTBYhZPQZIp73irHKxV5fWN9Ba+s36LRRvSVr3uFut4CYHRrkXfFoArxlqn0IakVbTTwTqGbB1MyQuUFrYzuLt0d+0D2U7q9VYTzmBZU9XxNT0xmlbRNlHlYH3rxKhCjS2kvJ1VGQWjCjW2HlxxsCx1Lm2Sz/Z1DK/bnu3BFQeLJKdlz634rs1hJEXLc8+m/MmDKw4WEQ+VLRcqfpam/IBpe2Ba4o8zcB6OafVQAgfLhXkbgcVrFwerz6LQWzNZtW+L/I9dOhACAABgIOQPNbW/iRRDYiEWiIVYiAViIRZiIRaIhViIBWIhFmKBWIhVbTs75/3SyQ5F8f92baBYwIYigoL1a0OxY0exK7qCqDwsWMGCIPbeFUWsSN6BwGHInYTvQxf2yZwflnFy0yaf3HsTWX+Hp+npaVbc2NjQLxcWFpRFKNI2m5ubyqKnpyeYdXV11dXV1dTUtLe3o5fb21vr/8d5eBgbG0Ob+BfPyin0qwcwOzur/PT+/r66ujo4ONjc3FxdXd3Q0IABjIyMLC8vX1xc4OMoi05PTycmJlpbW3Wt7u7ulZUVtGb9u0xbW/yM6+vryk+Pj4/aYGZm5n8P1vPz86+wFRcXx4r5+fn6ZUpKirIIRdqmvLxcCb28vGAVo6OjZUeRkZFYsPv7eyXU2dlJs7KyMmXX9fV1VFQUjY+OjowdNTo6ihk55ltbW6uE0E5BQYGvfXx8PNr8/PxUQklJSTTDqM7Pz5XQ2tqa8Z3/swKw7u7uMjIy3N1hnQ4PD82/b9rW5rXZ3d1VFjU1NXktt7e3lUctLS2Orm3DhifjTrCpuLj47e3NqEiCafPDwcL2MkIhtinnD1cvQ+HXwYK3yM3NZS8xMTH19fXj4+MILvBhCQkJLEpMTESsdIBVWlpqc1dwezaw9vf3vd6xqqoKHwHhcmpqCtPs6elBdCsqKhoYGFAenZyceKlKTU1FBJ+cnERQrqys9HaH6m6woKWlpZ8MltT8/LxcDOpbwMISsousrCxAYIRIxDgadHR0OMCi03K7K2MuoIfvHTmioZKSEtZCTvbx8aE8Ojg4wDbQpRERETs7O26wkpOTX19fA7C+EywEAnqLs7MzJYQvzqQkNjaWS0iwHE6L7soB1tDQkMy93ELsBi66Sk5Ojm8ihayczTY2NvqC5R1Yb29vANa3gQVKmFNLJijEIw5jb29PgoUV4krTPdBd0UbOhXOky7y8vGSR44TLKkwJpNLS0rRNenq6L1iIm4yneGAWH4BlgoUU+x+LUCTBgjuRW1ZqcXGRZniWYIFa5Eb6ORQKGe6KYdSYCz0iwxYPobibcNwveKOnPFJQGBLb9AUL9PT19bEphFcJVgBWWCJYTIH5HodzZRG/MoQh+YKF7Io2dFp0V9nZ2bijknPhxRKCLEuZjw8PDyPqKaH+/n6a3dzcKCF52LSBhTMjOqIZTpp/F1gBWPixsLCQTstwV3Nzc2jEMRfwgRxcptWI1KDTuEWDc6WB4/6Ww3OAhR818ZwIUAvAMsHCZUHIIhT9abDwCwDvaAEES5Ffu8Hi5TtO/hUVFTrzo3B68B4sGL/cYOGCJhywIPRISzQegPXV5P3q6ortI74oixAg5I2ABAtZEUKefpOZmUl3hVsxlLrBkr9RwXi4GaC8vDyWYg/w/fHxsbLoX/bunzWOK4oC+BeWQJUqgRASSF0qgdKpFBiXbuzKqVwY7MaR0FdIo0adYPLDA4fNe7uXXU3IBuudwtirmdk3T2fun3PvHd/c3ERxqInFXh4cHCSKl0AMYi0iFrOfbI6uOHXoFYHHx8dNxIIvX740vuzo6Eh4vhOxAlYqOQck3uJYt5G+5JiRqWpigaLkqmiylFhDx7q8vIwbXVtI5sUUfPI0Y0lBLAcnFm4M4U7ECm5vb/sEUE26T+WCXtCXZhbEivLCyuYUZfhBrEXE4qfyFSonpPaGVWLqHKDa48OCWKAWlOND1lcTS425t1iwWoZibJqzBPsnJyc5QHheECu4v78varK7YRDLkxohcfYaGlf8JijXnz59Ojs7y49EIRK9glgJwFNhFD7n84JYJC6VPiVCIhkFiwarJmMBynw55fT0tCFBnDjgn9rijx8/vn379u7dO/63qTHXxAoUZwexlhIrEP8mlOkRJ5jnviYWIAexnhOMuaqJVXxvFM6+cerjx49+VIMTlwdsT6ynp6coaoNYi4gViZwk0f9iIm8yIRMUxCpRE6vufmF+ols20NCXkK7novjs+fl5CmpidbFBihm/ILFEqTo5xZ6CGw/TtAGfP392DEjfisxuPqZoiRQdO4yoI4JR3JUcMTxk8aLUM18zPS0FCE7zvXA3jeApvfcIkT39lKxwfn4uQrIGd60YlbAvaFw598eZcnnWfHV1pZLDmBWKvBbTeRkJ2pqw0ibMS/WnDPQXJNbA6HkfGBjEGhjEGhjEGhgYxBoYxJIAE8GVVq6vr6XTkmpVLXI59U9yTq3Rnlvk5BpR1PmdpUPXWUCX8k8FHOm03JuM2asS2nanDaB8zsfMbQtgAb9vjTS2z7UXbSoauRSMLWy+qVk1MMThlpsaM5GWsuAipHaHKQzMZ9Em3KOuB4JcMQ/88PBA4qfYXVxcUDRcgUihI15Lqp4fNYO3RSwKUKEfRsejZk0d1DfK81qdMDUcomuhtTbHpGS7DdLRRUbKmMYmWM8UZHmlRq8PTKW8n5Ymj9Xnths4iBXEzMQepCmqgLrbHoiVQeoSTNFOxEp9kJlf7e5KW30B1ca3SyyPo45yBRaPoDZzNQ2WXDk2Fb34taZBj4bOB/3VgULNRywklobBP/+Jw8PD/I6bHxn4ns9KVyC7pc1L91W/vKYmk+VxnUoC9sFNqXVyZGrnqxXPFBiaVmZfyjKpKTlXa40SpMnKDx8+mM71ydslljCiLm+pgeRzk8H5PK29BV5NrKIex5hNGxA/KNSbYPHy3GPKjgpT+VwkOn+o7aKZuK8wiOWx7qe4mhZeF9k3sepjlhMrHGrbbDLl4RtjLysMYmUQfhArjYE9sSSSq0GbEZKpxiBWBIXeFYZYiUy/roNoY+/Ecp2vG5DXkNTLS5AututdoRHnzEqAkFTkR8jI6wKmQSwPnxjTTglsPXkCWFOd2c2mbz3EqvPz/RKrBoVp7fJoB/bBDtgHuyGPoaWtNq2n3SUCmF3qNRqZqchsEKtCBq12Ihb8n4nlFl4hN5BAV1PdyGbUYL3XOSwGTAsX0ziItQbHx8cRqdcSS7fn+3VgEvZOLPHQ+w2gCOxELDYbewofh3CkDeWKxoApSzD2b5dYdlZB47efyBBEo57/K8G7okpNLJBt7St4JxzYB2Uf+5AJNvC+hmk7yHiM9yT2yujHCN4nHb2RbZTYPKbLicUI5Qne9MRn3MCvdr9ZYWqpQq6EjKlFbgMTQVxhe8sjK9RsXiSM3NyuxPLEJ/JYe4qQuR1G3Texwo8M4yfA2gaq0e3cxCCWgnwcoqBBfNoMWez0srzm1SuaKV5eXpqvi1CU1xW9mjTiwkz3LyRW89KivPG7QKx+XkCi5WEQqx+ran1TfhRd5491kKWnF2B2K0Lp1ZBOxw62ff/+3Vfn4Z6DMIZhCbGYljwSyudrlyfQ3pJY0jqBV97Du1pkVEzUIWMHiDX6gsxqu7I/hfkhd7u3g1jAtDStColPk/sUaGZBiUPF/Greipb5qlcTS+m3+IrUjLchVtrC+vfw5gGr4cptGXEQywHJboiE8V/zXotntydWLsg9JWppBFXjfsnMlxCLpcwrGHpECN2eWCwoK9hH8SKwYhPcpkW+RR1Lukf5FIlD/98oNP/rCcQLZMqZo6FjiUJwAvzl7u6OSuSyWmtETpsIjZe06duf0HspdqkpFRC+58XU7//wDHCyXJIlAVeuL8hfrE0bjG9vQkOzqfNlGaFNMVP2YfX1pGrPqhQ8oHSHrGBa1T6waj5hekfP+8B/ib/bpQMBAAAAACD/10ZoMFZj1ViN1Vg1VmM1Vo3VWI1VYzVWY9VYjdVYBQInF8S0j+DtAAAAAElFTkSuQmCC"}</t>
   </si>
   <si>
-    <t>status=200||truid=(SYS_USER2)||mediaCategory=image-full||mediaType=image/png</t>
-  </si>
-  <si>
     <t>Verify that user is able to view his own profile</t>
   </si>
   <si>
@@ -242,9 +232,6 @@
     <t>OPQA-505</t>
   </si>
   <si>
-    <t>OPQA-693</t>
-  </si>
-  <si>
     <t>OPQA-694</t>
   </si>
   <si>
@@ -263,9 +250,6 @@
     <t>Verify that update user profile summary with exceeds Max length and verify that API should truncate to 1500 characters</t>
   </si>
   <si>
-    <t>{"summary":"Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test ..... now leading to last chars 1500. Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length"}</t>
-  </si>
-  <si>
     <t>status=200||truid=(SYS_USER1)||summary=Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test ..... now leading to last chars 1500.</t>
   </si>
   <si>
@@ -305,9 +289,6 @@
     <t>Verify that inactive user is not able to edit  info like title,role,Institution and country using Vanilla API &amp; check the error status.</t>
   </si>
   <si>
-    <t>/users/user/(SYS_USER1)/media</t>
-  </si>
-  <si>
     <t>Verify that for the given inactive user id, user media image is not returned and check the error status using Vanilla API</t>
   </si>
   <si>
@@ -371,9 +352,6 @@
     <t>OPQA-2580</t>
   </si>
   <si>
-    <t>OPQA-2583</t>
-  </si>
-  <si>
     <t>OPQA-2584</t>
   </si>
   <si>
@@ -404,9 +382,6 @@
     <t>status=200||truid=(SYS_USER2)||mediaCategory=image-full</t>
   </si>
   <si>
-    <t>{"interest":["computers","science","API AUTOMATION"]}</t>
-  </si>
-  <si>
     <t>{"active": false,"onboarded": true}</t>
   </si>
   <si>
@@ -419,15 +394,9 @@
     <t>status=413||statusCode=413||errorMessage=Too many TRUIDs provided.</t>
   </si>
   <si>
-    <t>status=400||statusCode=400||errorMessage=Image Content not set</t>
-  </si>
-  <si>
     <t>status=400||statusCode=400||errorMessage=Image Type not set.</t>
   </si>
   <si>
-    <t>status=404||statusCode=404||errorMessage=Media not found.</t>
-  </si>
-  <si>
     <t>status=409||statusCode=409||errorMessage=User already exists.</t>
   </si>
   <si>
@@ -440,9 +409,6 @@
     <t>Verify that user is able to edit first name and last name from his own profile page.</t>
   </si>
   <si>
-    <t>{"firstName":"ProjectEdited","lastName":"Neon1Edited"}</t>
-  </si>
-  <si>
     <t>status=200||firstName=ProjectEdited||lastName=Neon1Edited||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
   </si>
   <si>
@@ -452,15 +418,9 @@
     <t>OPQA-2679_1</t>
   </si>
   <si>
-    <t>{"firstName":"Project","lastName":"Neon1"}</t>
-  </si>
-  <si>
     <t>status=200||firstName=Project||lastName=Neon1||location=India||truid=(SYS_USER1)||location=India||primaryInstitution=Thomson Reuters||role=QA||title=Project Neon1||interest=API AUTOMATION</t>
   </si>
   <si>
-    <t>{"location":"India","primaryInstitution":"Thomson Reuters","role":"QA"}</t>
-  </si>
-  <si>
     <t>status=200||location=India||primaryInstitution=Thomson Reuters||role=QA</t>
   </si>
   <si>
@@ -482,12 +442,6 @@
     <t>OPQA-2957_1</t>
   </si>
   <si>
-    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAGEAAABhCAMAAADx2D+RAAAAgVBMVEX///8XltMAk9IAkdEAkNEKlNLw9fv0+Pz5+/6Ww+bu8/tssN48ndf8/f/W5fXR4/Snzerm7/nK3vJord6szOuGvOMwnNadx+hFodhXp9vX6PW11O3h7PiJveR8t+Fbqtt0sN++2O+50+54t+CfyujC3PCCtuKs0etfqNydxelOo9rthiAeAAAFvElEQVRoge1Z2XarOgwtMg6TIQQShgAN5DRD+f8PvGDLZiiHENKHc9eKXtpljLYsS1tC+fh4y1ve8pb/ubgWayQsy8L3M+94zPN887sIHqNcgAAQXScaY87ud1Tb55z/SanWlwZMv7yu3a2uSUQdo/1/P0RohLyKsNkeNB0aY7WMoyUjCOrYr+nPHAJCJzj8TisyBNCClwDOJw2UMuDuMOvBIcB6Rf/Ogb42yvhNXKCPQF8IJTOLhro0PW7Xjc/BMkSZuQ7APgwV6Vp9/+ZPgmh42XAwVgE43Y1S0Nl1m+9s1OQMsJt4XeMpL1FaKI2u+eDhThtFLNTeswBbJnVQksY/Av6K8MoKYE9C2B0AtSY8kOMhiu6gyVN5ZytHAwvcqR2x3jxsQqtiauczqW18EvXagJpdIe0hmrSD0ugbQz6XR5Sv7PocHs23WuH05FMSbfmqyg7IlgLkMtxpMbQq0HhRSFt3GL6F/jMKuV3LJ7RNyQn+cuyMO48ybrur7kflOJyWAewVgFzBuzBRk/SGqQyQdwH7JQCbkzg0ZfKSq7vf+iXPEsniQRvAXnGXObDB4KanJTU7k3kgaT/QAMLAs+ouvbST790SgEQ6PqB4Fwsu2w7FXmKhn4PWPhox2iOKpjizNucgRQjXEvFNw8dJEehia4qZXInspePqjA5L0FE7bBDI9hGAWwpf0BiPxAamQ9O/DIoo+cTaECNk+QjBEEVNsYzZKxKghdblklk16daodLwtwoDCo8Q+CyfBVS54idRFip3Z3o1reCXBk/VYBelWPz9AQCfpHZ/66KCwn7ABWhx1nL3Tl7kJCYP1lPElOsrvnCcZTXqrTJgSzQMcRYz0OhSXsw4Nx+49Cu/duhULRIwdZxEq4V692+Ux/trPKnTmh+gVhaNwk1bNIljCvaxTeGuDE74n9oY8E7uGbycCm853aAex6S4sM7wqrrlvpzI14Ilx+qo84UH7Ll4+zCL84b4Eca1mkWg8PeA61XIZTASxlvicYJDE4c8cgOmIiz5wjUYoeXySz8xSPhYUhslJnbkO0BbMja8YSIIameyuXUtWBbEd2Y+e5shPIgibFYI2SWdjBFkClyBAvOoMMTxG2Ky5B/rMPYxjidEFsRQl2fJYwt5HVirbq6xkPh9o6Ae5uAasjqMeaywTOQ1/y+n7qpw+o+N7vJQs5iUsfvMFwhPcSuJuibfXS7g1FsGqzbf5boTE1C1N14fjz/qAtBRN9uqdYAroXWd1EyE5rnEiJKIuFzfYpITzAB974czuaj05AhjWaUx26Pqjb5Ed5FFjaeO7CWbAo14DfHzRxI6BPGzJJFPgFW6G/VI77xl+A8sQuGnLnKSmFvT0XM+nmtH5GtqKbA/hCxdE36pFs33rxxcali74sPaxUVeU3fTe5FT96L2ztNd7H2V77/9N7dQhUkl3VY3fDzWewLm0luZWqJIrheVHaHJT0n4hVzA53EK4gmAUuCrd8EFTWJYANAbRH/vFcTKRZmxckDAVmiMsA/jwqLwK9KrhF3x2FUTttyhJR5+cPgYWpYsnDzGREclPYVpAWMu2G/yeHjLPtxyjkIU+ajXJb0sKReOfbdPLi062mwl0Usgx2mh+MC87NVSF1HOFB6bnhcdUUtTCOJLiKbIAhuW3nGBl21eDE/rs+Kc3X5LB+0ODmYUqCXFQsA5C6qiHG9w46SZlKwAaR6WjYR7IAmxsdvmt1HvfpM1tPQ/QDlvJ4Bg4UjD8g1ND/xFdNUhsZRPDEIKzhcuGwA1AvP4XiO1gik7v3FScGqhASF6Ze9vpwFqkvBJ6+uupZm2xuNbIHxovwlsZQ1RP/dd+P9mOB7eEG8xb4LZm37MXf58xy1G8yu7y0jRp0X3/2g8b3NYSxg0A5VXJzOJg5bh+JFXKmKbrOrTSgDUU6/yKYiXuLs/z43Eb7/1rWdbtD3EryOEtb3nLW/4x+Q8Jgk4C4MfyhwAAAABJRU5ErkJggg==</t>
-  </si>
-  <si>
-    <t>status=200||truid=(SYS_USER2)||imageType=png||mediaCategory=image-full||imageContent=data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAMgAAADICAIAAAAiOjnJAAAdqUlEQVR4AezSQREAAAgDIPsHtI6m2GN3kIG5AKiPhViIBWIhFmKBWIiFWCAWYiEWiIVYiAViIRZisc/e2W3HURxxfB9hHmEfYR9hH2EfQY+wb7BAQvwleSXLGINxRAgmEMwROBBC+JBJbDAfiRPyTTjHEC4SckNyldx1fse1/E+7e6YzszvSWrjq1NFZ7Y5GPT2/raquru7ZC7dm/AwuvYHl8v4s7AwWymukJC4O1j9vh8vDsD3gJ69Dk9gxprxufzYH6wEVCJgPFnqhCk3y4liHhWdHoUk4gw7jzA7WgytnB7GWTNFTQw7gJ6/bn83BelDlx2NxADRhRTH4dDYH69spfzsIr0xAh5/hq9uNpogDtgb85HUPEdszo/LZaIlaRQsdrGNI1eZAGnar8O87Ye1CG2hJ3LBjxpaDtT9Z3DnpO9OwdqENSatop4N1nOT5cTgziJV3vFUri4P1041wenCPfjwPaxfakLSKdh4ncbD++3V4eqT7x2ve6XlY8PIk/HV/Da1ysNbP1u/2wo1Z4GdXeXcatu+mTD/bzwPwFaNvtep+pcrB+mQvvDUNr23wos+bBDqWPT97N3GQyM0ZPClI4tcabp4bB/TT/SUviiviunixBnGwXpqEk4Mg/X53t8LxMFQLlvKcOVjESYaUuTNsTywAoSadGIRfzrq1h6uIL4prPFJxsD6c0++pvtolEL49Dzt3J5V/XRfU/2oezlfhkiZwGuKkvYxmIWU6r0J7of35RXGlRycO1pWxbt6Sd/HqGKo099xZvjgIaC5xe753V9sL7c8viitdszhYaHu5NlkEUozvepQLwwBM0mfvxeK3e+HdWUA/L0DpYK1R3pxy21K9OukW0ODv3pv1PDT7x+1wtgo05tFBOD8M/Gryn6/DpVH47iBIr6WOm/bnF4V/dLCOUP51x+6flF91FxOA1lBzh0FCY/n5NAip7yxUxwjK/KK4UgfryNl6cYJhQHlRTxVZqMcpvuOA/hzKX/YDDg79yUbADrWU3aGQkuITc4MXX9R9SZUnSFX5aYmDL7tkMslOUYZwriK5kMbsZkvs3oNXSzlTpVQ9Qni34QnSNRsncy4yS22FwNyo2hp0cIiUTG1+k6k6NeDXezICogrFCMVNooXXZwH9zV5WUTiJkTLlsE7Rm3VCH2bMwcLXEOTGMe8Pxx3wIsCyqrrf73WbChRVKFYqBiumKgYLSkTMw4PwwiTFAqPFR9InR+2R4qqTwJ+ecbBWEHVorJtVb936hz2Wc5FqT3HcqRZUkVvi19gmCSk0huN0JaoW+qf9EMvXdwK+7wdjFKvGJSzefHkjnKoCxz8x0p9IOIzrzTuBnnGwuotsgNxHonxlVxdy7pbKeqzKnS9zNUzI1PidP++TOOBm491ivlOqUOgpC1QZUrEm/pErbeoEjuwuDlaxT3eHTXkpzE+3HKkisBXldIYI5qco2CodLAW1mFeutO9vl4P1zDjvTWlK1TMjlbIo3C4LyQijir/9/6bl1hwLUXLB2CfBYX7N5O+3w/OT8BATfxUkxWeQuUr1zkGQFHqA/nGwlhHSPC37lNgcnlTN8vpG+wqZUkGVyMAaCRcjg59QAivbw/D+XL57EUL9bLo4jL/lGKiSXhyJrRwpOwawWn273pg6WB1Fd1RjqEQVXqgESgVSK9b7Mp3HVAzKCxMi7jh4un33/afHMS6NXs9sVaKcwYSRo3iKFQMp0WAzV/rHweos8i95h2IS8gDrieGilGW7kitM62QYAxaFUN3SVJYlZ5yv2y8CsE/c+BQFOKsVmatYD2bBBMuUf4q1S4TrzTuBnllSHCyNwhjVW2+eGzZ2KGyRJb+hcVxKlRXJlPPvpKwElubyaIDAAhSoysHCMpmJBQtUvgzHVwALwdThTEtU6QvGtSsBRpMQB2v9osxCPvrDvIlFop+tysAinwlAMi2WUtc7uSvkI7BLA3AYeqjk6eT0OV6oEb1xfgF6v4qDpTFgbq7emVqGXQXmQGYlU+X8Pgja7UdBQQwJLM0DcpiQgjwCrHICouAZHawVRGMrjcIKwQTGBue1SkHVucrAYu1Dow+iMVACSeYWKTr4RV2TiL1EFWpDNhkkPgUpTqL8BdaI9yWpeSuODGgVPWP/iObRYw5W95yhBvkN6w7mFXgtvzQZqjgJiyBkirjlKAIKcRqdjwi88JKP1pWi86lu9ulK0JTNEiODcqSvkUH6XxLlnA5W2xyjNJ/Tfc3WHSxT7Z4C+tEcPyhDorvLrTITogbgHAWWGS1W0WDwoFN3HeNBKpXz2NlIjqOUcMWGTcSkMz96P9PCF684g+RgFTLR0jjmhaRk2YKMljKfJBe6TtQkzkjxuIJxHBxsMQEMQwj/+hT2Kcv1azZGIAKlon5RJV9WBmt7KO4L/UPvOVgN6dBCryVTb/hBIWVK0B3boQuVVWJpFbw+ovov35gvNyeoPKOYTsXc8d6ovjrZqJKFi8F6OAVLH+UqN0dLOL7td8/BattruBgJzkVIoQTUsTD6U30ftaB53oH32XlBYmMFG7Ip8wRkLasCNa20de8OpWcqowqVQcVXNpYzJPM/GkgCd/a3xUlGB0tS9gXJDJrYujqhONiMQWqWqIThNm9mFgsXaR/p/c8joLEZdoOX+OoTafHvoJn/Hhfo0cIP5kkoKaevbILYog1x3lVUKVNfUneF5eFSKc5oH5UzuyxzUnbBmgrkRi4t/K8XxuFg2t5Cl5JkDZ8qTV/ymA5WKhqUlc1V70JIjgnZGR7itC6gd0y54ZcB3VLw9EzZaNlck4NVZEu+QLZKVCk53nFhRaGWXIWgfW5Ww/iAjZDiBs/v1jrvVGJL15svQqQ9CvXEjaDnRWq36LEyVQ6W+o4xIF9Z9Wb9ys9Lo/Z4cb/TKZ3z36z1g60ehUJWIi3mvCXYqpOLxAQOOq+9VgqjlILHpuZdhK5qZX2uMKFKNcot5WKVVjectfnmvsHCJlEhzdRkbLEMrHMVr2WrRJVdkWL81CCtOuhzsPjKKrAgFOV1IkIqVubv8k0+357WbC9zeYjdStc0axX1oQo8keIXVUp01ea6xFMxm0D/2EQ4PUZypNmhex4rj9wJNTD15QJwRu+6eUaVTf99ur/mjSq/bI7WZbFEFSqLpdnARJvCLMVhnsfKgyp1UCFDmK9SR2WxCF+MqlZblmHSnhsf4naMT/L4E+0Z0VzUL6qeiibaiZxyqpSg5zB9A3MVfA6WZjPKGRpN1ZXWE++p5EHRTEPOyRA8MThEsLYIyUfJ/5UN08gUj6xRYWHNj7BTtq9YCuFglc2VjJYEtqLid7o7r1bQQtPSCJE4GrAeHx5iUHXz3kWO/Apqj1W82TLzwrARwhIHV+goGS0Hq5D0K5Xz8hVvG6tq4pk7ynRefOM/VjR9JEJefkt19z1/CVdPJjtY3YUbaRPP3NojE7weKzs0I2nvsD3JGxudN3ADptiMOVjts+0dXCGG6tYcByEf0cpiEesAVmyxKJu5qRt/CGKp9jOq52leF/TqBnWLYJdapnPDWqdPb/T0JfTg/WCm7k6LARXXCzsG7SSEWG5aFpwjqJ2rDhGsk801gHLHJ74Zw25Hsz1che1dI9VODcrLe/C+0vRzsiZ9Z1gqyeWwyyNtXqU70bgjyNnDdI6YIsYQyqWVd6s/hUazPSRQYqSk6Uxiy6loryDN++tpuYDmSkBtv4GtElVaylyOvdYrGDNRdTpymtcbNq1AxBY9U04mO1gJXph6U3VTCay4wA0PKKrybYmxBzdkQg5ToHmzoiW447TA8EpWxExy5OKQR12w/UQ+2yO17eba95WDtULtcvxN1X4eMVVnopQ999X2CzkZBT1WqfzKpOet3pnStnw6NdPxWGFO2qx1SEfiV0iZkqZfVRws5jTsi6hFnppEawrtVf4gqlRLrm1FbbYnnsbZHhBpUYzQ/35xoEBZjsTYgu/um69iq6Aqn623LqKvHKySNE2valm6Pi3V46p0TjhKcDeAxbqa+KM/7oVrfVosjUxB4ZCyr/RGMtChT9wVFkTLVIrLzKMvK87x/rKypyrNFh/ef2kcD4otB6t9NouOqwVRy+EbP23Z3URauxUR9EqNt+DvkXsHDV81eEBys2Ro+bST0A/dMlgOFqao/UxF4hN5LZOmbfiakqhvTomsCVziUZvN+XR+przwpfHPT/LCKaYjbU1Yuj4WgnkfPZ/NSXMqHqayVVFIwzi309zXCrV+vmBV2dQCeao5Sf5WK121tZruxPUpE3nE+IuE+BftJrlBVgYVsi8SxlVaKqiKBsBi+Jk//9c+StNpz45tRGkas8VV+ILVzgIuLXqtWJCkvIN2QZLKTXyoJGpzBnWnsoquxi+AdmDLB6d5ChQny8RzMj6AYGzVWa2cjnJgQgplwueChpa+xL67FGZspDIhhUWb9WBpK0ezRngZPVciFw5QYsJ+xWlqn2bMks4px1Rekt9+1ZD2qjxhmoJFD5T6h95LxMEqlORqKXqrADbd4yAbVGrPPjIC2jFb20Bqm78fjdkxS9l8bUkaO1lMFDClE5r8/EhboS4lkCSqtHGXhH4obpriYLXfIiuNvjE/5WX4Oo9FPxBQKnjS+vpTNTO4xGSApQf42ObYcs3amy99YDgGDzSXnhGirpWToK/Jh5b3ptNMvINVjuLpO9wZ+sKEX8uFgW2dEZZJ2fyk0Dk2QrnAFnYrfsrX9eZ895WxVctQkHO4XUTPWBfRV+oiB6v/7DM+ov2OavJcgPVwBhY/7eSE/OBY3iqc2IuViVg+BUnbFWDlKbH8EdTrFweLO6eJGo0iMVFmhHgtr4TqsIKFM4ZUOag93EG21r3KSGCx6hcGFoIqbdk1x6zOls/zWSc4WL1FXXE5pTYwjsXyk/n0osxVef9F/sUti+Xrsv+2XdZD2VZp2rNPW6s1iaobmPO+Pa+vCiScenua0Kmr46rVA/TGyhGVg6UOTdYSJmxBQ2F6EbDKc0TlkYGZxnzXUN4XWNqrsswWdisXSsSs0A/dqXQeUaUHc0hXeJ60g6UhW53ylS2tiFJlqQKy8jZlBb8JsjpD/nAAYizbsw+Ts7TsT4wq8mcos0DlpwlJl3GLDpbWPdercpsJCskgvMEOqTacn3xkuQbBygltYxJMnUwjVqrVHu56qg+59ZbCs8oMKXRTS4nSij9/rNxRPghTYLXYnhp3BivRBnlAQ6SVpmELopFBm8X1hOoMA1uumT5XgRSqR3Ku/0GYbrEQGOr2sIbCJsSrb+dnVGlHkPY7pqISt1i9S2lNgfTdWXkuSLtodMvyE7jEGfDdoWUTqHiuGce9NCG9nq/OYHGsZRbYe+1QHzPrMdYKorrvWC/VQUPco3y95Q40UNdYUndCf5JQxeJjiahCteQm3lP0ZLxsK90ZizFgb2VqXG/eCdd8VLj6V3azijuUvm57SwClPJKCRVGlqNzMVUwVenVSv6foGS00bSfs103BzKWhyOu2sEJrK/oUz7x3EexWvp443W5U1Q16spJskqiyNNWb0/hTUYV2WHsDTFuL+j7qtJbJvGvK0sFac3I1D03ae2FRdbbSHVVWkzpmtNu2IoAFUhaBXZuUGELXIw4Wd/r80O49L6hBaBX2Ejm1FuIqPCC2qk87QQ00VF1ucIVcRXxR/F8H64ipwopgS2LlrpQGlfl6YqwCf/KBtl9btyRPnpKldLCOTqinU+9LL4/yTFU+khKa9lzxHMrVBWtEnTvaPvxCaH9+UVypg3WEQj3diUGu9XltPBpmKfnqPxXfRS2d6ElY8KNAqrXUXxFX6mAdnZCczO8B1eLtRUjpz/GM2Zb/6DKleYRQViRzZdS92t3BWqN8spffAzY6W/4uymKJqu3Kcgrpk5W0jpl01BbTi3WuiqcGs7HMxYq9IUJ7of35RXGlDtaRyltTspRSbFjnSFkrYdDk/t2YNZWyyNlpTpCIqkdLrCvSEh0Haw074vEtR3mx/G6OKC8kAisuZbk5a4yiUCL0dV2Ug7UGwZ29PWWeGErwZZ3vrkpZdqsadLBSFC+wjhmv10VoCe2hVSpEPibiYImqncrcmeKkzgUwGKr3Zj0aJNqQtOq4seVgUZap+6cHza1baEPaKtp5nMTBYhZPQZIp73irHKxV5fWN9Ba+s36LRRvSVr3uFut4CYHRrkXfFoArxlqn0IakVbTTwTqGbB1MyQuUFrYzuLt0d+0D2U7q9VYTzmBZU9XxNT0xmlbRNlHlYH3rxKhCjS2kvJ1VGQWjCjW2HlxxsCx1Lm2Sz/Z1DK/bnu3BFQeLJKdlz634rs1hJEXLc8+m/MmDKw4WEQ+VLRcqfpam/IBpe2Ba4o8zcB6OafVQAgfLhXkbgcVrFwerz6LQWzNZtW+L/I9dOhACAABgIOQPNbW/iRRDYiEWiIVYiAViIRZiIRaIhViIBWIhFmKBWIhVbTs75/3SyQ5F8f92baBYwIYigoL1a0OxY0exK7qCqDwsWMGCIPbeFUWsSN6BwGHInYTvQxf2yZwflnFy0yaf3HsTWX+Hp+npaVbc2NjQLxcWFpRFKNI2m5ubyqKnpyeYdXV11dXV1dTUtLe3o5fb21vr/8d5eBgbG0Ob+BfPyin0qwcwOzur/PT+/r66ujo4ONjc3FxdXd3Q0IABjIyMLC8vX1xc4OMoi05PTycmJlpbW3Wt7u7ulZUVtGb9u0xbW/yM6+vryk+Pj4/aYGZm5n8P1vPz86+wFRcXx4r5+fn6ZUpKirIIRdqmvLxcCb28vGAVo6OjZUeRkZFYsPv7eyXU2dlJs7KyMmXX9fV1VFQUjY+OjowdNTo6ihk55ltbW6uE0E5BQYGvfXx8PNr8/PxUQklJSTTDqM7Pz5XQ2tqa8Z3/swKw7u7uMjIy3N1hnQ4PD82/b9rW5rXZ3d1VFjU1NXktt7e3lUctLS2Orm3DhifjTrCpuLj47e3NqEiCafPDwcL2MkIhtinnD1cvQ+HXwYK3yM3NZS8xMTH19fXj4+MILvBhCQkJLEpMTESsdIBVWlpqc1dwezaw9vf3vd6xqqoKHwHhcmpqCtPs6elBdCsqKhoYGFAenZyceKlKTU1FBJ+cnERQrqys9HaH6m6woKWlpZ8MltT8/LxcDOpbwMISsousrCxAYIRIxDgadHR0OMCi03K7K2MuoIfvHTmioZKSEtZCTvbx8aE8Ojg4wDbQpRERETs7O26wkpOTX19fA7C+EywEAnqLs7MzJYQvzqQkNjaWS0iwHE6L7soB1tDQkMy93ELsBi66Sk5Ojm8ihayczTY2NvqC5R1Yb29vANa3gQVKmFNLJijEIw5jb29PgoUV4krTPdBd0UbOhXOky7y8vGSR44TLKkwJpNLS0rRNenq6L1iIm4yneGAWH4BlgoUU+x+LUCTBgjuRW1ZqcXGRZniWYIFa5Eb6ORQKGe6KYdSYCz0iwxYPobibcNwveKOnPFJQGBLb9AUL9PT19bEphFcJVgBWWCJYTIH5HodzZRG/MoQh+YKF7Io2dFp0V9nZ2bijknPhxRKCLEuZjw8PDyPqKaH+/n6a3dzcKCF52LSBhTMjOqIZTpp/F1gBWPixsLCQTstwV3Nzc2jEMRfwgRxcptWI1KDTuEWDc6WB4/6Ww3OAhR818ZwIUAvAMsHCZUHIIhT9abDwCwDvaAEES5Ffu8Hi5TtO/hUVFTrzo3B68B4sGL/cYOGCJhywIPRISzQegPXV5P3q6ortI74oixAg5I2ABAtZEUKefpOZmUl3hVsxlLrBkr9RwXi4GaC8vDyWYg/w/fHxsbLoX/bunzWOK4oC+BeWQJUqgRASSF0qgdKpFBiXbuzKqVwY7MaR0FdIo0adYPLDA4fNe7uXXU3IBuudwtirmdk3T2fun3PvHd/c3ERxqInFXh4cHCSKl0AMYi0iFrOfbI6uOHXoFYHHx8dNxIIvX740vuzo6Eh4vhOxAlYqOQck3uJYt5G+5JiRqWpigaLkqmiylFhDx7q8vIwbXVtI5sUUfPI0Y0lBLAcnFm4M4U7ECm5vb/sEUE26T+WCXtCXZhbEivLCyuYUZfhBrEXE4qfyFSonpPaGVWLqHKDa48OCWKAWlOND1lcTS425t1iwWoZibJqzBPsnJyc5QHheECu4v78varK7YRDLkxohcfYaGlf8JijXnz59Ojs7y49EIRK9glgJwFNhFD7n84JYJC6VPiVCIhkFiwarJmMBynw55fT0tCFBnDjgn9rijx8/vn379u7dO/63qTHXxAoUZwexlhIrEP8mlOkRJ5jnviYWIAexnhOMuaqJVXxvFM6+cerjx49+VIMTlwdsT6ynp6coaoNYi4gViZwk0f9iIm8yIRMUxCpRE6vufmF+ols20NCXkK7novjs+fl5CmpidbFBihm/ILFEqTo5xZ6CGw/TtAGfP392DEjfisxuPqZoiRQdO4yoI4JR3JUcMTxk8aLUM18zPS0FCE7zvXA3jeApvfcIkT39lKxwfn4uQrIGd60YlbAvaFw598eZcnnWfHV1pZLDmBWKvBbTeRkJ2pqw0ibMS/WnDPQXJNbA6HkfGBjEGhjEGhjEGhgYxBoYxJIAE8GVVq6vr6XTkmpVLXI59U9yTq3Rnlvk5BpR1PmdpUPXWUCX8k8FHOm03JuM2asS2nanDaB8zsfMbQtgAb9vjTS2z7UXbSoauRSMLWy+qVk1MMThlpsaM5GWsuAipHaHKQzMZ9Em3KOuB4JcMQ/88PBA4qfYXVxcUDRcgUihI15Lqp4fNYO3RSwKUKEfRsejZk0d1DfK81qdMDUcomuhtTbHpGS7DdLRRUbKmMYmWM8UZHmlRq8PTKW8n5Ymj9Xnths4iBXEzMQepCmqgLrbHoiVQeoSTNFOxEp9kJlf7e5KW30B1ca3SyyPo45yBRaPoDZzNQ2WXDk2Fb34taZBj4bOB/3VgULNRywklobBP/+Jw8PD/I6bHxn4ns9KVyC7pc1L91W/vKYmk+VxnUoC9sFNqXVyZGrnqxXPFBiaVmZfyjKpKTlXa40SpMnKDx8+mM71ydslljCiLm+pgeRzk8H5PK29BV5NrKIex5hNGxA/KNSbYPHy3GPKjgpT+VwkOn+o7aKZuK8wiOWx7qe4mhZeF9k3sepjlhMrHGrbbDLl4RtjLysMYmUQfhArjYE9sSSSq0GbEZKpxiBWBIXeFYZYiUy/roNoY+/Ecp2vG5DXkNTLS5AututdoRHnzEqAkFTkR8jI6wKmQSwPnxjTTglsPXkCWFOd2c2mbz3EqvPz/RKrBoVp7fJoB/bBDtgHuyGPoaWtNq2n3SUCmF3qNRqZqchsEKtCBq12Ihb8n4nlFl4hN5BAV1PdyGbUYL3XOSwGTAsX0ziItQbHx8cRqdcSS7fn+3VgEvZOLPHQ+w2gCOxELDYbewofh3CkDeWKxoApSzD2b5dYdlZB47efyBBEo57/K8G7okpNLJBt7St4JxzYB2Uf+5AJNvC+hmk7yHiM9yT2yujHCN4nHb2RbZTYPKbLicUI5Qne9MRn3MCvdr9ZYWqpQq6EjKlFbgMTQVxhe8sjK9RsXiSM3NyuxPLEJ/JYe4qQuR1G3Texwo8M4yfA2gaq0e3cxCCWgnwcoqBBfNoMWez0srzm1SuaKV5eXpqvi1CU1xW9mjTiwkz3LyRW89KivPG7QKx+XkCi5WEQqx+ran1TfhRd5491kKWnF2B2K0Lp1ZBOxw62ff/+3Vfn4Z6DMIZhCbGYljwSyudrlyfQ3pJY0jqBV97Du1pkVEzUIWMHiDX6gsxqu7I/hfkhd7u3g1jAtDStColPk/sUaGZBiUPF/Greipb5qlcTS+m3+IrUjLchVtrC+vfw5gGr4cptGXEQywHJboiE8V/zXotntydWLsg9JWppBFXjfsnMlxCLpcwrGHpECN2eWCwoK9hH8SKwYhPcpkW+RR1Lukf5FIlD/98oNP/rCcQLZMqZo6FjiUJwAvzl7u6OSuSyWmtETpsIjZe06duf0HspdqkpFRC+58XU7//wDHCyXJIlAVeuL8hfrE0bjG9vQkOzqfNlGaFNMVP2YfX1pGrPqhQ8oHSHrGBa1T6waj5hekfP+8B/ib/bpQMBAAAAACD/10ZoMFZj1ViN1Vg1VmM1Vo3VWI1VYzVWY9VYjdVYBQInF8S0j+DtAAAAAElFTkSuQmCC</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
@@ -563,12 +517,6 @@
     <t>OPQA-3289</t>
   </si>
   <si>
-    <t>Verify that for the given inactive user id, user's available  media info is returned using Vanilla API</t>
-  </si>
-  <si>
-    <t>status=200||mediaCategory=image-full||truid=(SYS_USER1)</t>
-  </si>
-  <si>
     <t>Verify that for the given invalid UUID for truid, Admin API doesn't allow to create profile and check the error status using Create User API</t>
   </si>
   <si>
@@ -579,13 +527,44 @@
   </si>
   <si>
     <t>OPQA-4602</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "summary":"Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test ..... now leading to last chars 1500. Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length Summary test with max length"}</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "firstName":"ProjectEdited","lastName":"Neon1Edited"}</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "interest":["computers","science","API AUTOMATION"]}</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "location":"India","primaryInstitution":"Thomson Reuters","role":"QA"}</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "summary":"I am test user for API Automation"}</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "title": "Project Neon1"}</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "location":"India","primaryInstitution":"Thomson Reuters","role":"SM"}</t>
+  </si>
+  <si>
+    <t>{"truid":"(SYS_USER1)", "firstName":"Project","lastName":"Neon1"}</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,7 +613,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -644,6 +623,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -675,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -725,12 +710,32 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -777,7 +782,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -809,9 +814,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -843,6 +849,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1018,30 +1025,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="53.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="52.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="96.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="80.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="90.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="53.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="49.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="52.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="96.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="80.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="5" width="90.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1079,12 +1086,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="225">
+    <row r="2" spans="1:12" ht="345" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>12</v>
@@ -1096,21 +1103,27 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G2"/>
       <c r="H2" s="7" t="s">
-        <v>82</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I2"/>
       <c r="J2" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30">
+        <v>76</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1126,16 +1139,19 @@
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" s="7" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="31.5">
+      <c r="L3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1147,24 +1163,27 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="7" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="31.5">
+      <c r="L4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1179,19 +1198,22 @@
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
       <c r="I5" s="8" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="45">
+      <c r="L5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1203,30 +1225,33 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="4" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="7" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="31.5">
+      <c r="L6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
@@ -1236,22 +1261,25 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="31.5">
+      <c r="L7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>0</v>
@@ -1261,16 +1289,19 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1"/>
       <c r="J8" s="4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="31.5">
+      <c r="L8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -1282,21 +1313,27 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G9"/>
       <c r="H9" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="I9"/>
       <c r="J9" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="31.5">
+        <v>126</v>
+      </c>
+      <c r="K9"/>
+      <c r="L9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1308,21 +1345,27 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G10"/>
       <c r="H10" s="5" t="s">
-        <v>147</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="I10"/>
       <c r="J10" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="18" customFormat="1" ht="31.5">
+        <v>133</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>12</v>
@@ -1334,97 +1377,117 @@
         <v>11</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11"/>
       <c r="H11" s="19" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="I11"/>
       <c r="J11" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="195" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
         <v>22</v>
-      </c>
-      <c r="K11"/>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:12" ht="180">
-      <c r="A12" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>0</v>
       </c>
+      <c r="F12"/>
       <c r="G12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12"/>
+      <c r="I12"/>
       <c r="J12" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="180">
+        <v>24</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="195" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
         <v>0</v>
       </c>
+      <c r="F13"/>
       <c r="G13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13"/>
+      <c r="I13"/>
       <c r="J13" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="31.5">
+        <v>123</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
         <v>0</v>
       </c>
+      <c r="F14"/>
       <c r="G14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14"/>
+      <c r="I14"/>
       <c r="J14" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45">
+        <v>122</v>
+      </c>
+      <c r="K14"/>
+      <c r="L14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1436,209 +1499,249 @@
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="4" t="s">
-        <v>32</v>
+        <v>174</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="7" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" ht="30">
+      <c r="L15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G16"/>
       <c r="H16" s="7" t="s">
-        <v>36</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="I16"/>
       <c r="J16" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="255">
+        <v>124</v>
+      </c>
+      <c r="K16"/>
+      <c r="L16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G17"/>
       <c r="H17" s="7" t="s">
-        <v>127</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="I17"/>
       <c r="J17" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="210.75">
-      <c r="A18" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>152</v>
-      </c>
-      <c r="E18" t="s">
+        <v>119</v>
+      </c>
+      <c r="K17"/>
+      <c r="L17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="32.25" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="32.25">
+      <c r="F18" s="23"/>
+      <c r="G18" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="H18" s="25"/>
+      <c r="I18" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="K18" s="23"/>
+      <c r="L18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E19" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F19" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="7"/>
       <c r="I19" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="32.25">
+        <v>18</v>
+      </c>
+      <c r="K19"/>
+      <c r="L19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E20" t="s">
         <v>0</v>
       </c>
+      <c r="F20"/>
       <c r="G20" s="20"/>
       <c r="H20" s="7"/>
       <c r="I20" s="8" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="240">
+        <v>119</v>
+      </c>
+      <c r="K20"/>
+      <c r="L20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G21"/>
       <c r="H21" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="I21"/>
       <c r="J21" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="210.75">
+        <v>119</v>
+      </c>
+      <c r="K21"/>
+      <c r="L21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="32.25" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E22" t="s">
         <v>0</v>
       </c>
+      <c r="F22"/>
       <c r="G22" s="20" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="31.5">
+        <v>119</v>
+      </c>
+      <c r="K22"/>
+      <c r="L22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1650,47 +1753,59 @@
         <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G23"/>
       <c r="H23" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I23"/>
       <c r="J23" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="60">
+        <v>124</v>
+      </c>
+      <c r="K23"/>
+      <c r="L23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="G24"/>
       <c r="H24" s="5" t="s">
-        <v>54</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="I24"/>
       <c r="J24" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.75">
+        <v>124</v>
+      </c>
+      <c r="K24"/>
+      <c r="L24" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -1701,373 +1816,390 @@
       <c r="E25" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F25"/>
       <c r="G25" s="1"/>
       <c r="H25" s="6"/>
       <c r="I25" s="1"/>
       <c r="J25" s="4" t="s">
-        <v>42</v>
+        <v>121</v>
       </c>
       <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" ht="31.5">
+      <c r="L25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="F26"/>
       <c r="G26" s="1"/>
       <c r="H26" s="6"/>
       <c r="I26" s="1"/>
       <c r="J26" s="4" t="s">
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:12" ht="31.5">
+      <c r="L26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27"/>
+      <c r="H27" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27"/>
+      <c r="J27" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27"/>
+      <c r="L27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="4" t="s">
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K28"/>
+      <c r="L28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:12" s="9" customFormat="1" ht="15.75">
-      <c r="A28" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G28"/>
-      <c r="H28" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28"/>
-      <c r="J28" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K28"/>
-      <c r="L28"/>
-    </row>
-    <row r="29" spans="1:12" ht="30">
-      <c r="A29" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29"/>
+      <c r="G29"/>
+      <c r="H29" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I29"/>
       <c r="J29" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="30">
+        <v>156</v>
+      </c>
+      <c r="K29"/>
+      <c r="L29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>167</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="G30"/>
+      <c r="H30" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I30"/>
       <c r="J30" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="45">
+        <v>157</v>
+      </c>
+      <c r="K30"/>
+      <c r="L30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>112</v>
+        <v>162</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" t="s">
-        <v>102</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="45">
+        <v>83</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="K31"/>
+      <c r="L31" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>179</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>177</v>
+        <v>106</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H32"/>
-      <c r="J32" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="31.5">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K32"/>
+      <c r="L32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="H33" s="4"/>
       <c r="I33" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="47.25">
+        <v>104</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K33"/>
+      <c r="L33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K34"/>
+      <c r="L34" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H34" s="4"/>
-      <c r="I34" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J34" s="7" t="s">
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K35"/>
+      <c r="L35" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36"/>
+      <c r="H36" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K36"/>
+      <c r="L36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="47.25">
-      <c r="A35" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="31.5">
-      <c r="A36" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="C36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" t="s">
-        <v>96</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H36"/>
-      <c r="I36" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="47.25">
-      <c r="A37" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H37"/>
+      <c r="G37"/>
+      <c r="H37" s="5" t="s">
+        <v>152</v>
+      </c>
       <c r="I37" s="8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="240">
-      <c r="A38" t="s">
-        <v>120</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="45">
-      <c r="A39" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" t="s">
-        <v>90</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" t="s">
-        <v>102</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>175</v>
+        <v>158</v>
+      </c>
+      <c r="K37"/>
+      <c r="L37" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -2077,28 +2209,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2:L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="51.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="68.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="64.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="51.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="40.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="5" width="30.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="68.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="5" width="64.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -2136,102 +2268,114 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="47.25">
+    <row r="2" spans="1:12" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="60">
+      <c r="L2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="4" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="4" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="75">
+      <c r="L3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
       <c r="I4" s="8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="31.5">
+        <v>147</v>
+      </c>
+      <c r="K4"/>
+      <c r="L4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -2241,153 +2385,193 @@
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="30">
+      <c r="L5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
       <c r="J6" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="45">
+        <v>148</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>102</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="G7"/>
       <c r="H7" s="5" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="45">
+        <v>159</v>
+      </c>
+      <c r="K7"/>
+      <c r="L7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G8"/>
       <c r="H8" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="30">
+        <v>158</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G9"/>
       <c r="H9" s="4" t="s">
-        <v>166</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="I9"/>
       <c r="J9" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45">
+        <v>153</v>
+      </c>
+      <c r="K9"/>
+      <c r="L9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
       <c r="J10" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="30">
+        <v>153</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
       <c r="J11" s="5" t="s">
-        <v>172</v>
+        <v>155</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>